<commit_message>
Agregacion del Boton guardar en el reporte Enexo 7 Boleta de Valorizacion Petroperu Lote I,VI, Z69 y Principal
</commit_message>
<xml_diff>
--- a/Unna.OperationalReport.WebSite/wwwroot/plantillas/reporte/mensual/BoletadeValorizacionPetroperu.xlsx
+++ b/Unna.OperationalReport.WebSite/wwwroot/plantillas/reporte/mensual/BoletadeValorizacionPetroperu.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desarrollos\SP\APSS SP\ProyectoPrincipalAenza5\UnnaReportesOperativos\Unna.OperationalReport.WebSite\wwwroot\plantillas\reporte\mensual\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F85AD6EE-75C9-432C-AAEB-3C3359DEC363}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D98DA4A1-9B09-4DF4-B041-85CF393A7EFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="8976" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -862,9 +862,6 @@
     <xf numFmtId="170" fontId="4" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -914,6 +911,30 @@
     <xf numFmtId="166" fontId="9" fillId="0" borderId="1" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -929,12 +950,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -980,23 +995,8 @@
     <xf numFmtId="169" fontId="7" fillId="0" borderId="17" xfId="103" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="104">
@@ -1499,7 +1499,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E15" sqref="E15"/>
+      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1518,385 +1518,385 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:38" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C1" s="30" t="s">
+      <c r="C1" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
-      <c r="L1" s="30"/>
-      <c r="M1" s="30"/>
-      <c r="N1" s="30"/>
-      <c r="O1" s="30"/>
-      <c r="P1" s="30"/>
-      <c r="Q1" s="30"/>
-      <c r="R1" s="30"/>
-      <c r="S1" s="30"/>
-      <c r="T1" s="30"/>
-      <c r="U1" s="30"/>
-      <c r="V1" s="30"/>
-      <c r="W1" s="30"/>
-      <c r="X1" s="30"/>
-      <c r="Y1" s="30"/>
-      <c r="Z1" s="30"/>
-      <c r="AA1" s="30"/>
-      <c r="AB1" s="30"/>
-      <c r="AC1" s="30"/>
-      <c r="AD1" s="30"/>
-      <c r="AE1" s="30"/>
-      <c r="AF1" s="30"/>
-      <c r="AG1" s="30"/>
-      <c r="AH1" s="30"/>
-      <c r="AI1" s="30"/>
-      <c r="AJ1" s="30"/>
-      <c r="AK1" s="27" t="s">
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
+      <c r="K1" s="37"/>
+      <c r="L1" s="37"/>
+      <c r="M1" s="37"/>
+      <c r="N1" s="37"/>
+      <c r="O1" s="37"/>
+      <c r="P1" s="37"/>
+      <c r="Q1" s="37"/>
+      <c r="R1" s="37"/>
+      <c r="S1" s="37"/>
+      <c r="T1" s="37"/>
+      <c r="U1" s="37"/>
+      <c r="V1" s="37"/>
+      <c r="W1" s="37"/>
+      <c r="X1" s="37"/>
+      <c r="Y1" s="37"/>
+      <c r="Z1" s="37"/>
+      <c r="AA1" s="37"/>
+      <c r="AB1" s="37"/>
+      <c r="AC1" s="37"/>
+      <c r="AD1" s="37"/>
+      <c r="AE1" s="37"/>
+      <c r="AF1" s="37"/>
+      <c r="AG1" s="37"/>
+      <c r="AH1" s="37"/>
+      <c r="AI1" s="37"/>
+      <c r="AJ1" s="37"/>
+      <c r="AK1" s="34" t="s">
         <v>63</v>
       </c>
-      <c r="AL1" s="28"/>
+      <c r="AL1" s="35"/>
     </row>
     <row r="2" spans="2:38" x14ac:dyDescent="0.3">
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
-      <c r="K2" s="30"/>
-      <c r="L2" s="30"/>
-      <c r="M2" s="30"/>
-      <c r="N2" s="30"/>
-      <c r="O2" s="30"/>
-      <c r="P2" s="30"/>
-      <c r="Q2" s="30"/>
-      <c r="R2" s="30"/>
-      <c r="S2" s="30"/>
-      <c r="T2" s="30"/>
-      <c r="U2" s="30"/>
-      <c r="V2" s="30"/>
-      <c r="W2" s="30"/>
-      <c r="X2" s="30"/>
-      <c r="Y2" s="30"/>
-      <c r="Z2" s="30"/>
-      <c r="AA2" s="30"/>
-      <c r="AB2" s="30"/>
-      <c r="AC2" s="30"/>
-      <c r="AD2" s="30"/>
-      <c r="AE2" s="30"/>
-      <c r="AF2" s="30"/>
-      <c r="AG2" s="30"/>
-      <c r="AH2" s="30"/>
-      <c r="AI2" s="30"/>
-      <c r="AJ2" s="30"/>
-      <c r="AK2" s="29" t="s">
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
+      <c r="K2" s="37"/>
+      <c r="L2" s="37"/>
+      <c r="M2" s="37"/>
+      <c r="N2" s="37"/>
+      <c r="O2" s="37"/>
+      <c r="P2" s="37"/>
+      <c r="Q2" s="37"/>
+      <c r="R2" s="37"/>
+      <c r="S2" s="37"/>
+      <c r="T2" s="37"/>
+      <c r="U2" s="37"/>
+      <c r="V2" s="37"/>
+      <c r="W2" s="37"/>
+      <c r="X2" s="37"/>
+      <c r="Y2" s="37"/>
+      <c r="Z2" s="37"/>
+      <c r="AA2" s="37"/>
+      <c r="AB2" s="37"/>
+      <c r="AC2" s="37"/>
+      <c r="AD2" s="37"/>
+      <c r="AE2" s="37"/>
+      <c r="AF2" s="37"/>
+      <c r="AG2" s="37"/>
+      <c r="AH2" s="37"/>
+      <c r="AI2" s="37"/>
+      <c r="AJ2" s="37"/>
+      <c r="AK2" s="36" t="s">
         <v>64</v>
       </c>
-      <c r="AL2" s="29"/>
+      <c r="AL2" s="36"/>
     </row>
     <row r="3" spans="2:38" ht="29.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="21" t="s">
+      <c r="D3" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
-      <c r="H3" s="21"/>
-      <c r="I3" s="50"/>
-      <c r="J3" s="50"/>
-      <c r="K3" s="50"/>
-      <c r="L3" s="50"/>
-      <c r="M3" s="50"/>
-      <c r="N3" s="50"/>
-      <c r="O3" s="50"/>
-      <c r="P3" s="50"/>
-      <c r="Q3" s="50"/>
-      <c r="R3" s="50"/>
-      <c r="S3" s="50"/>
-      <c r="T3" s="50"/>
-      <c r="U3" s="50"/>
-      <c r="V3" s="48" t="s">
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="20"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
+      <c r="K3" s="25"/>
+      <c r="L3" s="25"/>
+      <c r="M3" s="25"/>
+      <c r="N3" s="25"/>
+      <c r="O3" s="25"/>
+      <c r="P3" s="25"/>
+      <c r="Q3" s="25"/>
+      <c r="R3" s="25"/>
+      <c r="S3" s="25"/>
+      <c r="T3" s="25"/>
+      <c r="U3" s="25"/>
+      <c r="V3" s="31" t="s">
         <v>68</v>
       </c>
-      <c r="W3" s="52" t="s">
+      <c r="W3" s="30" t="s">
         <v>69</v>
       </c>
-      <c r="X3" s="34" t="s">
+      <c r="X3" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="Y3" s="35"/>
-      <c r="Z3" s="35"/>
-      <c r="AA3" s="35"/>
-      <c r="AB3" s="35"/>
-      <c r="AC3" s="36"/>
+      <c r="Y3" s="40"/>
+      <c r="Z3" s="40"/>
+      <c r="AA3" s="40"/>
+      <c r="AB3" s="40"/>
+      <c r="AC3" s="41"/>
     </row>
     <row r="4" spans="2:38" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C4" s="31" t="s">
+      <c r="C4" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="32"/>
-      <c r="E4" s="32"/>
-      <c r="F4" s="32"/>
-      <c r="G4" s="32"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="31" t="s">
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="J4" s="32"/>
-      <c r="K4" s="32"/>
-      <c r="L4" s="32"/>
-      <c r="M4" s="32"/>
-      <c r="N4" s="33"/>
-      <c r="O4" s="31" t="s">
+      <c r="J4" s="27"/>
+      <c r="K4" s="27"/>
+      <c r="L4" s="27"/>
+      <c r="M4" s="27"/>
+      <c r="N4" s="38"/>
+      <c r="O4" s="26" t="s">
         <v>66</v>
       </c>
-      <c r="P4" s="32"/>
-      <c r="Q4" s="32"/>
-      <c r="R4" s="32"/>
-      <c r="S4" s="32"/>
-      <c r="T4" s="32"/>
-      <c r="U4" s="53" t="s">
+      <c r="P4" s="27"/>
+      <c r="Q4" s="27"/>
+      <c r="R4" s="27"/>
+      <c r="S4" s="27"/>
+      <c r="T4" s="27"/>
+      <c r="U4" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="V4" s="48"/>
-      <c r="W4" s="48"/>
-      <c r="X4" s="31" t="s">
+      <c r="V4" s="31"/>
+      <c r="W4" s="31"/>
+      <c r="X4" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="Y4" s="32"/>
-      <c r="Z4" s="32"/>
-      <c r="AA4" s="32"/>
-      <c r="AB4" s="32"/>
-      <c r="AC4" s="33"/>
+      <c r="Y4" s="27"/>
+      <c r="Z4" s="27"/>
+      <c r="AA4" s="27"/>
+      <c r="AB4" s="27"/>
+      <c r="AC4" s="38"/>
     </row>
     <row r="5" spans="2:38" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="4"/>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="15" t="s">
+      <c r="D5" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="15" t="s">
+      <c r="E5" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="F5" s="15" t="s">
+      <c r="F5" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="G5" s="15" t="s">
+      <c r="G5" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="H5" s="12" t="s">
+      <c r="H5" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="I5" s="11" t="s">
+      <c r="I5" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="J5" s="15" t="s">
+      <c r="J5" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="K5" s="15" t="s">
+      <c r="K5" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="L5" s="15" t="s">
+      <c r="L5" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="M5" s="15" t="s">
+      <c r="M5" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="N5" s="12" t="s">
+      <c r="N5" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="O5" s="11" t="s">
+      <c r="O5" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="P5" s="15" t="s">
+      <c r="P5" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="Q5" s="15" t="s">
+      <c r="Q5" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="R5" s="15" t="s">
+      <c r="R5" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="S5" s="15" t="s">
+      <c r="S5" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="T5" s="12" t="s">
+      <c r="T5" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="U5" s="51"/>
-      <c r="V5" s="49"/>
-      <c r="W5" s="49"/>
-      <c r="X5" s="15" t="s">
+      <c r="U5" s="29"/>
+      <c r="V5" s="32"/>
+      <c r="W5" s="32"/>
+      <c r="X5" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="Y5" s="15" t="s">
+      <c r="Y5" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="Z5" s="15" t="s">
+      <c r="Z5" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="AA5" s="15" t="s">
+      <c r="AA5" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="AB5" s="15" t="s">
+      <c r="AB5" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="AC5" s="15" t="s">
+      <c r="AC5" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="AD5" s="15" t="s">
+      <c r="AD5" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="AE5" s="15" t="s">
+      <c r="AE5" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="AF5" s="15" t="s">
+      <c r="AF5" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="AG5" s="15" t="s">
+      <c r="AG5" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="AH5" s="15" t="s">
+      <c r="AH5" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="AI5" s="15" t="s">
+      <c r="AI5" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="AJ5" s="15" t="s">
+      <c r="AJ5" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="AK5" s="15" t="s">
+      <c r="AK5" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="AL5" s="15" t="s">
+      <c r="AL5" s="14" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="6" spans="2:38" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="53" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="23" t="s">
+      <c r="C6" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="D6" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="23" t="s">
+      <c r="E6" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="F6" s="23" t="s">
+      <c r="F6" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="G6" s="14" t="s">
+      <c r="G6" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="H6" s="14" t="s">
+      <c r="H6" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="I6" s="23" t="s">
+      <c r="I6" s="22" t="s">
         <v>73</v>
       </c>
-      <c r="J6" s="14" t="s">
+      <c r="J6" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="K6" s="23" t="s">
+      <c r="K6" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="L6" s="23" t="s">
+      <c r="L6" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="M6" s="14" t="s">
+      <c r="M6" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="N6" s="14" t="s">
+      <c r="N6" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="O6" s="23" t="s">
+      <c r="O6" s="22" t="s">
         <v>79</v>
       </c>
-      <c r="P6" s="14" t="s">
+      <c r="P6" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="Q6" s="23" t="s">
+      <c r="Q6" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="R6" s="23" t="s">
+      <c r="R6" s="22" t="s">
         <v>82</v>
       </c>
-      <c r="S6" s="14" t="s">
+      <c r="S6" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="T6" s="14" t="s">
+      <c r="T6" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="U6" s="14" t="s">
+      <c r="U6" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="V6" s="14" t="s">
+      <c r="V6" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="W6" s="14" t="s">
+      <c r="W6" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="X6" s="23" t="s">
+      <c r="X6" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="Y6" s="23" t="s">
+      <c r="Y6" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="Z6" s="23" t="s">
+      <c r="Z6" s="22" t="s">
         <v>86</v>
       </c>
-      <c r="AA6" s="23" t="s">
+      <c r="AA6" s="22" t="s">
         <v>90</v>
       </c>
-      <c r="AB6" s="14" t="s">
+      <c r="AB6" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="AC6" s="23" t="s">
+      <c r="AC6" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="AD6" s="23" t="s">
+      <c r="AD6" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="AE6" s="23" t="s">
+      <c r="AE6" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="AF6" s="23" t="s">
+      <c r="AF6" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="AG6" s="14" t="s">
+      <c r="AG6" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="AH6" s="22" t="s">
+      <c r="AH6" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="AI6" s="14" t="s">
+      <c r="AI6" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="AJ6" s="14" t="s">
+      <c r="AJ6" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="AK6" s="23" t="s">
+      <c r="AK6" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="AL6" s="14" t="s">
+      <c r="AL6" s="13" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="7" spans="2:38" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="9"/>
+      <c r="B7" s="8"/>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
       <c r="E7" s="7"/>
@@ -1904,90 +1904,90 @@
       <c r="G7" s="5"/>
     </row>
     <row r="8" spans="2:38" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="D8" s="13"/>
-      <c r="E8" s="24" t="s">
+      <c r="D8" s="12"/>
+      <c r="E8" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="13" t="s">
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="I8" s="13" t="s">
+      <c r="I8" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="J8" s="13"/>
-      <c r="K8" s="24" t="s">
+      <c r="J8" s="12"/>
+      <c r="K8" s="23" t="s">
         <v>92</v>
       </c>
-      <c r="L8" s="13"/>
-      <c r="M8" s="13"/>
-      <c r="N8" s="13" t="s">
+      <c r="L8" s="12"/>
+      <c r="M8" s="12"/>
+      <c r="N8" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="O8" s="13" t="s">
+      <c r="O8" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="P8" s="13"/>
-      <c r="Q8" s="24" t="s">
+      <c r="P8" s="12"/>
+      <c r="Q8" s="23" t="s">
         <v>95</v>
       </c>
-      <c r="R8" s="13"/>
-      <c r="S8" s="13"/>
-      <c r="T8" s="13" t="s">
+      <c r="R8" s="12"/>
+      <c r="S8" s="12"/>
+      <c r="T8" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="U8" s="13" t="s">
+      <c r="U8" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="V8" s="13" t="s">
+      <c r="V8" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="W8" s="13"/>
-      <c r="X8" s="24" t="s">
+      <c r="W8" s="12"/>
+      <c r="X8" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="Y8" s="24" t="s">
+      <c r="Y8" s="23" t="s">
         <v>97</v>
       </c>
-      <c r="Z8" s="24" t="s">
+      <c r="Z8" s="23" t="s">
         <v>98</v>
       </c>
-      <c r="AA8" s="24" t="s">
+      <c r="AA8" s="23" t="s">
         <v>99</v>
       </c>
-      <c r="AB8" s="13"/>
-      <c r="AC8" s="24" t="s">
+      <c r="AB8" s="12"/>
+      <c r="AC8" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="AD8" s="13"/>
-      <c r="AE8" s="13"/>
-      <c r="AF8" s="13"/>
-      <c r="AG8" s="13"/>
-      <c r="AH8" s="13"/>
-      <c r="AI8" s="13"/>
-      <c r="AJ8" s="13" t="s">
+      <c r="AD8" s="12"/>
+      <c r="AE8" s="12"/>
+      <c r="AF8" s="12"/>
+      <c r="AG8" s="12"/>
+      <c r="AH8" s="12"/>
+      <c r="AI8" s="12"/>
+      <c r="AJ8" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="AK8" s="24" t="s">
+      <c r="AK8" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="AL8" s="13" t="s">
+      <c r="AL8" s="12" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="9" spans="2:38" x14ac:dyDescent="0.3">
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
     </row>
     <row r="10" spans="2:38" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="1"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
       <c r="E10" s="2"/>
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
@@ -2009,12 +2009,12 @@
       <c r="W10" s="6"/>
     </row>
     <row r="11" spans="2:38" ht="16.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="45" t="s">
+      <c r="B11" s="50" t="s">
         <v>54</v>
       </c>
-      <c r="C11" s="46"/>
-      <c r="D11" s="47"/>
-      <c r="E11" s="25" t="s">
+      <c r="C11" s="51"/>
+      <c r="D11" s="52"/>
+      <c r="E11" s="24" t="s">
         <v>53</v>
       </c>
       <c r="F11" s="6"/>
@@ -2038,73 +2038,75 @@
     </row>
     <row r="12" spans="2:38" x14ac:dyDescent="0.3">
       <c r="B12" s="3"/>
-      <c r="C12" s="43"/>
-      <c r="D12" s="44"/>
+      <c r="C12" s="48"/>
+      <c r="D12" s="49"/>
     </row>
     <row r="13" spans="2:38" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B13" s="1"/>
-      <c r="C13" s="16"/>
-      <c r="D13" s="16"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15"/>
       <c r="E13" s="2"/>
     </row>
     <row r="14" spans="2:38" ht="39.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="37" t="s">
+      <c r="B14" s="42" t="s">
         <v>58</v>
       </c>
-      <c r="C14" s="38"/>
-      <c r="D14" s="39"/>
-      <c r="E14" s="19" t="s">
+      <c r="C14" s="43"/>
+      <c r="D14" s="44"/>
+      <c r="E14" s="18" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="15" spans="2:38" ht="43.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="40" t="s">
+      <c r="B15" s="45" t="s">
         <v>59</v>
       </c>
-      <c r="C15" s="41"/>
-      <c r="D15" s="42"/>
-      <c r="E15" s="19" t="s">
+      <c r="C15" s="46"/>
+      <c r="D15" s="47"/>
+      <c r="E15" s="18" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="16" spans="2:38" x14ac:dyDescent="0.3">
       <c r="B16" s="3"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B17" s="3"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B18" s="17" t="s">
+      <c r="B18" s="16" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B19" s="26" t="s">
+      <c r="B19" s="33" t="s">
         <v>60</v>
       </c>
-      <c r="C19" s="26"/>
-      <c r="D19" s="26"/>
+      <c r="C19" s="33"/>
+      <c r="D19" s="33"/>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B20" s="26" t="s">
+      <c r="B20" s="33" t="s">
         <v>61</v>
       </c>
-      <c r="C20" s="26"/>
-      <c r="D20" s="26"/>
+      <c r="C20" s="33"/>
+      <c r="D20" s="33"/>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B21" s="26" t="s">
+      <c r="B21" s="33" t="s">
         <v>62</v>
       </c>
-      <c r="C21" s="26"/>
-      <c r="D21" s="26"/>
+      <c r="C21" s="33"/>
+      <c r="D21" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="C4:H4"/>
+    <mergeCell ref="I4:N4"/>
     <mergeCell ref="O4:T4"/>
     <mergeCell ref="U4:U5"/>
     <mergeCell ref="W3:W5"/>
@@ -2121,8 +2123,6 @@
     <mergeCell ref="B11:D11"/>
     <mergeCell ref="B19:D19"/>
     <mergeCell ref="V3:V5"/>
-    <mergeCell ref="C4:H4"/>
-    <mergeCell ref="I4:N4"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" horizontalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Correccion de las Observaciones para Reporte Anexo 7
</commit_message>
<xml_diff>
--- a/Unna.OperationalReport.WebSite/wwwroot/plantillas/reporte/mensual/BoletadeValorizacionPetroperu.xlsx
+++ b/Unna.OperationalReport.WebSite/wwwroot/plantillas/reporte/mensual/BoletadeValorizacionPetroperu.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desarrollos\SP\APSS SP\ProyectoPrincipalAenza6\UnnaReportesOperativos\Unna.OperationalReport.WebSite\wwwroot\plantillas\reporte\mensual\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03F317C0-752D-47CE-AC5D-34B06E6BB3EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{420807EA-80B2-4D1C-BB1B-9D151D126C1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="111">
   <si>
     <t>Energía
 (MMBTU)</t>
@@ -397,6 +397,9 @@
   <si>
     <t>MONTO
 (US$)</t>
+  </si>
+  <si>
+    <t>{{Observacion4}}</t>
   </si>
 </sst>
 </file>
@@ -889,7 +892,7 @@
     <xf numFmtId="168" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="169" fontId="7" fillId="4" borderId="0" xfId="103" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -963,6 +966,33 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="8" fillId="0" borderId="0" xfId="103" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="103" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="9" fillId="0" borderId="1" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -975,6 +1005,63 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="2" xfId="103" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="3" xfId="103" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="11" xfId="103" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="12" xfId="103" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="8" xfId="103" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="13" xfId="103" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" xfId="103" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="6" xfId="103" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="15" xfId="103" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="16" xfId="103" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="17" xfId="103" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -982,91 +1069,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="2" xfId="103" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="3" xfId="103" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="11" xfId="103" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="12" xfId="103" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="8" xfId="103" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="13" xfId="103" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" xfId="103" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="6" xfId="103" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="15" xfId="103" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="16" xfId="103" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="17" xfId="103" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="8" fillId="0" borderId="0" xfId="103" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="103" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" xfId="103" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="9" fillId="0" borderId="1" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="104">
@@ -1199,13 +1205,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>1150620</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>37</xdr:row>
       <xdr:rowOff>76201</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1619250</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:row>42</xdr:row>
       <xdr:rowOff>97340</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1684,11 +1690,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:AL24"/>
+  <dimension ref="B1:AL31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F17" sqref="F17"/>
+      <selection pane="bottomLeft" activeCell="B31" sqref="B31:O31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
@@ -1707,92 +1713,92 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:38" ht="27" customHeight="1">
-      <c r="C1" s="37" t="s">
+      <c r="C1" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
-      <c r="K1" s="37"/>
-      <c r="L1" s="37"/>
-      <c r="M1" s="37"/>
-      <c r="N1" s="37"/>
-      <c r="O1" s="37"/>
-      <c r="P1" s="37"/>
-      <c r="Q1" s="37"/>
-      <c r="R1" s="37"/>
-      <c r="S1" s="37"/>
-      <c r="T1" s="37"/>
-      <c r="U1" s="37"/>
-      <c r="V1" s="37"/>
-      <c r="W1" s="37"/>
-      <c r="X1" s="37"/>
-      <c r="Y1" s="37"/>
-      <c r="Z1" s="37"/>
-      <c r="AA1" s="37"/>
-      <c r="AB1" s="37"/>
-      <c r="AC1" s="37"/>
-      <c r="AD1" s="37"/>
-      <c r="AE1" s="37"/>
-      <c r="AF1" s="37"/>
-      <c r="AG1" s="37"/>
-      <c r="AH1" s="37"/>
-      <c r="AI1" s="37"/>
-      <c r="AJ1" s="37"/>
-      <c r="AK1" s="34" t="s">
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="43"/>
+      <c r="J1" s="43"/>
+      <c r="K1" s="43"/>
+      <c r="L1" s="43"/>
+      <c r="M1" s="43"/>
+      <c r="N1" s="43"/>
+      <c r="O1" s="43"/>
+      <c r="P1" s="43"/>
+      <c r="Q1" s="43"/>
+      <c r="R1" s="43"/>
+      <c r="S1" s="43"/>
+      <c r="T1" s="43"/>
+      <c r="U1" s="43"/>
+      <c r="V1" s="43"/>
+      <c r="W1" s="43"/>
+      <c r="X1" s="43"/>
+      <c r="Y1" s="43"/>
+      <c r="Z1" s="43"/>
+      <c r="AA1" s="43"/>
+      <c r="AB1" s="43"/>
+      <c r="AC1" s="43"/>
+      <c r="AD1" s="43"/>
+      <c r="AE1" s="43"/>
+      <c r="AF1" s="43"/>
+      <c r="AG1" s="43"/>
+      <c r="AH1" s="43"/>
+      <c r="AI1" s="43"/>
+      <c r="AJ1" s="43"/>
+      <c r="AK1" s="40" t="s">
         <v>63</v>
       </c>
-      <c r="AL1" s="35"/>
+      <c r="AL1" s="41"/>
     </row>
     <row r="2" spans="2:38" ht="15" thickBot="1">
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
-      <c r="K2" s="37"/>
-      <c r="L2" s="37"/>
-      <c r="M2" s="37"/>
-      <c r="N2" s="37"/>
-      <c r="O2" s="37"/>
-      <c r="P2" s="37"/>
-      <c r="Q2" s="37"/>
-      <c r="R2" s="37"/>
-      <c r="S2" s="37"/>
-      <c r="T2" s="37"/>
-      <c r="U2" s="37"/>
-      <c r="V2" s="37"/>
-      <c r="W2" s="37"/>
-      <c r="X2" s="37"/>
-      <c r="Y2" s="37"/>
-      <c r="Z2" s="37"/>
-      <c r="AA2" s="37"/>
-      <c r="AB2" s="37"/>
-      <c r="AC2" s="37"/>
-      <c r="AD2" s="37"/>
-      <c r="AE2" s="37"/>
-      <c r="AF2" s="37"/>
-      <c r="AG2" s="37"/>
-      <c r="AH2" s="37"/>
-      <c r="AI2" s="37"/>
-      <c r="AJ2" s="37"/>
-      <c r="AK2" s="36" t="s">
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
+      <c r="K2" s="43"/>
+      <c r="L2" s="43"/>
+      <c r="M2" s="43"/>
+      <c r="N2" s="43"/>
+      <c r="O2" s="43"/>
+      <c r="P2" s="43"/>
+      <c r="Q2" s="43"/>
+      <c r="R2" s="43"/>
+      <c r="S2" s="43"/>
+      <c r="T2" s="43"/>
+      <c r="U2" s="43"/>
+      <c r="V2" s="43"/>
+      <c r="W2" s="43"/>
+      <c r="X2" s="43"/>
+      <c r="Y2" s="43"/>
+      <c r="Z2" s="43"/>
+      <c r="AA2" s="43"/>
+      <c r="AB2" s="43"/>
+      <c r="AC2" s="43"/>
+      <c r="AD2" s="43"/>
+      <c r="AE2" s="43"/>
+      <c r="AF2" s="43"/>
+      <c r="AG2" s="43"/>
+      <c r="AH2" s="43"/>
+      <c r="AI2" s="43"/>
+      <c r="AJ2" s="43"/>
+      <c r="AK2" s="42" t="s">
         <v>64</v>
       </c>
-      <c r="AL2" s="36"/>
+      <c r="AL2" s="42"/>
     </row>
     <row r="3" spans="2:38" ht="15" thickBot="1">
-      <c r="C3" s="54" t="s">
+      <c r="C3" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="54" t="s">
+      <c r="D3" s="27" t="s">
         <v>26</v>
       </c>
       <c r="E3" s="25"/>
@@ -1831,80 +1837,80 @@
       <c r="AL3" s="24"/>
     </row>
     <row r="4" spans="2:38" ht="29.4" customHeight="1" thickBot="1">
-      <c r="C4" s="38" t="s">
+      <c r="C4" s="32" t="s">
         <v>105</v>
       </c>
-      <c r="D4" s="39"/>
-      <c r="E4" s="39"/>
-      <c r="F4" s="39"/>
-      <c r="G4" s="39"/>
-      <c r="H4" s="39"/>
-      <c r="I4" s="39"/>
-      <c r="J4" s="39"/>
-      <c r="K4" s="39"/>
-      <c r="L4" s="39"/>
-      <c r="M4" s="39"/>
-      <c r="N4" s="39"/>
-      <c r="O4" s="39"/>
-      <c r="P4" s="39"/>
-      <c r="Q4" s="39"/>
-      <c r="R4" s="39"/>
-      <c r="S4" s="39"/>
-      <c r="T4" s="39"/>
-      <c r="U4" s="40"/>
-      <c r="V4" s="27" t="s">
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="33"/>
+      <c r="J4" s="33"/>
+      <c r="K4" s="33"/>
+      <c r="L4" s="33"/>
+      <c r="M4" s="33"/>
+      <c r="N4" s="33"/>
+      <c r="O4" s="33"/>
+      <c r="P4" s="33"/>
+      <c r="Q4" s="33"/>
+      <c r="R4" s="33"/>
+      <c r="S4" s="33"/>
+      <c r="T4" s="33"/>
+      <c r="U4" s="34"/>
+      <c r="V4" s="36" t="s">
         <v>68</v>
       </c>
-      <c r="W4" s="27" t="s">
+      <c r="W4" s="36" t="s">
         <v>69</v>
       </c>
-      <c r="X4" s="38" t="s">
+      <c r="X4" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="Y4" s="39"/>
-      <c r="Z4" s="39"/>
-      <c r="AA4" s="39"/>
-      <c r="AB4" s="39"/>
-      <c r="AC4" s="40"/>
+      <c r="Y4" s="33"/>
+      <c r="Z4" s="33"/>
+      <c r="AA4" s="33"/>
+      <c r="AB4" s="33"/>
+      <c r="AC4" s="34"/>
     </row>
     <row r="5" spans="2:38" ht="15" thickBot="1">
-      <c r="C5" s="38" t="s">
+      <c r="C5" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="39"/>
-      <c r="E5" s="39"/>
-      <c r="F5" s="39"/>
-      <c r="G5" s="39"/>
-      <c r="H5" s="40"/>
-      <c r="I5" s="38" t="s">
+      <c r="D5" s="33"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="33"/>
+      <c r="H5" s="34"/>
+      <c r="I5" s="32" t="s">
         <v>65</v>
       </c>
-      <c r="J5" s="39"/>
-      <c r="K5" s="39"/>
-      <c r="L5" s="39"/>
-      <c r="M5" s="39"/>
-      <c r="N5" s="40"/>
-      <c r="O5" s="38" t="s">
+      <c r="J5" s="33"/>
+      <c r="K5" s="33"/>
+      <c r="L5" s="33"/>
+      <c r="M5" s="33"/>
+      <c r="N5" s="34"/>
+      <c r="O5" s="32" t="s">
         <v>66</v>
       </c>
-      <c r="P5" s="39"/>
-      <c r="Q5" s="39"/>
-      <c r="R5" s="39"/>
-      <c r="S5" s="39"/>
-      <c r="T5" s="39"/>
-      <c r="U5" s="27" t="s">
+      <c r="P5" s="33"/>
+      <c r="Q5" s="33"/>
+      <c r="R5" s="33"/>
+      <c r="S5" s="33"/>
+      <c r="T5" s="33"/>
+      <c r="U5" s="36" t="s">
         <v>67</v>
       </c>
-      <c r="V5" s="29"/>
-      <c r="W5" s="29"/>
-      <c r="X5" s="38" t="s">
+      <c r="V5" s="38"/>
+      <c r="W5" s="38"/>
+      <c r="X5" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="Y5" s="39"/>
-      <c r="Z5" s="39"/>
-      <c r="AA5" s="39"/>
-      <c r="AB5" s="39"/>
-      <c r="AC5" s="40"/>
+      <c r="Y5" s="33"/>
+      <c r="Z5" s="33"/>
+      <c r="AA5" s="33"/>
+      <c r="AB5" s="33"/>
+      <c r="AC5" s="34"/>
     </row>
     <row r="6" spans="2:38" ht="58.2" thickBot="1">
       <c r="B6" s="4"/>
@@ -1962,9 +1968,9 @@
       <c r="T6" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="U6" s="28"/>
-      <c r="V6" s="30"/>
-      <c r="W6" s="30"/>
+      <c r="U6" s="37"/>
+      <c r="V6" s="39"/>
+      <c r="W6" s="39"/>
       <c r="X6" s="14" t="s">
         <v>8</v>
       </c>
@@ -2222,10 +2228,10 @@
       <c r="E11" s="9"/>
     </row>
     <row r="12" spans="2:38" ht="24.6" customHeight="1">
-      <c r="B12" s="56" t="s">
+      <c r="B12" s="35" t="s">
         <v>107</v>
       </c>
-      <c r="C12" s="56"/>
+      <c r="C12" s="35"/>
       <c r="D12" s="9"/>
       <c r="E12" s="9"/>
     </row>
@@ -2234,8 +2240,8 @@
         <v>108</v>
       </c>
       <c r="C13" s="57"/>
-      <c r="D13" s="58"/>
-      <c r="E13" s="59"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="30"/>
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
       <c r="H13" s="6"/>
@@ -2256,11 +2262,11 @@
       <c r="W13" s="6"/>
     </row>
     <row r="14" spans="2:38" ht="16.8" customHeight="1" thickBot="1">
-      <c r="B14" s="50" t="s">
+      <c r="B14" s="54" t="s">
         <v>54</v>
       </c>
-      <c r="C14" s="51"/>
-      <c r="D14" s="52"/>
+      <c r="C14" s="55"/>
+      <c r="D14" s="56"/>
       <c r="E14" s="22" t="s">
         <v>53</v>
       </c>
@@ -2285,95 +2291,243 @@
     </row>
     <row r="15" spans="2:38" ht="15" thickBot="1">
       <c r="B15" s="3"/>
-      <c r="C15" s="48"/>
-      <c r="D15" s="49"/>
+      <c r="C15" s="52"/>
+      <c r="D15" s="53"/>
     </row>
     <row r="16" spans="2:38" ht="29.4" thickBot="1">
-      <c r="B16" s="60"/>
-      <c r="C16" s="58"/>
-      <c r="D16" s="58"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="29"/>
+      <c r="D16" s="29"/>
       <c r="E16" s="14" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="17" spans="2:5" ht="39.6" customHeight="1" thickBot="1">
-      <c r="B17" s="42" t="s">
+    <row r="17" spans="2:15" ht="39.6" customHeight="1" thickBot="1">
+      <c r="B17" s="46" t="s">
         <v>58</v>
       </c>
-      <c r="C17" s="43"/>
-      <c r="D17" s="44"/>
-      <c r="E17" s="61" t="s">
+      <c r="C17" s="47"/>
+      <c r="D17" s="48"/>
+      <c r="E17" s="31" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="18" spans="2:5" ht="43.8" customHeight="1" thickBot="1">
-      <c r="B18" s="45" t="s">
+    <row r="18" spans="2:15" ht="43.8" customHeight="1" thickBot="1">
+      <c r="B18" s="49" t="s">
         <v>59</v>
       </c>
-      <c r="C18" s="46"/>
-      <c r="D18" s="47"/>
-      <c r="E18" s="61" t="s">
+      <c r="C18" s="50"/>
+      <c r="D18" s="51"/>
+      <c r="E18" s="31" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="19" spans="2:5">
+    <row r="19" spans="2:15">
       <c r="B19" s="3"/>
       <c r="C19" s="17"/>
       <c r="D19" s="17"/>
     </row>
-    <row r="20" spans="2:5">
+    <row r="20" spans="2:15">
       <c r="B20" s="3"/>
       <c r="C20" s="17"/>
       <c r="D20" s="17"/>
     </row>
-    <row r="21" spans="2:5">
+    <row r="21" spans="2:15">
       <c r="B21" s="16" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="22" spans="2:5">
-      <c r="B22" s="33" t="s">
+    <row r="22" spans="2:15">
+      <c r="B22" s="61" t="s">
         <v>60</v>
       </c>
-      <c r="C22" s="33"/>
-      <c r="D22" s="33"/>
-    </row>
-    <row r="23" spans="2:5">
-      <c r="B23" s="33" t="s">
+      <c r="C22" s="61"/>
+      <c r="D22" s="61"/>
+      <c r="E22" s="61"/>
+      <c r="F22" s="61"/>
+      <c r="G22" s="61"/>
+      <c r="H22" s="61"/>
+      <c r="I22" s="61"/>
+      <c r="J22" s="61"/>
+      <c r="K22" s="61"/>
+      <c r="L22" s="61"/>
+      <c r="M22" s="61"/>
+      <c r="N22" s="61"/>
+      <c r="O22" s="61"/>
+    </row>
+    <row r="23" spans="2:15">
+      <c r="B23" s="61"/>
+      <c r="C23" s="61"/>
+      <c r="D23" s="61"/>
+      <c r="E23" s="61"/>
+      <c r="F23" s="61"/>
+      <c r="G23" s="61"/>
+      <c r="H23" s="61"/>
+      <c r="I23" s="61"/>
+      <c r="J23" s="61"/>
+      <c r="K23" s="61"/>
+      <c r="L23" s="61"/>
+      <c r="M23" s="61"/>
+      <c r="N23" s="61"/>
+      <c r="O23" s="61"/>
+    </row>
+    <row r="24" spans="2:15">
+      <c r="B24" s="61"/>
+      <c r="C24" s="61"/>
+      <c r="D24" s="61"/>
+      <c r="E24" s="61"/>
+      <c r="F24" s="61"/>
+      <c r="G24" s="61"/>
+      <c r="H24" s="61"/>
+      <c r="I24" s="61"/>
+      <c r="J24" s="61"/>
+      <c r="K24" s="61"/>
+      <c r="L24" s="61"/>
+      <c r="M24" s="61"/>
+      <c r="N24" s="61"/>
+      <c r="O24" s="61"/>
+    </row>
+    <row r="25" spans="2:15">
+      <c r="B25" s="61"/>
+      <c r="C25" s="61"/>
+      <c r="D25" s="61"/>
+      <c r="E25" s="61"/>
+      <c r="F25" s="61"/>
+      <c r="G25" s="61"/>
+      <c r="H25" s="61"/>
+      <c r="I25" s="61"/>
+      <c r="J25" s="61"/>
+      <c r="K25" s="61"/>
+      <c r="L25" s="61"/>
+      <c r="M25" s="61"/>
+      <c r="N25" s="61"/>
+      <c r="O25" s="61"/>
+    </row>
+    <row r="26" spans="2:15">
+      <c r="B26" s="61"/>
+      <c r="C26" s="61"/>
+      <c r="D26" s="61"/>
+      <c r="E26" s="61"/>
+      <c r="F26" s="61"/>
+      <c r="G26" s="61"/>
+      <c r="H26" s="61"/>
+      <c r="I26" s="61"/>
+      <c r="J26" s="61"/>
+      <c r="K26" s="61"/>
+      <c r="L26" s="61"/>
+      <c r="M26" s="61"/>
+      <c r="N26" s="61"/>
+      <c r="O26" s="61"/>
+    </row>
+    <row r="27" spans="2:15">
+      <c r="B27" s="61"/>
+      <c r="C27" s="61"/>
+      <c r="D27" s="61"/>
+      <c r="E27" s="61"/>
+      <c r="F27" s="61"/>
+      <c r="G27" s="61"/>
+      <c r="H27" s="61"/>
+      <c r="I27" s="61"/>
+      <c r="J27" s="61"/>
+      <c r="K27" s="61"/>
+      <c r="L27" s="61"/>
+      <c r="M27" s="61"/>
+      <c r="N27" s="61"/>
+      <c r="O27" s="61"/>
+    </row>
+    <row r="28" spans="2:15">
+      <c r="B28" s="24"/>
+      <c r="C28" s="24"/>
+      <c r="D28" s="24"/>
+      <c r="E28" s="24"/>
+      <c r="F28" s="24"/>
+      <c r="G28" s="24"/>
+      <c r="H28" s="24"/>
+      <c r="I28" s="24"/>
+      <c r="J28" s="24"/>
+      <c r="K28" s="24"/>
+      <c r="L28" s="24"/>
+      <c r="M28" s="24"/>
+      <c r="N28" s="24"/>
+      <c r="O28" s="24"/>
+    </row>
+    <row r="29" spans="2:15">
+      <c r="B29" s="62" t="s">
         <v>61</v>
       </c>
-      <c r="C23" s="33"/>
-      <c r="D23" s="33"/>
-    </row>
-    <row r="24" spans="2:5">
-      <c r="B24" s="33" t="s">
+      <c r="C29" s="62"/>
+      <c r="D29" s="62"/>
+      <c r="E29" s="62"/>
+      <c r="F29" s="62"/>
+      <c r="G29" s="62"/>
+      <c r="H29" s="62"/>
+      <c r="I29" s="62"/>
+      <c r="J29" s="62"/>
+      <c r="K29" s="62"/>
+      <c r="L29" s="62"/>
+      <c r="M29" s="62"/>
+      <c r="N29" s="62"/>
+      <c r="O29" s="62"/>
+    </row>
+    <row r="30" spans="2:15">
+      <c r="B30" s="62" t="s">
         <v>62</v>
       </c>
-      <c r="C24" s="33"/>
-      <c r="D24" s="33"/>
+      <c r="C30" s="62"/>
+      <c r="D30" s="62"/>
+      <c r="E30" s="62"/>
+      <c r="F30" s="62"/>
+      <c r="G30" s="62"/>
+      <c r="H30" s="62"/>
+      <c r="I30" s="62"/>
+      <c r="J30" s="62"/>
+      <c r="K30" s="62"/>
+      <c r="L30" s="62"/>
+      <c r="M30" s="62"/>
+      <c r="N30" s="62"/>
+      <c r="O30" s="62"/>
+    </row>
+    <row r="31" spans="2:15">
+      <c r="B31" s="62" t="s">
+        <v>110</v>
+      </c>
+      <c r="C31" s="62"/>
+      <c r="D31" s="62"/>
+      <c r="E31" s="62"/>
+      <c r="F31" s="62"/>
+      <c r="G31" s="62"/>
+      <c r="H31" s="62"/>
+      <c r="I31" s="62"/>
+      <c r="J31" s="62"/>
+      <c r="K31" s="62"/>
+      <c r="L31" s="62"/>
+      <c r="M31" s="62"/>
+      <c r="N31" s="62"/>
+      <c r="O31" s="62"/>
     </row>
   </sheetData>
-  <mergeCells count="21">
-    <mergeCell ref="B13:C13"/>
+  <mergeCells count="22">
+    <mergeCell ref="B29:O29"/>
+    <mergeCell ref="B30:O30"/>
+    <mergeCell ref="B31:O31"/>
     <mergeCell ref="C5:H5"/>
     <mergeCell ref="I5:N5"/>
     <mergeCell ref="O5:T5"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B22:O27"/>
     <mergeCell ref="C4:U4"/>
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="U5:U6"/>
     <mergeCell ref="W4:W6"/>
-    <mergeCell ref="B24:D24"/>
     <mergeCell ref="AK1:AL1"/>
     <mergeCell ref="AK2:AL2"/>
     <mergeCell ref="C1:AJ2"/>
     <mergeCell ref="X5:AC5"/>
     <mergeCell ref="X4:AC4"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="B22:D22"/>
     <mergeCell ref="V4:V6"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2405,58 +2559,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:21" ht="27" customHeight="1">
-      <c r="C1" s="37" t="s">
+      <c r="C1" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
-      <c r="K1" s="37"/>
-      <c r="L1" s="37"/>
-      <c r="M1" s="37"/>
-      <c r="N1" s="37"/>
-      <c r="O1" s="37"/>
-      <c r="P1" s="37"/>
-      <c r="Q1" s="37"/>
-      <c r="R1" s="37"/>
-      <c r="S1" s="37"/>
-      <c r="T1" s="34" t="s">
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="43"/>
+      <c r="J1" s="43"/>
+      <c r="K1" s="43"/>
+      <c r="L1" s="43"/>
+      <c r="M1" s="43"/>
+      <c r="N1" s="43"/>
+      <c r="O1" s="43"/>
+      <c r="P1" s="43"/>
+      <c r="Q1" s="43"/>
+      <c r="R1" s="43"/>
+      <c r="S1" s="43"/>
+      <c r="T1" s="40" t="s">
         <v>63</v>
       </c>
-      <c r="U1" s="35"/>
+      <c r="U1" s="41"/>
     </row>
     <row r="2" spans="2:21" ht="15" thickBot="1">
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
-      <c r="K2" s="37"/>
-      <c r="L2" s="37"/>
-      <c r="M2" s="37"/>
-      <c r="N2" s="37"/>
-      <c r="O2" s="37"/>
-      <c r="P2" s="37"/>
-      <c r="Q2" s="37"/>
-      <c r="R2" s="37"/>
-      <c r="S2" s="37"/>
-      <c r="T2" s="36" t="s">
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
+      <c r="K2" s="43"/>
+      <c r="L2" s="43"/>
+      <c r="M2" s="43"/>
+      <c r="N2" s="43"/>
+      <c r="O2" s="43"/>
+      <c r="P2" s="43"/>
+      <c r="Q2" s="43"/>
+      <c r="R2" s="43"/>
+      <c r="S2" s="43"/>
+      <c r="T2" s="42" t="s">
         <v>64</v>
       </c>
-      <c r="U2" s="36"/>
+      <c r="U2" s="42"/>
     </row>
     <row r="3" spans="2:21" ht="15" thickBot="1">
-      <c r="C3" s="55" t="s">
+      <c r="C3" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="55" t="s">
+      <c r="D3" s="28" t="s">
         <v>26</v>
       </c>
       <c r="E3" s="25"/>
@@ -2478,38 +2632,38 @@
       <c r="U3" s="24"/>
     </row>
     <row r="4" spans="2:21" ht="29.4" customHeight="1" thickBot="1">
-      <c r="C4" s="38" t="s">
+      <c r="C4" s="32" t="s">
         <v>105</v>
       </c>
-      <c r="D4" s="39"/>
-      <c r="E4" s="39"/>
-      <c r="F4" s="39"/>
-      <c r="G4" s="39"/>
-      <c r="H4" s="40"/>
-      <c r="I4" s="27" t="s">
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="34"/>
+      <c r="I4" s="36" t="s">
         <v>68</v>
       </c>
-      <c r="J4" s="41" t="s">
+      <c r="J4" s="58" t="s">
         <v>12</v>
       </c>
-      <c r="K4" s="31"/>
-      <c r="L4" s="32"/>
+      <c r="K4" s="59"/>
+      <c r="L4" s="60"/>
     </row>
     <row r="5" spans="2:21" ht="15" thickBot="1">
-      <c r="C5" s="38" t="s">
+      <c r="C5" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="39"/>
-      <c r="E5" s="39"/>
-      <c r="F5" s="39"/>
-      <c r="G5" s="39"/>
-      <c r="H5" s="40"/>
-      <c r="I5" s="29"/>
-      <c r="J5" s="38" t="s">
+      <c r="D5" s="33"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="33"/>
+      <c r="H5" s="34"/>
+      <c r="I5" s="38"/>
+      <c r="J5" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="K5" s="39"/>
-      <c r="L5" s="40"/>
+      <c r="K5" s="33"/>
+      <c r="L5" s="34"/>
     </row>
     <row r="6" spans="2:21" ht="58.2" thickBot="1">
       <c r="B6" s="4"/>
@@ -2531,7 +2685,7 @@
       <c r="H6" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="I6" s="30"/>
+      <c r="I6" s="39"/>
       <c r="J6" s="14" t="s">
         <v>8</v>
       </c>
@@ -2694,11 +2848,11 @@
       <c r="I11" s="6"/>
     </row>
     <row r="12" spans="2:21" ht="16.8" customHeight="1" thickBot="1">
-      <c r="B12" s="50" t="s">
+      <c r="B12" s="54" t="s">
         <v>54</v>
       </c>
-      <c r="C12" s="51"/>
-      <c r="D12" s="52"/>
+      <c r="C12" s="55"/>
+      <c r="D12" s="56"/>
       <c r="E12" s="22" t="s">
         <v>53</v>
       </c>
@@ -2709,8 +2863,8 @@
     </row>
     <row r="13" spans="2:21">
       <c r="B13" s="3"/>
-      <c r="C13" s="48"/>
-      <c r="D13" s="49"/>
+      <c r="C13" s="52"/>
+      <c r="D13" s="53"/>
     </row>
     <row r="14" spans="2:21" ht="15" thickBot="1">
       <c r="B14" s="1"/>
@@ -2719,21 +2873,21 @@
       <c r="E14" s="2"/>
     </row>
     <row r="15" spans="2:21" ht="39.6" customHeight="1" thickBot="1">
-      <c r="B15" s="42" t="s">
+      <c r="B15" s="46" t="s">
         <v>58</v>
       </c>
-      <c r="C15" s="43"/>
-      <c r="D15" s="44"/>
+      <c r="C15" s="47"/>
+      <c r="D15" s="48"/>
       <c r="E15" s="18" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="16" spans="2:21" ht="43.8" customHeight="1" thickBot="1">
-      <c r="B16" s="45" t="s">
+      <c r="B16" s="49" t="s">
         <v>59</v>
       </c>
-      <c r="C16" s="46"/>
-      <c r="D16" s="47"/>
+      <c r="C16" s="50"/>
+      <c r="D16" s="51"/>
       <c r="E16" s="18" t="s">
         <v>104</v>
       </c>
@@ -2754,25 +2908,25 @@
       </c>
     </row>
     <row r="20" spans="2:4">
-      <c r="B20" s="33" t="s">
+      <c r="B20" s="45" t="s">
         <v>60</v>
       </c>
-      <c r="C20" s="33"/>
-      <c r="D20" s="33"/>
+      <c r="C20" s="45"/>
+      <c r="D20" s="45"/>
     </row>
     <row r="21" spans="2:4">
-      <c r="B21" s="33" t="s">
+      <c r="B21" s="45" t="s">
         <v>61</v>
       </c>
-      <c r="C21" s="33"/>
-      <c r="D21" s="33"/>
+      <c r="C21" s="45"/>
+      <c r="D21" s="45"/>
     </row>
     <row r="22" spans="2:4">
-      <c r="B22" s="33" t="s">
+      <c r="B22" s="45" t="s">
         <v>62</v>
       </c>
-      <c r="C22" s="33"/>
-      <c r="D22" s="33"/>
+      <c r="C22" s="45"/>
+      <c r="D22" s="45"/>
     </row>
   </sheetData>
   <mergeCells count="15">

</xml_diff>

<commit_message>
Actualizacion de Reportes Anexo 7 con todas las observaciones y impresion de las 4 hojas en un excel
</commit_message>
<xml_diff>
--- a/Unna.OperationalReport.WebSite/wwwroot/plantillas/reporte/mensual/BoletadeValorizacionPetroperu.xlsx
+++ b/Unna.OperationalReport.WebSite/wwwroot/plantillas/reporte/mensual/BoletadeValorizacionPetroperu.xlsx
@@ -8,16 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desarrollos\SP\APSS SP\ProyectoPrincipalAenza6\UnnaReportesOperativos\Unna.OperationalReport.WebSite\wwwroot\plantillas\reporte\mensual\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{420807EA-80B2-4D1C-BB1B-9D151D126C1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6203B72-BC8D-4237-A174-BF1CD37AEFB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="759" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
+    <sheet name="ANEXO 7- VALORIZACIÓN MENS." sheetId="1" r:id="rId1"/>
+    <sheet name="ANEXO 7- VALORIZACIÓN LOTE I" sheetId="2" r:id="rId2"/>
+    <sheet name="ANEXO 7- VALORIZACIÓN LOTE  VI" sheetId="3" r:id="rId3"/>
+    <sheet name="ANEXO 7- VALORIZACIÓN LOTE Z-69" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="Composicion_Items">Hoja1!$B$7:$AL$8</definedName>
+    <definedName name="Composicion_Items">'ANEXO 7- VALORIZACIÓN MENS.'!$B$7:$AL$8</definedName>
+    <definedName name="ComposicionLI_Items">'ANEXO 7- VALORIZACIÓN LOTE I'!$B$7:$U$8</definedName>
+    <definedName name="ComposicionLVI_Items">'ANEXO 7- VALORIZACIÓN LOTE  VI'!$B$7:$U$8</definedName>
+    <definedName name="ComposicionLZ69_Items">'ANEXO 7- VALORIZACIÓN LOTE Z-69'!$B$7:$U$8</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -29,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="121">
   <si>
     <t>Energía
 (MMBTU)</t>
@@ -400,6 +405,36 @@
   </si>
   <si>
     <t>{{Observacion4}}</t>
+  </si>
+  <si>
+    <t>{{TotalValorLiquidosUS_LVI}}</t>
+  </si>
+  <si>
+    <t>{{TotalCostoMaquilaUS_LVI}}</t>
+  </si>
+  <si>
+    <t>{{TotalGasSecoMS9215EnergiaMMBTU_LVI}}</t>
+  </si>
+  <si>
+    <t>{{TotalMontoFacturarporUnnaE_LVI}}</t>
+  </si>
+  <si>
+    <t>{{TotalMontoFacturarporPetroperu_LVI}}</t>
+  </si>
+  <si>
+    <t>{{TotalCostoMaquilaUS_LZ69}}</t>
+  </si>
+  <si>
+    <t>{{TotalValorLiquidosUS_LZ69}}</t>
+  </si>
+  <si>
+    <t>{{TotalGasSecoMS9215EnergiaMMBTU_LZ69}}</t>
+  </si>
+  <si>
+    <t>{{TotalMontoFacturarporUnnaE_LZ69}}</t>
+  </si>
+  <si>
+    <t>{{TotalMontoFacturarporPetroperu_LZ69}}</t>
   </si>
 </sst>
 </file>
@@ -981,6 +1016,12 @@
     <xf numFmtId="2" fontId="9" fillId="0" borderId="1" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -990,6 +1031,45 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="2" xfId="103" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="3" xfId="103" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="11" xfId="103" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="12" xfId="103" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="8" xfId="103" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="13" xfId="103" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" xfId="103" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="6" xfId="103" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="15" xfId="103" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="16" xfId="103" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="17" xfId="103" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1020,45 +1100,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="2" xfId="103" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="3" xfId="103" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="11" xfId="103" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="12" xfId="103" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="8" xfId="103" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="13" xfId="103" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" xfId="103" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="6" xfId="103" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="15" xfId="103" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="16" xfId="103" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="17" xfId="103" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1067,12 +1108,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="104">
@@ -1319,13 +1354,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>1150620</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>76201</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1604010</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>97340</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1406,6 +1441,234 @@
         <a:xfrm>
           <a:off x="106680" y="22860"/>
           <a:ext cx="853440" cy="499787"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1150620</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>76201</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1588770</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>97340</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Imagen 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E6C2696E-0F97-4CD2-BBD5-885C5A642452}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2110740" y="8168641"/>
+          <a:ext cx="1672590" cy="935539"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>15240</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>861060</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>156887</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Imagen 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A027747B-E828-4F29-A1E7-9D7699AB72FA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="-102" t="2426" r="242" b="540"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="106680" y="22860"/>
+          <a:ext cx="853440" cy="499787"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1150620</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>76201</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1573530</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>97340</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B90BA493-F415-47BE-892A-6D3693FAD3A4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2110740" y="8168641"/>
+          <a:ext cx="1657350" cy="935539"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>15240</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>853440</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>141647</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9A141C48-5B59-42D6-99EC-71450C9DA429}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="-102" t="2426" r="242" b="540"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="106680" y="22860"/>
+          <a:ext cx="845820" cy="667427"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1692,9 +1955,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:AL31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B31" sqref="B31:O31"/>
+      <selection pane="bottomLeft" activeCell="B22" sqref="B22:O27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
@@ -1713,86 +1976,86 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:38" ht="27" customHeight="1">
-      <c r="C1" s="43" t="s">
+      <c r="C1" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-      <c r="I1" s="43"/>
-      <c r="J1" s="43"/>
-      <c r="K1" s="43"/>
-      <c r="L1" s="43"/>
-      <c r="M1" s="43"/>
-      <c r="N1" s="43"/>
-      <c r="O1" s="43"/>
-      <c r="P1" s="43"/>
-      <c r="Q1" s="43"/>
-      <c r="R1" s="43"/>
-      <c r="S1" s="43"/>
-      <c r="T1" s="43"/>
-      <c r="U1" s="43"/>
-      <c r="V1" s="43"/>
-      <c r="W1" s="43"/>
-      <c r="X1" s="43"/>
-      <c r="Y1" s="43"/>
-      <c r="Z1" s="43"/>
-      <c r="AA1" s="43"/>
-      <c r="AB1" s="43"/>
-      <c r="AC1" s="43"/>
-      <c r="AD1" s="43"/>
-      <c r="AE1" s="43"/>
-      <c r="AF1" s="43"/>
-      <c r="AG1" s="43"/>
-      <c r="AH1" s="43"/>
-      <c r="AI1" s="43"/>
-      <c r="AJ1" s="43"/>
-      <c r="AK1" s="40" t="s">
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+      <c r="G1" s="58"/>
+      <c r="H1" s="58"/>
+      <c r="I1" s="58"/>
+      <c r="J1" s="58"/>
+      <c r="K1" s="58"/>
+      <c r="L1" s="58"/>
+      <c r="M1" s="58"/>
+      <c r="N1" s="58"/>
+      <c r="O1" s="58"/>
+      <c r="P1" s="58"/>
+      <c r="Q1" s="58"/>
+      <c r="R1" s="58"/>
+      <c r="S1" s="58"/>
+      <c r="T1" s="58"/>
+      <c r="U1" s="58"/>
+      <c r="V1" s="58"/>
+      <c r="W1" s="58"/>
+      <c r="X1" s="58"/>
+      <c r="Y1" s="58"/>
+      <c r="Z1" s="58"/>
+      <c r="AA1" s="58"/>
+      <c r="AB1" s="58"/>
+      <c r="AC1" s="58"/>
+      <c r="AD1" s="58"/>
+      <c r="AE1" s="58"/>
+      <c r="AF1" s="58"/>
+      <c r="AG1" s="58"/>
+      <c r="AH1" s="58"/>
+      <c r="AI1" s="58"/>
+      <c r="AJ1" s="58"/>
+      <c r="AK1" s="55" t="s">
         <v>63</v>
       </c>
-      <c r="AL1" s="41"/>
+      <c r="AL1" s="56"/>
     </row>
     <row r="2" spans="2:38" ht="15" thickBot="1">
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
-      <c r="K2" s="43"/>
-      <c r="L2" s="43"/>
-      <c r="M2" s="43"/>
-      <c r="N2" s="43"/>
-      <c r="O2" s="43"/>
-      <c r="P2" s="43"/>
-      <c r="Q2" s="43"/>
-      <c r="R2" s="43"/>
-      <c r="S2" s="43"/>
-      <c r="T2" s="43"/>
-      <c r="U2" s="43"/>
-      <c r="V2" s="43"/>
-      <c r="W2" s="43"/>
-      <c r="X2" s="43"/>
-      <c r="Y2" s="43"/>
-      <c r="Z2" s="43"/>
-      <c r="AA2" s="43"/>
-      <c r="AB2" s="43"/>
-      <c r="AC2" s="43"/>
-      <c r="AD2" s="43"/>
-      <c r="AE2" s="43"/>
-      <c r="AF2" s="43"/>
-      <c r="AG2" s="43"/>
-      <c r="AH2" s="43"/>
-      <c r="AI2" s="43"/>
-      <c r="AJ2" s="43"/>
-      <c r="AK2" s="42" t="s">
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="58"/>
+      <c r="F2" s="58"/>
+      <c r="G2" s="58"/>
+      <c r="H2" s="58"/>
+      <c r="I2" s="58"/>
+      <c r="J2" s="58"/>
+      <c r="K2" s="58"/>
+      <c r="L2" s="58"/>
+      <c r="M2" s="58"/>
+      <c r="N2" s="58"/>
+      <c r="O2" s="58"/>
+      <c r="P2" s="58"/>
+      <c r="Q2" s="58"/>
+      <c r="R2" s="58"/>
+      <c r="S2" s="58"/>
+      <c r="T2" s="58"/>
+      <c r="U2" s="58"/>
+      <c r="V2" s="58"/>
+      <c r="W2" s="58"/>
+      <c r="X2" s="58"/>
+      <c r="Y2" s="58"/>
+      <c r="Z2" s="58"/>
+      <c r="AA2" s="58"/>
+      <c r="AB2" s="58"/>
+      <c r="AC2" s="58"/>
+      <c r="AD2" s="58"/>
+      <c r="AE2" s="58"/>
+      <c r="AF2" s="58"/>
+      <c r="AG2" s="58"/>
+      <c r="AH2" s="58"/>
+      <c r="AI2" s="58"/>
+      <c r="AJ2" s="58"/>
+      <c r="AK2" s="57" t="s">
         <v>64</v>
       </c>
-      <c r="AL2" s="42"/>
+      <c r="AL2" s="57"/>
     </row>
     <row r="3" spans="2:38" ht="15" thickBot="1">
       <c r="C3" s="27" t="s">
@@ -1837,80 +2100,80 @@
       <c r="AL3" s="24"/>
     </row>
     <row r="4" spans="2:38" ht="29.4" customHeight="1" thickBot="1">
-      <c r="C4" s="32" t="s">
+      <c r="C4" s="34" t="s">
         <v>105</v>
       </c>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="33"/>
-      <c r="J4" s="33"/>
-      <c r="K4" s="33"/>
-      <c r="L4" s="33"/>
-      <c r="M4" s="33"/>
-      <c r="N4" s="33"/>
-      <c r="O4" s="33"/>
-      <c r="P4" s="33"/>
-      <c r="Q4" s="33"/>
-      <c r="R4" s="33"/>
-      <c r="S4" s="33"/>
-      <c r="T4" s="33"/>
-      <c r="U4" s="34"/>
-      <c r="V4" s="36" t="s">
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="35"/>
+      <c r="H4" s="35"/>
+      <c r="I4" s="35"/>
+      <c r="J4" s="35"/>
+      <c r="K4" s="35"/>
+      <c r="L4" s="35"/>
+      <c r="M4" s="35"/>
+      <c r="N4" s="35"/>
+      <c r="O4" s="35"/>
+      <c r="P4" s="35"/>
+      <c r="Q4" s="35"/>
+      <c r="R4" s="35"/>
+      <c r="S4" s="35"/>
+      <c r="T4" s="35"/>
+      <c r="U4" s="36"/>
+      <c r="V4" s="51" t="s">
         <v>68</v>
       </c>
-      <c r="W4" s="36" t="s">
+      <c r="W4" s="51" t="s">
         <v>69</v>
       </c>
-      <c r="X4" s="32" t="s">
+      <c r="X4" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="Y4" s="33"/>
-      <c r="Z4" s="33"/>
-      <c r="AA4" s="33"/>
-      <c r="AB4" s="33"/>
-      <c r="AC4" s="34"/>
+      <c r="Y4" s="35"/>
+      <c r="Z4" s="35"/>
+      <c r="AA4" s="35"/>
+      <c r="AB4" s="35"/>
+      <c r="AC4" s="36"/>
     </row>
     <row r="5" spans="2:38" ht="15" thickBot="1">
-      <c r="C5" s="32" t="s">
+      <c r="C5" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="33"/>
-      <c r="E5" s="33"/>
-      <c r="F5" s="33"/>
-      <c r="G5" s="33"/>
-      <c r="H5" s="34"/>
-      <c r="I5" s="32" t="s">
+      <c r="D5" s="35"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="35"/>
+      <c r="G5" s="35"/>
+      <c r="H5" s="36"/>
+      <c r="I5" s="34" t="s">
         <v>65</v>
       </c>
-      <c r="J5" s="33"/>
-      <c r="K5" s="33"/>
-      <c r="L5" s="33"/>
-      <c r="M5" s="33"/>
-      <c r="N5" s="34"/>
-      <c r="O5" s="32" t="s">
+      <c r="J5" s="35"/>
+      <c r="K5" s="35"/>
+      <c r="L5" s="35"/>
+      <c r="M5" s="35"/>
+      <c r="N5" s="36"/>
+      <c r="O5" s="34" t="s">
         <v>66</v>
       </c>
-      <c r="P5" s="33"/>
-      <c r="Q5" s="33"/>
-      <c r="R5" s="33"/>
-      <c r="S5" s="33"/>
-      <c r="T5" s="33"/>
-      <c r="U5" s="36" t="s">
+      <c r="P5" s="35"/>
+      <c r="Q5" s="35"/>
+      <c r="R5" s="35"/>
+      <c r="S5" s="35"/>
+      <c r="T5" s="35"/>
+      <c r="U5" s="51" t="s">
         <v>67</v>
       </c>
-      <c r="V5" s="38"/>
-      <c r="W5" s="38"/>
-      <c r="X5" s="32" t="s">
+      <c r="V5" s="53"/>
+      <c r="W5" s="53"/>
+      <c r="X5" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="Y5" s="33"/>
-      <c r="Z5" s="33"/>
-      <c r="AA5" s="33"/>
-      <c r="AB5" s="33"/>
-      <c r="AC5" s="34"/>
+      <c r="Y5" s="35"/>
+      <c r="Z5" s="35"/>
+      <c r="AA5" s="35"/>
+      <c r="AB5" s="35"/>
+      <c r="AC5" s="36"/>
     </row>
     <row r="6" spans="2:38" ht="58.2" thickBot="1">
       <c r="B6" s="4"/>
@@ -1968,9 +2231,9 @@
       <c r="T6" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="U6" s="37"/>
-      <c r="V6" s="39"/>
-      <c r="W6" s="39"/>
+      <c r="U6" s="52"/>
+      <c r="V6" s="54"/>
+      <c r="W6" s="54"/>
       <c r="X6" s="14" t="s">
         <v>8</v>
       </c>
@@ -2228,18 +2491,18 @@
       <c r="E11" s="9"/>
     </row>
     <row r="12" spans="2:38" ht="24.6" customHeight="1">
-      <c r="B12" s="35" t="s">
+      <c r="B12" s="50" t="s">
         <v>107</v>
       </c>
-      <c r="C12" s="35"/>
+      <c r="C12" s="50"/>
       <c r="D12" s="9"/>
       <c r="E12" s="9"/>
     </row>
     <row r="13" spans="2:38" ht="27.6" customHeight="1" thickBot="1">
-      <c r="B13" s="57" t="s">
+      <c r="B13" s="48" t="s">
         <v>108</v>
       </c>
-      <c r="C13" s="57"/>
+      <c r="C13" s="48"/>
       <c r="D13" s="29"/>
       <c r="E13" s="30"/>
       <c r="F13" s="6"/>
@@ -2262,11 +2525,11 @@
       <c r="W13" s="6"/>
     </row>
     <row r="14" spans="2:38" ht="16.8" customHeight="1" thickBot="1">
-      <c r="B14" s="54" t="s">
+      <c r="B14" s="45" t="s">
         <v>54</v>
       </c>
-      <c r="C14" s="55"/>
-      <c r="D14" s="56"/>
+      <c r="C14" s="46"/>
+      <c r="D14" s="47"/>
       <c r="E14" s="22" t="s">
         <v>53</v>
       </c>
@@ -2291,8 +2554,8 @@
     </row>
     <row r="15" spans="2:38" ht="15" thickBot="1">
       <c r="B15" s="3"/>
-      <c r="C15" s="52"/>
-      <c r="D15" s="53"/>
+      <c r="C15" s="43"/>
+      <c r="D15" s="44"/>
     </row>
     <row r="16" spans="2:38" ht="29.4" thickBot="1">
       <c r="B16" s="3"/>
@@ -2303,21 +2566,21 @@
       </c>
     </row>
     <row r="17" spans="2:15" ht="39.6" customHeight="1" thickBot="1">
-      <c r="B17" s="46" t="s">
+      <c r="B17" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="C17" s="47"/>
-      <c r="D17" s="48"/>
+      <c r="C17" s="38"/>
+      <c r="D17" s="39"/>
       <c r="E17" s="31" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="18" spans="2:15" ht="43.8" customHeight="1" thickBot="1">
-      <c r="B18" s="49" t="s">
+      <c r="B18" s="40" t="s">
         <v>59</v>
       </c>
-      <c r="C18" s="50"/>
-      <c r="D18" s="51"/>
+      <c r="C18" s="41"/>
+      <c r="D18" s="42"/>
       <c r="E18" s="31" t="s">
         <v>57</v>
       </c>
@@ -2338,102 +2601,102 @@
       </c>
     </row>
     <row r="22" spans="2:15">
-      <c r="B22" s="61" t="s">
+      <c r="B22" s="49" t="s">
         <v>60</v>
       </c>
-      <c r="C22" s="61"/>
-      <c r="D22" s="61"/>
-      <c r="E22" s="61"/>
-      <c r="F22" s="61"/>
-      <c r="G22" s="61"/>
-      <c r="H22" s="61"/>
-      <c r="I22" s="61"/>
-      <c r="J22" s="61"/>
-      <c r="K22" s="61"/>
-      <c r="L22" s="61"/>
-      <c r="M22" s="61"/>
-      <c r="N22" s="61"/>
-      <c r="O22" s="61"/>
+      <c r="C22" s="49"/>
+      <c r="D22" s="49"/>
+      <c r="E22" s="49"/>
+      <c r="F22" s="49"/>
+      <c r="G22" s="49"/>
+      <c r="H22" s="49"/>
+      <c r="I22" s="49"/>
+      <c r="J22" s="49"/>
+      <c r="K22" s="49"/>
+      <c r="L22" s="49"/>
+      <c r="M22" s="49"/>
+      <c r="N22" s="49"/>
+      <c r="O22" s="49"/>
     </row>
     <row r="23" spans="2:15">
-      <c r="B23" s="61"/>
-      <c r="C23" s="61"/>
-      <c r="D23" s="61"/>
-      <c r="E23" s="61"/>
-      <c r="F23" s="61"/>
-      <c r="G23" s="61"/>
-      <c r="H23" s="61"/>
-      <c r="I23" s="61"/>
-      <c r="J23" s="61"/>
-      <c r="K23" s="61"/>
-      <c r="L23" s="61"/>
-      <c r="M23" s="61"/>
-      <c r="N23" s="61"/>
-      <c r="O23" s="61"/>
+      <c r="B23" s="49"/>
+      <c r="C23" s="49"/>
+      <c r="D23" s="49"/>
+      <c r="E23" s="49"/>
+      <c r="F23" s="49"/>
+      <c r="G23" s="49"/>
+      <c r="H23" s="49"/>
+      <c r="I23" s="49"/>
+      <c r="J23" s="49"/>
+      <c r="K23" s="49"/>
+      <c r="L23" s="49"/>
+      <c r="M23" s="49"/>
+      <c r="N23" s="49"/>
+      <c r="O23" s="49"/>
     </row>
     <row r="24" spans="2:15">
-      <c r="B24" s="61"/>
-      <c r="C24" s="61"/>
-      <c r="D24" s="61"/>
-      <c r="E24" s="61"/>
-      <c r="F24" s="61"/>
-      <c r="G24" s="61"/>
-      <c r="H24" s="61"/>
-      <c r="I24" s="61"/>
-      <c r="J24" s="61"/>
-      <c r="K24" s="61"/>
-      <c r="L24" s="61"/>
-      <c r="M24" s="61"/>
-      <c r="N24" s="61"/>
-      <c r="O24" s="61"/>
+      <c r="B24" s="49"/>
+      <c r="C24" s="49"/>
+      <c r="D24" s="49"/>
+      <c r="E24" s="49"/>
+      <c r="F24" s="49"/>
+      <c r="G24" s="49"/>
+      <c r="H24" s="49"/>
+      <c r="I24" s="49"/>
+      <c r="J24" s="49"/>
+      <c r="K24" s="49"/>
+      <c r="L24" s="49"/>
+      <c r="M24" s="49"/>
+      <c r="N24" s="49"/>
+      <c r="O24" s="49"/>
     </row>
     <row r="25" spans="2:15">
-      <c r="B25" s="61"/>
-      <c r="C25" s="61"/>
-      <c r="D25" s="61"/>
-      <c r="E25" s="61"/>
-      <c r="F25" s="61"/>
-      <c r="G25" s="61"/>
-      <c r="H25" s="61"/>
-      <c r="I25" s="61"/>
-      <c r="J25" s="61"/>
-      <c r="K25" s="61"/>
-      <c r="L25" s="61"/>
-      <c r="M25" s="61"/>
-      <c r="N25" s="61"/>
-      <c r="O25" s="61"/>
+      <c r="B25" s="49"/>
+      <c r="C25" s="49"/>
+      <c r="D25" s="49"/>
+      <c r="E25" s="49"/>
+      <c r="F25" s="49"/>
+      <c r="G25" s="49"/>
+      <c r="H25" s="49"/>
+      <c r="I25" s="49"/>
+      <c r="J25" s="49"/>
+      <c r="K25" s="49"/>
+      <c r="L25" s="49"/>
+      <c r="M25" s="49"/>
+      <c r="N25" s="49"/>
+      <c r="O25" s="49"/>
     </row>
     <row r="26" spans="2:15">
-      <c r="B26" s="61"/>
-      <c r="C26" s="61"/>
-      <c r="D26" s="61"/>
-      <c r="E26" s="61"/>
-      <c r="F26" s="61"/>
-      <c r="G26" s="61"/>
-      <c r="H26" s="61"/>
-      <c r="I26" s="61"/>
-      <c r="J26" s="61"/>
-      <c r="K26" s="61"/>
-      <c r="L26" s="61"/>
-      <c r="M26" s="61"/>
-      <c r="N26" s="61"/>
-      <c r="O26" s="61"/>
+      <c r="B26" s="49"/>
+      <c r="C26" s="49"/>
+      <c r="D26" s="49"/>
+      <c r="E26" s="49"/>
+      <c r="F26" s="49"/>
+      <c r="G26" s="49"/>
+      <c r="H26" s="49"/>
+      <c r="I26" s="49"/>
+      <c r="J26" s="49"/>
+      <c r="K26" s="49"/>
+      <c r="L26" s="49"/>
+      <c r="M26" s="49"/>
+      <c r="N26" s="49"/>
+      <c r="O26" s="49"/>
     </row>
     <row r="27" spans="2:15">
-      <c r="B27" s="61"/>
-      <c r="C27" s="61"/>
-      <c r="D27" s="61"/>
-      <c r="E27" s="61"/>
-      <c r="F27" s="61"/>
-      <c r="G27" s="61"/>
-      <c r="H27" s="61"/>
-      <c r="I27" s="61"/>
-      <c r="J27" s="61"/>
-      <c r="K27" s="61"/>
-      <c r="L27" s="61"/>
-      <c r="M27" s="61"/>
-      <c r="N27" s="61"/>
-      <c r="O27" s="61"/>
+      <c r="B27" s="49"/>
+      <c r="C27" s="49"/>
+      <c r="D27" s="49"/>
+      <c r="E27" s="49"/>
+      <c r="F27" s="49"/>
+      <c r="G27" s="49"/>
+      <c r="H27" s="49"/>
+      <c r="I27" s="49"/>
+      <c r="J27" s="49"/>
+      <c r="K27" s="49"/>
+      <c r="L27" s="49"/>
+      <c r="M27" s="49"/>
+      <c r="N27" s="49"/>
+      <c r="O27" s="49"/>
     </row>
     <row r="28" spans="2:15">
       <c r="B28" s="24"/>
@@ -2452,61 +2715,71 @@
       <c r="O28" s="24"/>
     </row>
     <row r="29" spans="2:15">
-      <c r="B29" s="62" t="s">
+      <c r="B29" s="33" t="s">
         <v>61</v>
       </c>
-      <c r="C29" s="62"/>
-      <c r="D29" s="62"/>
-      <c r="E29" s="62"/>
-      <c r="F29" s="62"/>
-      <c r="G29" s="62"/>
-      <c r="H29" s="62"/>
-      <c r="I29" s="62"/>
-      <c r="J29" s="62"/>
-      <c r="K29" s="62"/>
-      <c r="L29" s="62"/>
-      <c r="M29" s="62"/>
-      <c r="N29" s="62"/>
-      <c r="O29" s="62"/>
+      <c r="C29" s="33"/>
+      <c r="D29" s="33"/>
+      <c r="E29" s="33"/>
+      <c r="F29" s="33"/>
+      <c r="G29" s="33"/>
+      <c r="H29" s="33"/>
+      <c r="I29" s="33"/>
+      <c r="J29" s="33"/>
+      <c r="K29" s="33"/>
+      <c r="L29" s="33"/>
+      <c r="M29" s="33"/>
+      <c r="N29" s="33"/>
+      <c r="O29" s="33"/>
     </row>
     <row r="30" spans="2:15">
-      <c r="B30" s="62" t="s">
+      <c r="B30" s="33" t="s">
         <v>62</v>
       </c>
-      <c r="C30" s="62"/>
-      <c r="D30" s="62"/>
-      <c r="E30" s="62"/>
-      <c r="F30" s="62"/>
-      <c r="G30" s="62"/>
-      <c r="H30" s="62"/>
-      <c r="I30" s="62"/>
-      <c r="J30" s="62"/>
-      <c r="K30" s="62"/>
-      <c r="L30" s="62"/>
-      <c r="M30" s="62"/>
-      <c r="N30" s="62"/>
-      <c r="O30" s="62"/>
+      <c r="C30" s="33"/>
+      <c r="D30" s="33"/>
+      <c r="E30" s="33"/>
+      <c r="F30" s="33"/>
+      <c r="G30" s="33"/>
+      <c r="H30" s="33"/>
+      <c r="I30" s="33"/>
+      <c r="J30" s="33"/>
+      <c r="K30" s="33"/>
+      <c r="L30" s="33"/>
+      <c r="M30" s="33"/>
+      <c r="N30" s="33"/>
+      <c r="O30" s="33"/>
     </row>
     <row r="31" spans="2:15">
-      <c r="B31" s="62" t="s">
+      <c r="B31" s="33" t="s">
         <v>110</v>
       </c>
-      <c r="C31" s="62"/>
-      <c r="D31" s="62"/>
-      <c r="E31" s="62"/>
-      <c r="F31" s="62"/>
-      <c r="G31" s="62"/>
-      <c r="H31" s="62"/>
-      <c r="I31" s="62"/>
-      <c r="J31" s="62"/>
-      <c r="K31" s="62"/>
-      <c r="L31" s="62"/>
-      <c r="M31" s="62"/>
-      <c r="N31" s="62"/>
-      <c r="O31" s="62"/>
+      <c r="C31" s="33"/>
+      <c r="D31" s="33"/>
+      <c r="E31" s="33"/>
+      <c r="F31" s="33"/>
+      <c r="G31" s="33"/>
+      <c r="H31" s="33"/>
+      <c r="I31" s="33"/>
+      <c r="J31" s="33"/>
+      <c r="K31" s="33"/>
+      <c r="L31" s="33"/>
+      <c r="M31" s="33"/>
+      <c r="N31" s="33"/>
+      <c r="O31" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="C4:U4"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="U5:U6"/>
+    <mergeCell ref="W4:W6"/>
+    <mergeCell ref="AK1:AL1"/>
+    <mergeCell ref="AK2:AL2"/>
+    <mergeCell ref="C1:AJ2"/>
+    <mergeCell ref="X5:AC5"/>
+    <mergeCell ref="X4:AC4"/>
+    <mergeCell ref="V4:V6"/>
     <mergeCell ref="B29:O29"/>
     <mergeCell ref="B30:O30"/>
     <mergeCell ref="B31:O31"/>
@@ -2519,16 +2792,6 @@
     <mergeCell ref="B14:D14"/>
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="B22:O27"/>
-    <mergeCell ref="C4:U4"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="U5:U6"/>
-    <mergeCell ref="W4:W6"/>
-    <mergeCell ref="AK1:AL1"/>
-    <mergeCell ref="AK2:AL2"/>
-    <mergeCell ref="C1:AJ2"/>
-    <mergeCell ref="X5:AC5"/>
-    <mergeCell ref="X4:AC4"/>
-    <mergeCell ref="V4:V6"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" horizontalDpi="300" r:id="rId1"/>
@@ -2538,10 +2801,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15F5674C-6194-49DE-8C68-201941F0F769}">
-  <dimension ref="B1:U22"/>
+  <dimension ref="B1:U28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20:O25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
@@ -2559,52 +2822,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:21" ht="27" customHeight="1">
-      <c r="C1" s="43" t="s">
+      <c r="C1" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-      <c r="I1" s="43"/>
-      <c r="J1" s="43"/>
-      <c r="K1" s="43"/>
-      <c r="L1" s="43"/>
-      <c r="M1" s="43"/>
-      <c r="N1" s="43"/>
-      <c r="O1" s="43"/>
-      <c r="P1" s="43"/>
-      <c r="Q1" s="43"/>
-      <c r="R1" s="43"/>
-      <c r="S1" s="43"/>
-      <c r="T1" s="40" t="s">
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+      <c r="G1" s="58"/>
+      <c r="H1" s="58"/>
+      <c r="I1" s="58"/>
+      <c r="J1" s="58"/>
+      <c r="K1" s="58"/>
+      <c r="L1" s="58"/>
+      <c r="M1" s="58"/>
+      <c r="N1" s="58"/>
+      <c r="O1" s="58"/>
+      <c r="P1" s="58"/>
+      <c r="Q1" s="58"/>
+      <c r="R1" s="58"/>
+      <c r="S1" s="58"/>
+      <c r="T1" s="55" t="s">
         <v>63</v>
       </c>
-      <c r="U1" s="41"/>
+      <c r="U1" s="56"/>
     </row>
     <row r="2" spans="2:21" ht="15" thickBot="1">
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
-      <c r="K2" s="43"/>
-      <c r="L2" s="43"/>
-      <c r="M2" s="43"/>
-      <c r="N2" s="43"/>
-      <c r="O2" s="43"/>
-      <c r="P2" s="43"/>
-      <c r="Q2" s="43"/>
-      <c r="R2" s="43"/>
-      <c r="S2" s="43"/>
-      <c r="T2" s="42" t="s">
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="58"/>
+      <c r="F2" s="58"/>
+      <c r="G2" s="58"/>
+      <c r="H2" s="58"/>
+      <c r="I2" s="58"/>
+      <c r="J2" s="58"/>
+      <c r="K2" s="58"/>
+      <c r="L2" s="58"/>
+      <c r="M2" s="58"/>
+      <c r="N2" s="58"/>
+      <c r="O2" s="58"/>
+      <c r="P2" s="58"/>
+      <c r="Q2" s="58"/>
+      <c r="R2" s="58"/>
+      <c r="S2" s="58"/>
+      <c r="T2" s="57" t="s">
         <v>64</v>
       </c>
-      <c r="U2" s="42"/>
+      <c r="U2" s="57"/>
     </row>
     <row r="3" spans="2:21" ht="15" thickBot="1">
       <c r="C3" s="28" t="s">
@@ -2632,38 +2895,38 @@
       <c r="U3" s="24"/>
     </row>
     <row r="4" spans="2:21" ht="29.4" customHeight="1" thickBot="1">
-      <c r="C4" s="32" t="s">
+      <c r="C4" s="34" t="s">
         <v>105</v>
       </c>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="34"/>
-      <c r="I4" s="36" t="s">
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="35"/>
+      <c r="H4" s="36"/>
+      <c r="I4" s="51" t="s">
         <v>68</v>
       </c>
-      <c r="J4" s="58" t="s">
+      <c r="J4" s="60" t="s">
         <v>12</v>
       </c>
-      <c r="K4" s="59"/>
-      <c r="L4" s="60"/>
+      <c r="K4" s="61"/>
+      <c r="L4" s="62"/>
     </row>
     <row r="5" spans="2:21" ht="15" thickBot="1">
-      <c r="C5" s="32" t="s">
+      <c r="C5" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="33"/>
-      <c r="E5" s="33"/>
-      <c r="F5" s="33"/>
-      <c r="G5" s="33"/>
-      <c r="H5" s="34"/>
-      <c r="I5" s="38"/>
-      <c r="J5" s="32" t="s">
+      <c r="D5" s="35"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="35"/>
+      <c r="G5" s="35"/>
+      <c r="H5" s="36"/>
+      <c r="I5" s="53"/>
+      <c r="J5" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="K5" s="33"/>
-      <c r="L5" s="34"/>
+      <c r="K5" s="35"/>
+      <c r="L5" s="36"/>
     </row>
     <row r="6" spans="2:21" ht="58.2" thickBot="1">
       <c r="B6" s="4"/>
@@ -2685,7 +2948,7 @@
       <c r="H6" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="I6" s="39"/>
+      <c r="I6" s="54"/>
       <c r="J6" s="14" t="s">
         <v>8</v>
       </c>
@@ -2848,11 +3111,11 @@
       <c r="I11" s="6"/>
     </row>
     <row r="12" spans="2:21" ht="16.8" customHeight="1" thickBot="1">
-      <c r="B12" s="54" t="s">
+      <c r="B12" s="45" t="s">
         <v>54</v>
       </c>
-      <c r="C12" s="55"/>
-      <c r="D12" s="56"/>
+      <c r="C12" s="46"/>
+      <c r="D12" s="47"/>
       <c r="E12" s="22" t="s">
         <v>53</v>
       </c>
@@ -2863,8 +3126,8 @@
     </row>
     <row r="13" spans="2:21">
       <c r="B13" s="3"/>
-      <c r="C13" s="52"/>
-      <c r="D13" s="53"/>
+      <c r="C13" s="43"/>
+      <c r="D13" s="44"/>
     </row>
     <row r="14" spans="2:21" ht="15" thickBot="1">
       <c r="B14" s="1"/>
@@ -2873,71 +3136,191 @@
       <c r="E14" s="2"/>
     </row>
     <row r="15" spans="2:21" ht="39.6" customHeight="1" thickBot="1">
-      <c r="B15" s="46" t="s">
+      <c r="B15" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="C15" s="47"/>
-      <c r="D15" s="48"/>
+      <c r="C15" s="38"/>
+      <c r="D15" s="39"/>
       <c r="E15" s="18" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="16" spans="2:21" ht="43.8" customHeight="1" thickBot="1">
-      <c r="B16" s="49" t="s">
+      <c r="B16" s="40" t="s">
         <v>59</v>
       </c>
-      <c r="C16" s="50"/>
-      <c r="D16" s="51"/>
+      <c r="C16" s="41"/>
+      <c r="D16" s="42"/>
       <c r="E16" s="18" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="17" spans="2:4">
+    <row r="17" spans="2:15">
       <c r="B17" s="3"/>
       <c r="C17" s="17"/>
       <c r="D17" s="17"/>
     </row>
-    <row r="18" spans="2:4">
+    <row r="18" spans="2:15">
       <c r="B18" s="3"/>
       <c r="C18" s="17"/>
       <c r="D18" s="17"/>
     </row>
-    <row r="19" spans="2:4">
+    <row r="19" spans="2:15">
       <c r="B19" s="16" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="20" spans="2:4">
-      <c r="B20" s="45" t="s">
+    <row r="20" spans="2:15">
+      <c r="B20" s="49" t="s">
         <v>60</v>
       </c>
-      <c r="C20" s="45"/>
-      <c r="D20" s="45"/>
-    </row>
-    <row r="21" spans="2:4">
-      <c r="B21" s="45" t="s">
-        <v>61</v>
-      </c>
-      <c r="C21" s="45"/>
-      <c r="D21" s="45"/>
-    </row>
-    <row r="22" spans="2:4">
-      <c r="B22" s="45" t="s">
-        <v>62</v>
-      </c>
-      <c r="C22" s="45"/>
-      <c r="D22" s="45"/>
+      <c r="C20" s="49"/>
+      <c r="D20" s="49"/>
+      <c r="E20" s="49"/>
+      <c r="F20" s="49"/>
+      <c r="G20" s="49"/>
+      <c r="H20" s="49"/>
+      <c r="I20" s="49"/>
+      <c r="J20" s="49"/>
+      <c r="K20" s="49"/>
+      <c r="L20" s="49"/>
+      <c r="M20" s="49"/>
+      <c r="N20" s="49"/>
+      <c r="O20" s="49"/>
+    </row>
+    <row r="21" spans="2:15">
+      <c r="B21" s="49"/>
+      <c r="C21" s="49"/>
+      <c r="D21" s="49"/>
+      <c r="E21" s="49"/>
+      <c r="F21" s="49"/>
+      <c r="G21" s="49"/>
+      <c r="H21" s="49"/>
+      <c r="I21" s="49"/>
+      <c r="J21" s="49"/>
+      <c r="K21" s="49"/>
+      <c r="L21" s="49"/>
+      <c r="M21" s="49"/>
+      <c r="N21" s="49"/>
+      <c r="O21" s="49"/>
+    </row>
+    <row r="22" spans="2:15">
+      <c r="B22" s="49"/>
+      <c r="C22" s="49"/>
+      <c r="D22" s="49"/>
+      <c r="E22" s="49"/>
+      <c r="F22" s="49"/>
+      <c r="G22" s="49"/>
+      <c r="H22" s="49"/>
+      <c r="I22" s="49"/>
+      <c r="J22" s="49"/>
+      <c r="K22" s="49"/>
+      <c r="L22" s="49"/>
+      <c r="M22" s="49"/>
+      <c r="N22" s="49"/>
+      <c r="O22" s="49"/>
+    </row>
+    <row r="23" spans="2:15">
+      <c r="B23" s="49"/>
+      <c r="C23" s="49"/>
+      <c r="D23" s="49"/>
+      <c r="E23" s="49"/>
+      <c r="F23" s="49"/>
+      <c r="G23" s="49"/>
+      <c r="H23" s="49"/>
+      <c r="I23" s="49"/>
+      <c r="J23" s="49"/>
+      <c r="K23" s="49"/>
+      <c r="L23" s="49"/>
+      <c r="M23" s="49"/>
+      <c r="N23" s="49"/>
+      <c r="O23" s="49"/>
+    </row>
+    <row r="24" spans="2:15">
+      <c r="B24" s="49"/>
+      <c r="C24" s="49"/>
+      <c r="D24" s="49"/>
+      <c r="E24" s="49"/>
+      <c r="F24" s="49"/>
+      <c r="G24" s="49"/>
+      <c r="H24" s="49"/>
+      <c r="I24" s="49"/>
+      <c r="J24" s="49"/>
+      <c r="K24" s="49"/>
+      <c r="L24" s="49"/>
+      <c r="M24" s="49"/>
+      <c r="N24" s="49"/>
+      <c r="O24" s="49"/>
+    </row>
+    <row r="25" spans="2:15">
+      <c r="B25" s="49"/>
+      <c r="C25" s="49"/>
+      <c r="D25" s="49"/>
+      <c r="E25" s="49"/>
+      <c r="F25" s="49"/>
+      <c r="G25" s="49"/>
+      <c r="H25" s="49"/>
+      <c r="I25" s="49"/>
+      <c r="J25" s="49"/>
+      <c r="K25" s="49"/>
+      <c r="L25" s="49"/>
+      <c r="M25" s="49"/>
+      <c r="N25" s="49"/>
+      <c r="O25" s="49"/>
+    </row>
+    <row r="26" spans="2:15">
+      <c r="B26" s="32"/>
+      <c r="C26" s="32"/>
+      <c r="D26" s="32"/>
+      <c r="E26" s="32"/>
+      <c r="F26" s="32"/>
+      <c r="G26" s="32"/>
+      <c r="H26" s="32"/>
+      <c r="I26" s="32"/>
+      <c r="J26" s="32"/>
+      <c r="K26" s="32"/>
+      <c r="L26" s="32"/>
+      <c r="M26" s="32"/>
+      <c r="N26" s="32"/>
+      <c r="O26" s="32"/>
+    </row>
+    <row r="27" spans="2:15">
+      <c r="B27" s="33"/>
+      <c r="C27" s="33"/>
+      <c r="D27" s="33"/>
+      <c r="E27" s="33"/>
+      <c r="F27" s="33"/>
+      <c r="G27" s="33"/>
+      <c r="H27" s="33"/>
+      <c r="I27" s="33"/>
+      <c r="J27" s="33"/>
+      <c r="K27" s="33"/>
+      <c r="L27" s="33"/>
+      <c r="M27" s="33"/>
+      <c r="N27" s="33"/>
+      <c r="O27" s="33"/>
+    </row>
+    <row r="28" spans="2:15">
+      <c r="B28" s="33"/>
+      <c r="C28" s="33"/>
+      <c r="D28" s="33"/>
+      <c r="E28" s="33"/>
+      <c r="F28" s="33"/>
+      <c r="G28" s="33"/>
+      <c r="H28" s="33"/>
+      <c r="I28" s="33"/>
+      <c r="J28" s="33"/>
+      <c r="K28" s="33"/>
+      <c r="L28" s="33"/>
+      <c r="M28" s="33"/>
+      <c r="N28" s="33"/>
+      <c r="O28" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="J5:L5"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B20:O25"/>
+    <mergeCell ref="B27:O27"/>
+    <mergeCell ref="B28:O28"/>
     <mergeCell ref="C1:S2"/>
     <mergeCell ref="T1:U1"/>
     <mergeCell ref="T2:U2"/>
@@ -2945,6 +3328,1091 @@
     <mergeCell ref="J4:L4"/>
     <mergeCell ref="C5:H5"/>
     <mergeCell ref="C4:H4"/>
+    <mergeCell ref="J5:L5"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B16:D16"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91203543-4EED-4AE0-859B-F0BC4BB889AE}">
+  <dimension ref="B1:U28"/>
+  <sheetViews>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20:O25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="1.33203125" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" customWidth="1"/>
+    <col min="3" max="3" width="17.77734375" customWidth="1"/>
+    <col min="4" max="4" width="24.44140625" customWidth="1"/>
+    <col min="5" max="5" width="29" customWidth="1"/>
+    <col min="8" max="8" width="12.88671875" customWidth="1"/>
+    <col min="13" max="13" width="14.109375" customWidth="1"/>
+    <col min="14" max="14" width="13.109375" customWidth="1"/>
+    <col min="15" max="15" width="15.6640625" customWidth="1"/>
+    <col min="20" max="20" width="13.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:21" ht="27" customHeight="1">
+      <c r="C1" s="58" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+      <c r="G1" s="58"/>
+      <c r="H1" s="58"/>
+      <c r="I1" s="58"/>
+      <c r="J1" s="58"/>
+      <c r="K1" s="58"/>
+      <c r="L1" s="58"/>
+      <c r="M1" s="58"/>
+      <c r="N1" s="58"/>
+      <c r="O1" s="58"/>
+      <c r="P1" s="58"/>
+      <c r="Q1" s="58"/>
+      <c r="R1" s="58"/>
+      <c r="S1" s="58"/>
+      <c r="T1" s="55" t="s">
+        <v>63</v>
+      </c>
+      <c r="U1" s="56"/>
+    </row>
+    <row r="2" spans="2:21" ht="15" thickBot="1">
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="58"/>
+      <c r="F2" s="58"/>
+      <c r="G2" s="58"/>
+      <c r="H2" s="58"/>
+      <c r="I2" s="58"/>
+      <c r="J2" s="58"/>
+      <c r="K2" s="58"/>
+      <c r="L2" s="58"/>
+      <c r="M2" s="58"/>
+      <c r="N2" s="58"/>
+      <c r="O2" s="58"/>
+      <c r="P2" s="58"/>
+      <c r="Q2" s="58"/>
+      <c r="R2" s="58"/>
+      <c r="S2" s="58"/>
+      <c r="T2" s="57" t="s">
+        <v>64</v>
+      </c>
+      <c r="U2" s="57"/>
+    </row>
+    <row r="3" spans="2:21" ht="15" thickBot="1">
+      <c r="C3" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
+      <c r="K3" s="25"/>
+      <c r="L3" s="25"/>
+      <c r="M3" s="25"/>
+      <c r="N3" s="25"/>
+      <c r="O3" s="25"/>
+      <c r="P3" s="25"/>
+      <c r="Q3" s="25"/>
+      <c r="R3" s="25"/>
+      <c r="S3" s="25"/>
+      <c r="T3" s="24"/>
+      <c r="U3" s="24"/>
+    </row>
+    <row r="4" spans="2:21" ht="29.4" customHeight="1" thickBot="1">
+      <c r="C4" s="34" t="s">
+        <v>105</v>
+      </c>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="35"/>
+      <c r="H4" s="36"/>
+      <c r="I4" s="51" t="s">
+        <v>68</v>
+      </c>
+      <c r="J4" s="60" t="s">
+        <v>12</v>
+      </c>
+      <c r="K4" s="61"/>
+      <c r="L4" s="62"/>
+    </row>
+    <row r="5" spans="2:21" ht="15" thickBot="1">
+      <c r="C5" s="34" t="s">
+        <v>65</v>
+      </c>
+      <c r="D5" s="35"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="35"/>
+      <c r="G5" s="35"/>
+      <c r="H5" s="36"/>
+      <c r="I5" s="53"/>
+      <c r="J5" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="K5" s="35"/>
+      <c r="L5" s="36"/>
+    </row>
+    <row r="6" spans="2:21" ht="58.2" thickBot="1">
+      <c r="B6" s="4"/>
+      <c r="C6" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="G6" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="I6" s="54"/>
+      <c r="J6" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="K6" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="L6" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="M6" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="N6" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="O6" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="P6" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q6" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="R6" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="S6" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="T6" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="U6" s="14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="2:21" ht="15" thickBot="1">
+      <c r="B7" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="E7" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="F7" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="G7" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="H7" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="I7" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="J7" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="K7" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="L7" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="M7" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="N7" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="O7" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="P7" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q7" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="R7" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="S7" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="T7" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="U7" s="13" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="2:21" ht="15" thickBot="1">
+      <c r="B8" s="8"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+    </row>
+    <row r="9" spans="2:21" ht="15" thickBot="1">
+      <c r="C9" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="D9" s="12"/>
+      <c r="E9" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="I9" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="J9" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="K9" s="12"/>
+      <c r="L9" s="21" t="s">
+        <v>113</v>
+      </c>
+      <c r="M9" s="12"/>
+      <c r="N9" s="12"/>
+      <c r="O9" s="12"/>
+      <c r="P9" s="12"/>
+      <c r="Q9" s="12"/>
+      <c r="R9" s="12"/>
+      <c r="S9" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="T9" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="U9" s="12" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="10" spans="2:21">
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+    </row>
+    <row r="11" spans="2:21" ht="15" thickBot="1">
+      <c r="B11" s="1"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+    </row>
+    <row r="12" spans="2:21" ht="16.8" customHeight="1" thickBot="1">
+      <c r="B12" s="45" t="s">
+        <v>54</v>
+      </c>
+      <c r="C12" s="46"/>
+      <c r="D12" s="47"/>
+      <c r="E12" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+    </row>
+    <row r="13" spans="2:21">
+      <c r="B13" s="3"/>
+      <c r="C13" s="43"/>
+      <c r="D13" s="44"/>
+    </row>
+    <row r="14" spans="2:21" ht="15" thickBot="1">
+      <c r="B14" s="1"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="2"/>
+    </row>
+    <row r="15" spans="2:21" ht="39.6" customHeight="1" thickBot="1">
+      <c r="B15" s="37" t="s">
+        <v>58</v>
+      </c>
+      <c r="C15" s="38"/>
+      <c r="D15" s="39"/>
+      <c r="E15" s="18" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="16" spans="2:21" ht="43.8" customHeight="1" thickBot="1">
+      <c r="B16" s="40" t="s">
+        <v>59</v>
+      </c>
+      <c r="C16" s="41"/>
+      <c r="D16" s="42"/>
+      <c r="E16" s="18" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="17" spans="2:15">
+      <c r="B17" s="3"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
+    </row>
+    <row r="18" spans="2:15">
+      <c r="B18" s="3"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="17"/>
+    </row>
+    <row r="19" spans="2:15">
+      <c r="B19" s="16" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="20" spans="2:15">
+      <c r="B20" s="49" t="s">
+        <v>60</v>
+      </c>
+      <c r="C20" s="49"/>
+      <c r="D20" s="49"/>
+      <c r="E20" s="49"/>
+      <c r="F20" s="49"/>
+      <c r="G20" s="49"/>
+      <c r="H20" s="49"/>
+      <c r="I20" s="49"/>
+      <c r="J20" s="49"/>
+      <c r="K20" s="49"/>
+      <c r="L20" s="49"/>
+      <c r="M20" s="49"/>
+      <c r="N20" s="49"/>
+      <c r="O20" s="49"/>
+    </row>
+    <row r="21" spans="2:15">
+      <c r="B21" s="49"/>
+      <c r="C21" s="49"/>
+      <c r="D21" s="49"/>
+      <c r="E21" s="49"/>
+      <c r="F21" s="49"/>
+      <c r="G21" s="49"/>
+      <c r="H21" s="49"/>
+      <c r="I21" s="49"/>
+      <c r="J21" s="49"/>
+      <c r="K21" s="49"/>
+      <c r="L21" s="49"/>
+      <c r="M21" s="49"/>
+      <c r="N21" s="49"/>
+      <c r="O21" s="49"/>
+    </row>
+    <row r="22" spans="2:15">
+      <c r="B22" s="49"/>
+      <c r="C22" s="49"/>
+      <c r="D22" s="49"/>
+      <c r="E22" s="49"/>
+      <c r="F22" s="49"/>
+      <c r="G22" s="49"/>
+      <c r="H22" s="49"/>
+      <c r="I22" s="49"/>
+      <c r="J22" s="49"/>
+      <c r="K22" s="49"/>
+      <c r="L22" s="49"/>
+      <c r="M22" s="49"/>
+      <c r="N22" s="49"/>
+      <c r="O22" s="49"/>
+    </row>
+    <row r="23" spans="2:15">
+      <c r="B23" s="49"/>
+      <c r="C23" s="49"/>
+      <c r="D23" s="49"/>
+      <c r="E23" s="49"/>
+      <c r="F23" s="49"/>
+      <c r="G23" s="49"/>
+      <c r="H23" s="49"/>
+      <c r="I23" s="49"/>
+      <c r="J23" s="49"/>
+      <c r="K23" s="49"/>
+      <c r="L23" s="49"/>
+      <c r="M23" s="49"/>
+      <c r="N23" s="49"/>
+      <c r="O23" s="49"/>
+    </row>
+    <row r="24" spans="2:15">
+      <c r="B24" s="49"/>
+      <c r="C24" s="49"/>
+      <c r="D24" s="49"/>
+      <c r="E24" s="49"/>
+      <c r="F24" s="49"/>
+      <c r="G24" s="49"/>
+      <c r="H24" s="49"/>
+      <c r="I24" s="49"/>
+      <c r="J24" s="49"/>
+      <c r="K24" s="49"/>
+      <c r="L24" s="49"/>
+      <c r="M24" s="49"/>
+      <c r="N24" s="49"/>
+      <c r="O24" s="49"/>
+    </row>
+    <row r="25" spans="2:15">
+      <c r="B25" s="49"/>
+      <c r="C25" s="49"/>
+      <c r="D25" s="49"/>
+      <c r="E25" s="49"/>
+      <c r="F25" s="49"/>
+      <c r="G25" s="49"/>
+      <c r="H25" s="49"/>
+      <c r="I25" s="49"/>
+      <c r="J25" s="49"/>
+      <c r="K25" s="49"/>
+      <c r="L25" s="49"/>
+      <c r="M25" s="49"/>
+      <c r="N25" s="49"/>
+      <c r="O25" s="49"/>
+    </row>
+    <row r="26" spans="2:15">
+      <c r="B26" s="32"/>
+      <c r="C26" s="32"/>
+      <c r="D26" s="32"/>
+      <c r="E26" s="32"/>
+      <c r="F26" s="32"/>
+      <c r="G26" s="32"/>
+      <c r="H26" s="32"/>
+      <c r="I26" s="32"/>
+      <c r="J26" s="32"/>
+      <c r="K26" s="32"/>
+      <c r="L26" s="32"/>
+      <c r="M26" s="32"/>
+      <c r="N26" s="32"/>
+      <c r="O26" s="32"/>
+    </row>
+    <row r="27" spans="2:15">
+      <c r="B27" s="33"/>
+      <c r="C27" s="33"/>
+      <c r="D27" s="33"/>
+      <c r="E27" s="33"/>
+      <c r="F27" s="33"/>
+      <c r="G27" s="33"/>
+      <c r="H27" s="33"/>
+      <c r="I27" s="33"/>
+      <c r="J27" s="33"/>
+      <c r="K27" s="33"/>
+      <c r="L27" s="33"/>
+      <c r="M27" s="33"/>
+      <c r="N27" s="33"/>
+      <c r="O27" s="33"/>
+    </row>
+    <row r="28" spans="2:15">
+      <c r="B28" s="33"/>
+      <c r="C28" s="33"/>
+      <c r="D28" s="33"/>
+      <c r="E28" s="33"/>
+      <c r="F28" s="33"/>
+      <c r="G28" s="33"/>
+      <c r="H28" s="33"/>
+      <c r="I28" s="33"/>
+      <c r="J28" s="33"/>
+      <c r="K28" s="33"/>
+      <c r="L28" s="33"/>
+      <c r="M28" s="33"/>
+      <c r="N28" s="33"/>
+      <c r="O28" s="33"/>
+    </row>
+  </sheetData>
+  <mergeCells count="15">
+    <mergeCell ref="C1:S2"/>
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="T2:U2"/>
+    <mergeCell ref="C4:H4"/>
+    <mergeCell ref="I4:I6"/>
+    <mergeCell ref="J4:L4"/>
+    <mergeCell ref="C5:H5"/>
+    <mergeCell ref="J5:L5"/>
+    <mergeCell ref="B28:O28"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="B20:O25"/>
+    <mergeCell ref="B27:O27"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FBF716D-FD41-4431-A8BB-5A81BFB0390B}">
+  <dimension ref="B1:U28"/>
+  <sheetViews>
+    <sheetView topLeftCell="B7" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20:O25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="1.33203125" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" customWidth="1"/>
+    <col min="3" max="3" width="17.77734375" customWidth="1"/>
+    <col min="4" max="4" width="24.44140625" customWidth="1"/>
+    <col min="5" max="5" width="29" customWidth="1"/>
+    <col min="8" max="8" width="12.88671875" customWidth="1"/>
+    <col min="13" max="13" width="14.109375" customWidth="1"/>
+    <col min="14" max="14" width="13.109375" customWidth="1"/>
+    <col min="15" max="15" width="15.6640625" customWidth="1"/>
+    <col min="20" max="20" width="13.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:21" ht="27" customHeight="1">
+      <c r="C1" s="58" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+      <c r="G1" s="58"/>
+      <c r="H1" s="58"/>
+      <c r="I1" s="58"/>
+      <c r="J1" s="58"/>
+      <c r="K1" s="58"/>
+      <c r="L1" s="58"/>
+      <c r="M1" s="58"/>
+      <c r="N1" s="58"/>
+      <c r="O1" s="58"/>
+      <c r="P1" s="58"/>
+      <c r="Q1" s="58"/>
+      <c r="R1" s="58"/>
+      <c r="S1" s="58"/>
+      <c r="T1" s="55" t="s">
+        <v>63</v>
+      </c>
+      <c r="U1" s="56"/>
+    </row>
+    <row r="2" spans="2:21" ht="15" thickBot="1">
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="58"/>
+      <c r="F2" s="58"/>
+      <c r="G2" s="58"/>
+      <c r="H2" s="58"/>
+      <c r="I2" s="58"/>
+      <c r="J2" s="58"/>
+      <c r="K2" s="58"/>
+      <c r="L2" s="58"/>
+      <c r="M2" s="58"/>
+      <c r="N2" s="58"/>
+      <c r="O2" s="58"/>
+      <c r="P2" s="58"/>
+      <c r="Q2" s="58"/>
+      <c r="R2" s="58"/>
+      <c r="S2" s="58"/>
+      <c r="T2" s="57" t="s">
+        <v>64</v>
+      </c>
+      <c r="U2" s="57"/>
+    </row>
+    <row r="3" spans="2:21" ht="15" thickBot="1">
+      <c r="C3" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
+      <c r="K3" s="25"/>
+      <c r="L3" s="25"/>
+      <c r="M3" s="25"/>
+      <c r="N3" s="25"/>
+      <c r="O3" s="25"/>
+      <c r="P3" s="25"/>
+      <c r="Q3" s="25"/>
+      <c r="R3" s="25"/>
+      <c r="S3" s="25"/>
+      <c r="T3" s="24"/>
+      <c r="U3" s="24"/>
+    </row>
+    <row r="4" spans="2:21" ht="29.4" customHeight="1" thickBot="1">
+      <c r="C4" s="34" t="s">
+        <v>105</v>
+      </c>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="35"/>
+      <c r="H4" s="36"/>
+      <c r="I4" s="51" t="s">
+        <v>68</v>
+      </c>
+      <c r="J4" s="60" t="s">
+        <v>12</v>
+      </c>
+      <c r="K4" s="61"/>
+      <c r="L4" s="62"/>
+    </row>
+    <row r="5" spans="2:21" ht="15" thickBot="1">
+      <c r="C5" s="34" t="s">
+        <v>66</v>
+      </c>
+      <c r="D5" s="35"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="35"/>
+      <c r="G5" s="35"/>
+      <c r="H5" s="36"/>
+      <c r="I5" s="53"/>
+      <c r="J5" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="K5" s="35"/>
+      <c r="L5" s="36"/>
+    </row>
+    <row r="6" spans="2:21" ht="58.2" thickBot="1">
+      <c r="B6" s="4"/>
+      <c r="C6" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="G6" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="I6" s="54"/>
+      <c r="J6" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="K6" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="L6" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="M6" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="N6" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="O6" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="P6" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q6" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="R6" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="S6" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="T6" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="U6" s="14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="2:21" ht="15" thickBot="1">
+      <c r="B7" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="E7" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="F7" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="G7" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="H7" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="I7" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="J7" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="K7" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="L7" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="M7" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="N7" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="O7" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="P7" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q7" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="R7" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="S7" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="T7" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="U7" s="13" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="2:21" ht="15" thickBot="1">
+      <c r="B8" s="8"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+    </row>
+    <row r="9" spans="2:21" ht="15" thickBot="1">
+      <c r="C9" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="D9" s="12"/>
+      <c r="E9" s="21" t="s">
+        <v>95</v>
+      </c>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="I9" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="J9" s="21" t="s">
+        <v>98</v>
+      </c>
+      <c r="K9" s="12"/>
+      <c r="L9" s="21" t="s">
+        <v>118</v>
+      </c>
+      <c r="M9" s="12"/>
+      <c r="N9" s="12"/>
+      <c r="O9" s="12"/>
+      <c r="P9" s="12"/>
+      <c r="Q9" s="12"/>
+      <c r="R9" s="12"/>
+      <c r="S9" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="T9" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="U9" s="12" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="10" spans="2:21">
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+    </row>
+    <row r="11" spans="2:21" ht="15" thickBot="1">
+      <c r="B11" s="1"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+    </row>
+    <row r="12" spans="2:21" ht="16.8" customHeight="1" thickBot="1">
+      <c r="B12" s="45" t="s">
+        <v>54</v>
+      </c>
+      <c r="C12" s="46"/>
+      <c r="D12" s="47"/>
+      <c r="E12" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+    </row>
+    <row r="13" spans="2:21">
+      <c r="B13" s="3"/>
+      <c r="C13" s="43"/>
+      <c r="D13" s="44"/>
+    </row>
+    <row r="14" spans="2:21" ht="15" thickBot="1">
+      <c r="B14" s="1"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="2"/>
+    </row>
+    <row r="15" spans="2:21" ht="39.6" customHeight="1" thickBot="1">
+      <c r="B15" s="37" t="s">
+        <v>58</v>
+      </c>
+      <c r="C15" s="38"/>
+      <c r="D15" s="39"/>
+      <c r="E15" s="18" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="16" spans="2:21" ht="43.8" customHeight="1" thickBot="1">
+      <c r="B16" s="40" t="s">
+        <v>59</v>
+      </c>
+      <c r="C16" s="41"/>
+      <c r="D16" s="42"/>
+      <c r="E16" s="18" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="17" spans="2:15">
+      <c r="B17" s="3"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
+    </row>
+    <row r="18" spans="2:15">
+      <c r="B18" s="3"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="17"/>
+    </row>
+    <row r="19" spans="2:15">
+      <c r="B19" s="16" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="20" spans="2:15">
+      <c r="B20" s="49" t="s">
+        <v>60</v>
+      </c>
+      <c r="C20" s="49"/>
+      <c r="D20" s="49"/>
+      <c r="E20" s="49"/>
+      <c r="F20" s="49"/>
+      <c r="G20" s="49"/>
+      <c r="H20" s="49"/>
+      <c r="I20" s="49"/>
+      <c r="J20" s="49"/>
+      <c r="K20" s="49"/>
+      <c r="L20" s="49"/>
+      <c r="M20" s="49"/>
+      <c r="N20" s="49"/>
+      <c r="O20" s="49"/>
+    </row>
+    <row r="21" spans="2:15">
+      <c r="B21" s="49"/>
+      <c r="C21" s="49"/>
+      <c r="D21" s="49"/>
+      <c r="E21" s="49"/>
+      <c r="F21" s="49"/>
+      <c r="G21" s="49"/>
+      <c r="H21" s="49"/>
+      <c r="I21" s="49"/>
+      <c r="J21" s="49"/>
+      <c r="K21" s="49"/>
+      <c r="L21" s="49"/>
+      <c r="M21" s="49"/>
+      <c r="N21" s="49"/>
+      <c r="O21" s="49"/>
+    </row>
+    <row r="22" spans="2:15">
+      <c r="B22" s="49"/>
+      <c r="C22" s="49"/>
+      <c r="D22" s="49"/>
+      <c r="E22" s="49"/>
+      <c r="F22" s="49"/>
+      <c r="G22" s="49"/>
+      <c r="H22" s="49"/>
+      <c r="I22" s="49"/>
+      <c r="J22" s="49"/>
+      <c r="K22" s="49"/>
+      <c r="L22" s="49"/>
+      <c r="M22" s="49"/>
+      <c r="N22" s="49"/>
+      <c r="O22" s="49"/>
+    </row>
+    <row r="23" spans="2:15">
+      <c r="B23" s="49"/>
+      <c r="C23" s="49"/>
+      <c r="D23" s="49"/>
+      <c r="E23" s="49"/>
+      <c r="F23" s="49"/>
+      <c r="G23" s="49"/>
+      <c r="H23" s="49"/>
+      <c r="I23" s="49"/>
+      <c r="J23" s="49"/>
+      <c r="K23" s="49"/>
+      <c r="L23" s="49"/>
+      <c r="M23" s="49"/>
+      <c r="N23" s="49"/>
+      <c r="O23" s="49"/>
+    </row>
+    <row r="24" spans="2:15">
+      <c r="B24" s="49"/>
+      <c r="C24" s="49"/>
+      <c r="D24" s="49"/>
+      <c r="E24" s="49"/>
+      <c r="F24" s="49"/>
+      <c r="G24" s="49"/>
+      <c r="H24" s="49"/>
+      <c r="I24" s="49"/>
+      <c r="J24" s="49"/>
+      <c r="K24" s="49"/>
+      <c r="L24" s="49"/>
+      <c r="M24" s="49"/>
+      <c r="N24" s="49"/>
+      <c r="O24" s="49"/>
+    </row>
+    <row r="25" spans="2:15">
+      <c r="B25" s="49"/>
+      <c r="C25" s="49"/>
+      <c r="D25" s="49"/>
+      <c r="E25" s="49"/>
+      <c r="F25" s="49"/>
+      <c r="G25" s="49"/>
+      <c r="H25" s="49"/>
+      <c r="I25" s="49"/>
+      <c r="J25" s="49"/>
+      <c r="K25" s="49"/>
+      <c r="L25" s="49"/>
+      <c r="M25" s="49"/>
+      <c r="N25" s="49"/>
+      <c r="O25" s="49"/>
+    </row>
+    <row r="26" spans="2:15">
+      <c r="B26" s="32"/>
+      <c r="C26" s="32"/>
+      <c r="D26" s="32"/>
+      <c r="E26" s="32"/>
+      <c r="F26" s="32"/>
+      <c r="G26" s="32"/>
+      <c r="H26" s="32"/>
+      <c r="I26" s="32"/>
+      <c r="J26" s="32"/>
+      <c r="K26" s="32"/>
+      <c r="L26" s="32"/>
+      <c r="M26" s="32"/>
+      <c r="N26" s="32"/>
+      <c r="O26" s="32"/>
+    </row>
+    <row r="27" spans="2:15">
+      <c r="B27" s="33"/>
+      <c r="C27" s="33"/>
+      <c r="D27" s="33"/>
+      <c r="E27" s="33"/>
+      <c r="F27" s="33"/>
+      <c r="G27" s="33"/>
+      <c r="H27" s="33"/>
+      <c r="I27" s="33"/>
+      <c r="J27" s="33"/>
+      <c r="K27" s="33"/>
+      <c r="L27" s="33"/>
+      <c r="M27" s="33"/>
+      <c r="N27" s="33"/>
+      <c r="O27" s="33"/>
+    </row>
+    <row r="28" spans="2:15">
+      <c r="B28" s="33"/>
+      <c r="C28" s="33"/>
+      <c r="D28" s="33"/>
+      <c r="E28" s="33"/>
+      <c r="F28" s="33"/>
+      <c r="G28" s="33"/>
+      <c r="H28" s="33"/>
+      <c r="I28" s="33"/>
+      <c r="J28" s="33"/>
+      <c r="K28" s="33"/>
+      <c r="L28" s="33"/>
+      <c r="M28" s="33"/>
+      <c r="N28" s="33"/>
+      <c r="O28" s="33"/>
+    </row>
+  </sheetData>
+  <mergeCells count="15">
+    <mergeCell ref="B28:O28"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="B20:O25"/>
+    <mergeCell ref="B27:O27"/>
+    <mergeCell ref="C1:S2"/>
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="T2:U2"/>
+    <mergeCell ref="C4:H4"/>
+    <mergeCell ref="I4:I6"/>
+    <mergeCell ref="J4:L4"/>
+    <mergeCell ref="C5:H5"/>
+    <mergeCell ref="J5:L5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
ultima actualizacion de la observacion de Cristel. Reporte excel Anexo 7 ( Notas)
</commit_message>
<xml_diff>
--- a/Unna.OperationalReport.WebSite/wwwroot/plantillas/reporte/mensual/BoletadeValorizacionPetroperu.xlsx
+++ b/Unna.OperationalReport.WebSite/wwwroot/plantillas/reporte/mensual/BoletadeValorizacionPetroperu.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desarrollos\SP\APSS SP\ProyectoPrincipalAenza6\UnnaReportesOperativos\Unna.OperationalReport.WebSite\wwwroot\plantillas\reporte\mensual\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6203B72-BC8D-4237-A174-BF1CD37AEFB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83D164D3-FEA4-4200-87EA-63631BC9B2F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="759" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="121">
   <si>
     <t>Energía
 (MMBTU)</t>
@@ -523,7 +523,7 @@
       <name val="Liberation-Regular"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -542,14 +542,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="22">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -622,15 +616,6 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -929,12 +914,6 @@
   </cellStyleXfs>
   <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="169" fontId="7" fillId="4" borderId="0" xfId="103" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="7" fillId="4" borderId="0" xfId="103" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="169" fontId="7" fillId="0" borderId="0" xfId="103" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -961,26 +940,20 @@
     <xf numFmtId="4" fontId="2" fillId="0" borderId="1" xfId="47" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="7" xfId="7" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="6" xfId="7" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="8" fillId="4" borderId="0" xfId="103" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="169" fontId="7" fillId="0" borderId="0" xfId="103" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="9" fillId="0" borderId="7" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="171" fontId="3" fillId="0" borderId="6" xfId="7" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="3" fillId="0" borderId="7" xfId="7" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="7" xfId="7" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="6" xfId="7" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="172" fontId="2" fillId="0" borderId="1" xfId="47" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -998,117 +971,127 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="8" fillId="0" borderId="0" xfId="103" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="103" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="9" fillId="0" borderId="1" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="8" fillId="0" borderId="0" xfId="103" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="103" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="2" xfId="103" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="3" xfId="103" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="10" xfId="103" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="11" xfId="103" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="7" xfId="103" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="12" xfId="103" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" xfId="103" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="9" fillId="0" borderId="1" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="14" xfId="103" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="15" xfId="103" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="16" xfId="103" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="2" xfId="103" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="3" xfId="103" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="11" xfId="103" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="12" xfId="103" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="8" xfId="103" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="13" xfId="103" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" xfId="103" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="6" xfId="103" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="15" xfId="103" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="16" xfId="103" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="17" xfId="103" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" xfId="103" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="8" fillId="0" borderId="0" xfId="103" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="103" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" xfId="103" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="104">
     <cellStyle name="Euro" xfId="35" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -1354,13 +1337,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>1150620</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>37</xdr:row>
       <xdr:rowOff>76201</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1604010</xdr:colOff>
-      <xdr:row>40</xdr:row>
+      <xdr:row>42</xdr:row>
       <xdr:rowOff>97340</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1468,13 +1451,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>1150620</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>37</xdr:row>
       <xdr:rowOff>76201</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1588770</xdr:colOff>
-      <xdr:row>40</xdr:row>
+      <xdr:row>42</xdr:row>
       <xdr:rowOff>97340</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1582,13 +1565,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>1150620</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>37</xdr:row>
       <xdr:rowOff>76201</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1573530</xdr:colOff>
-      <xdr:row>40</xdr:row>
+      <xdr:row>42</xdr:row>
       <xdr:rowOff>97340</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1956,8 +1939,8 @@
   <dimension ref="B1:AL31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B22" sqref="B22:O27"/>
+      <pane ySplit="6" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B12" sqref="B12:C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
@@ -1976,810 +1959,801 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:38" ht="27" customHeight="1">
-      <c r="C1" s="58" t="s">
+      <c r="C1" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
-      <c r="F1" s="58"/>
-      <c r="G1" s="58"/>
-      <c r="H1" s="58"/>
-      <c r="I1" s="58"/>
-      <c r="J1" s="58"/>
-      <c r="K1" s="58"/>
-      <c r="L1" s="58"/>
-      <c r="M1" s="58"/>
-      <c r="N1" s="58"/>
-      <c r="O1" s="58"/>
-      <c r="P1" s="58"/>
-      <c r="Q1" s="58"/>
-      <c r="R1" s="58"/>
-      <c r="S1" s="58"/>
-      <c r="T1" s="58"/>
-      <c r="U1" s="58"/>
-      <c r="V1" s="58"/>
-      <c r="W1" s="58"/>
-      <c r="X1" s="58"/>
-      <c r="Y1" s="58"/>
-      <c r="Z1" s="58"/>
-      <c r="AA1" s="58"/>
-      <c r="AB1" s="58"/>
-      <c r="AC1" s="58"/>
-      <c r="AD1" s="58"/>
-      <c r="AE1" s="58"/>
-      <c r="AF1" s="58"/>
-      <c r="AG1" s="58"/>
-      <c r="AH1" s="58"/>
-      <c r="AI1" s="58"/>
-      <c r="AJ1" s="58"/>
-      <c r="AK1" s="55" t="s">
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
+      <c r="I1" s="40"/>
+      <c r="J1" s="40"/>
+      <c r="K1" s="40"/>
+      <c r="L1" s="40"/>
+      <c r="M1" s="40"/>
+      <c r="N1" s="40"/>
+      <c r="O1" s="40"/>
+      <c r="P1" s="40"/>
+      <c r="Q1" s="40"/>
+      <c r="R1" s="40"/>
+      <c r="S1" s="40"/>
+      <c r="T1" s="40"/>
+      <c r="U1" s="40"/>
+      <c r="V1" s="40"/>
+      <c r="W1" s="40"/>
+      <c r="X1" s="40"/>
+      <c r="Y1" s="40"/>
+      <c r="Z1" s="40"/>
+      <c r="AA1" s="40"/>
+      <c r="AB1" s="40"/>
+      <c r="AC1" s="40"/>
+      <c r="AD1" s="40"/>
+      <c r="AE1" s="40"/>
+      <c r="AF1" s="40"/>
+      <c r="AG1" s="40"/>
+      <c r="AH1" s="40"/>
+      <c r="AI1" s="40"/>
+      <c r="AJ1" s="40"/>
+      <c r="AK1" s="37" t="s">
         <v>63</v>
       </c>
-      <c r="AL1" s="56"/>
+      <c r="AL1" s="38"/>
     </row>
     <row r="2" spans="2:38" ht="15" thickBot="1">
-      <c r="C2" s="59"/>
-      <c r="D2" s="59"/>
-      <c r="E2" s="58"/>
-      <c r="F2" s="58"/>
-      <c r="G2" s="58"/>
-      <c r="H2" s="58"/>
-      <c r="I2" s="58"/>
-      <c r="J2" s="58"/>
-      <c r="K2" s="58"/>
-      <c r="L2" s="58"/>
-      <c r="M2" s="58"/>
-      <c r="N2" s="58"/>
-      <c r="O2" s="58"/>
-      <c r="P2" s="58"/>
-      <c r="Q2" s="58"/>
-      <c r="R2" s="58"/>
-      <c r="S2" s="58"/>
-      <c r="T2" s="58"/>
-      <c r="U2" s="58"/>
-      <c r="V2" s="58"/>
-      <c r="W2" s="58"/>
-      <c r="X2" s="58"/>
-      <c r="Y2" s="58"/>
-      <c r="Z2" s="58"/>
-      <c r="AA2" s="58"/>
-      <c r="AB2" s="58"/>
-      <c r="AC2" s="58"/>
-      <c r="AD2" s="58"/>
-      <c r="AE2" s="58"/>
-      <c r="AF2" s="58"/>
-      <c r="AG2" s="58"/>
-      <c r="AH2" s="58"/>
-      <c r="AI2" s="58"/>
-      <c r="AJ2" s="58"/>
-      <c r="AK2" s="57" t="s">
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="40"/>
+      <c r="K2" s="40"/>
+      <c r="L2" s="40"/>
+      <c r="M2" s="40"/>
+      <c r="N2" s="40"/>
+      <c r="O2" s="40"/>
+      <c r="P2" s="40"/>
+      <c r="Q2" s="40"/>
+      <c r="R2" s="40"/>
+      <c r="S2" s="40"/>
+      <c r="T2" s="40"/>
+      <c r="U2" s="40"/>
+      <c r="V2" s="40"/>
+      <c r="W2" s="40"/>
+      <c r="X2" s="40"/>
+      <c r="Y2" s="40"/>
+      <c r="Z2" s="40"/>
+      <c r="AA2" s="40"/>
+      <c r="AB2" s="40"/>
+      <c r="AC2" s="40"/>
+      <c r="AD2" s="40"/>
+      <c r="AE2" s="40"/>
+      <c r="AF2" s="40"/>
+      <c r="AG2" s="40"/>
+      <c r="AH2" s="40"/>
+      <c r="AI2" s="40"/>
+      <c r="AJ2" s="40"/>
+      <c r="AK2" s="39" t="s">
         <v>64</v>
       </c>
-      <c r="AL2" s="57"/>
+      <c r="AL2" s="39"/>
     </row>
     <row r="3" spans="2:38" ht="15" thickBot="1">
-      <c r="C3" s="27" t="s">
+      <c r="C3" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="27" t="s">
+      <c r="D3" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
-      <c r="K3" s="25"/>
-      <c r="L3" s="25"/>
-      <c r="M3" s="25"/>
-      <c r="N3" s="25"/>
-      <c r="O3" s="25"/>
-      <c r="P3" s="25"/>
-      <c r="Q3" s="25"/>
-      <c r="R3" s="25"/>
-      <c r="S3" s="25"/>
-      <c r="T3" s="25"/>
-      <c r="U3" s="25"/>
-      <c r="V3" s="25"/>
-      <c r="W3" s="26"/>
-      <c r="X3" s="25"/>
-      <c r="Y3" s="25"/>
-      <c r="Z3" s="25"/>
-      <c r="AA3" s="25"/>
-      <c r="AB3" s="25"/>
-      <c r="AC3" s="25"/>
-      <c r="AD3" s="25"/>
-      <c r="AE3" s="25"/>
-      <c r="AF3" s="25"/>
-      <c r="AG3" s="25"/>
-      <c r="AH3" s="25"/>
-      <c r="AI3" s="25"/>
-      <c r="AJ3" s="25"/>
-      <c r="AK3" s="24"/>
-      <c r="AL3" s="24"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="21"/>
+      <c r="K3" s="21"/>
+      <c r="L3" s="21"/>
+      <c r="M3" s="21"/>
+      <c r="N3" s="21"/>
+      <c r="O3" s="21"/>
+      <c r="P3" s="21"/>
+      <c r="Q3" s="21"/>
+      <c r="R3" s="21"/>
+      <c r="S3" s="21"/>
+      <c r="T3" s="21"/>
+      <c r="U3" s="21"/>
+      <c r="V3" s="21"/>
+      <c r="W3" s="22"/>
+      <c r="X3" s="21"/>
+      <c r="Y3" s="21"/>
+      <c r="Z3" s="21"/>
+      <c r="AA3" s="21"/>
+      <c r="AB3" s="21"/>
+      <c r="AC3" s="21"/>
+      <c r="AD3" s="21"/>
+      <c r="AE3" s="21"/>
+      <c r="AF3" s="21"/>
+      <c r="AG3" s="21"/>
+      <c r="AH3" s="21"/>
+      <c r="AI3" s="21"/>
+      <c r="AJ3" s="21"/>
+      <c r="AK3" s="20"/>
+      <c r="AL3" s="20"/>
     </row>
     <row r="4" spans="2:38" ht="29.4" customHeight="1" thickBot="1">
-      <c r="C4" s="34" t="s">
+      <c r="C4" s="29" t="s">
         <v>105</v>
       </c>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="35"/>
-      <c r="H4" s="35"/>
-      <c r="I4" s="35"/>
-      <c r="J4" s="35"/>
-      <c r="K4" s="35"/>
-      <c r="L4" s="35"/>
-      <c r="M4" s="35"/>
-      <c r="N4" s="35"/>
-      <c r="O4" s="35"/>
-      <c r="P4" s="35"/>
-      <c r="Q4" s="35"/>
-      <c r="R4" s="35"/>
-      <c r="S4" s="35"/>
-      <c r="T4" s="35"/>
-      <c r="U4" s="36"/>
-      <c r="V4" s="51" t="s">
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="30"/>
+      <c r="I4" s="30"/>
+      <c r="J4" s="30"/>
+      <c r="K4" s="30"/>
+      <c r="L4" s="30"/>
+      <c r="M4" s="30"/>
+      <c r="N4" s="30"/>
+      <c r="O4" s="30"/>
+      <c r="P4" s="30"/>
+      <c r="Q4" s="30"/>
+      <c r="R4" s="30"/>
+      <c r="S4" s="30"/>
+      <c r="T4" s="30"/>
+      <c r="U4" s="31"/>
+      <c r="V4" s="33" t="s">
         <v>68</v>
       </c>
-      <c r="W4" s="51" t="s">
+      <c r="W4" s="33" t="s">
         <v>69</v>
       </c>
-      <c r="X4" s="34" t="s">
+      <c r="X4" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="Y4" s="35"/>
-      <c r="Z4" s="35"/>
-      <c r="AA4" s="35"/>
-      <c r="AB4" s="35"/>
-      <c r="AC4" s="36"/>
+      <c r="Y4" s="30"/>
+      <c r="Z4" s="30"/>
+      <c r="AA4" s="30"/>
+      <c r="AB4" s="30"/>
+      <c r="AC4" s="31"/>
     </row>
     <row r="5" spans="2:38" ht="15" thickBot="1">
-      <c r="C5" s="34" t="s">
+      <c r="C5" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="35"/>
-      <c r="G5" s="35"/>
-      <c r="H5" s="36"/>
-      <c r="I5" s="34" t="s">
+      <c r="D5" s="30"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="30"/>
+      <c r="H5" s="31"/>
+      <c r="I5" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="J5" s="35"/>
-      <c r="K5" s="35"/>
-      <c r="L5" s="35"/>
-      <c r="M5" s="35"/>
-      <c r="N5" s="36"/>
-      <c r="O5" s="34" t="s">
+      <c r="J5" s="30"/>
+      <c r="K5" s="30"/>
+      <c r="L5" s="30"/>
+      <c r="M5" s="30"/>
+      <c r="N5" s="31"/>
+      <c r="O5" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="P5" s="35"/>
-      <c r="Q5" s="35"/>
-      <c r="R5" s="35"/>
-      <c r="S5" s="35"/>
-      <c r="T5" s="35"/>
-      <c r="U5" s="51" t="s">
+      <c r="P5" s="30"/>
+      <c r="Q5" s="30"/>
+      <c r="R5" s="30"/>
+      <c r="S5" s="30"/>
+      <c r="T5" s="30"/>
+      <c r="U5" s="33" t="s">
         <v>67</v>
       </c>
-      <c r="V5" s="53"/>
-      <c r="W5" s="53"/>
-      <c r="X5" s="34" t="s">
+      <c r="V5" s="35"/>
+      <c r="W5" s="35"/>
+      <c r="X5" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="Y5" s="35"/>
-      <c r="Z5" s="35"/>
-      <c r="AA5" s="35"/>
-      <c r="AB5" s="35"/>
-      <c r="AC5" s="36"/>
+      <c r="Y5" s="30"/>
+      <c r="Z5" s="30"/>
+      <c r="AA5" s="30"/>
+      <c r="AB5" s="30"/>
+      <c r="AC5" s="31"/>
     </row>
     <row r="6" spans="2:38" ht="58.2" thickBot="1">
-      <c r="B6" s="4"/>
-      <c r="C6" s="10" t="s">
+      <c r="B6" s="2"/>
+      <c r="C6" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="D6" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="E6" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="F6" s="14" t="s">
+      <c r="F6" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="G6" s="14" t="s">
+      <c r="G6" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="H6" s="11" t="s">
+      <c r="H6" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="I6" s="10" t="s">
+      <c r="I6" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="J6" s="14" t="s">
+      <c r="J6" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="K6" s="14" t="s">
+      <c r="K6" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="L6" s="14" t="s">
+      <c r="L6" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="M6" s="14" t="s">
+      <c r="M6" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="N6" s="11" t="s">
+      <c r="N6" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="O6" s="10" t="s">
+      <c r="O6" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="P6" s="14" t="s">
+      <c r="P6" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="Q6" s="14" t="s">
+      <c r="Q6" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="R6" s="14" t="s">
+      <c r="R6" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="S6" s="14" t="s">
+      <c r="S6" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="T6" s="11" t="s">
+      <c r="T6" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="U6" s="52"/>
-      <c r="V6" s="54"/>
-      <c r="W6" s="54"/>
-      <c r="X6" s="14" t="s">
+      <c r="U6" s="34"/>
+      <c r="V6" s="36"/>
+      <c r="W6" s="36"/>
+      <c r="X6" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="Y6" s="14" t="s">
+      <c r="Y6" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="Z6" s="14" t="s">
+      <c r="Z6" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="AA6" s="14" t="s">
+      <c r="AA6" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="AB6" s="14" t="s">
+      <c r="AB6" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="AC6" s="14" t="s">
+      <c r="AC6" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="AD6" s="14" t="s">
+      <c r="AD6" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="AE6" s="14" t="s">
+      <c r="AE6" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="AF6" s="14" t="s">
+      <c r="AF6" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="AG6" s="14" t="s">
+      <c r="AG6" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="AH6" s="14" t="s">
+      <c r="AH6" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="AI6" s="14" t="s">
+      <c r="AI6" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="AJ6" s="14" t="s">
+      <c r="AJ6" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="AK6" s="14" t="s">
+      <c r="AK6" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="AL6" s="14" t="s">
+      <c r="AL6" s="12" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="7" spans="2:38" ht="15" thickBot="1">
-      <c r="B7" s="23" t="s">
+      <c r="B7" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="20" t="s">
+      <c r="C7" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="D7" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="E7" s="20" t="s">
+      <c r="E7" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="F7" s="20" t="s">
+      <c r="F7" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="G7" s="13" t="s">
+      <c r="G7" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="H7" s="13" t="s">
+      <c r="H7" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="I7" s="20" t="s">
+      <c r="I7" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="J7" s="13" t="s">
+      <c r="J7" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="K7" s="20" t="s">
+      <c r="K7" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="L7" s="20" t="s">
+      <c r="L7" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="M7" s="13" t="s">
+      <c r="M7" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="N7" s="13" t="s">
+      <c r="N7" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="O7" s="20" t="s">
+      <c r="O7" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="P7" s="13" t="s">
+      <c r="P7" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="Q7" s="20" t="s">
+      <c r="Q7" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="R7" s="20" t="s">
+      <c r="R7" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="S7" s="13" t="s">
+      <c r="S7" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="T7" s="13" t="s">
+      <c r="T7" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="U7" s="13" t="s">
+      <c r="U7" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="V7" s="13" t="s">
+      <c r="V7" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="W7" s="13" t="s">
+      <c r="W7" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="X7" s="20" t="s">
+      <c r="X7" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="Y7" s="20" t="s">
+      <c r="Y7" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="Z7" s="20" t="s">
+      <c r="Z7" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="AA7" s="20" t="s">
+      <c r="AA7" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="AB7" s="13" t="s">
+      <c r="AB7" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="AC7" s="20" t="s">
+      <c r="AC7" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="AD7" s="20" t="s">
+      <c r="AD7" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="AE7" s="20" t="s">
+      <c r="AE7" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="AF7" s="20" t="s">
+      <c r="AF7" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="AG7" s="13" t="s">
+      <c r="AG7" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="AH7" s="19" t="s">
+      <c r="AH7" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="AI7" s="13" t="s">
+      <c r="AI7" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="AJ7" s="13" t="s">
+      <c r="AJ7" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="AK7" s="20" t="s">
+      <c r="AK7" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="AL7" s="13" t="s">
+      <c r="AL7" s="11" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="8" spans="2:38" ht="15" thickBot="1">
-      <c r="B8" s="8"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
     </row>
     <row r="9" spans="2:38" ht="15" thickBot="1">
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="D9" s="12"/>
-      <c r="E9" s="21" t="s">
+      <c r="D9" s="10"/>
+      <c r="E9" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12" t="s">
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="I9" s="12" t="s">
+      <c r="I9" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="J9" s="12"/>
-      <c r="K9" s="21" t="s">
+      <c r="J9" s="10"/>
+      <c r="K9" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="L9" s="12"/>
-      <c r="M9" s="12"/>
-      <c r="N9" s="12" t="s">
+      <c r="L9" s="10"/>
+      <c r="M9" s="10"/>
+      <c r="N9" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="O9" s="12" t="s">
+      <c r="O9" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="P9" s="12"/>
-      <c r="Q9" s="21" t="s">
+      <c r="P9" s="10"/>
+      <c r="Q9" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="R9" s="12"/>
-      <c r="S9" s="12"/>
-      <c r="T9" s="12" t="s">
+      <c r="R9" s="10"/>
+      <c r="S9" s="10"/>
+      <c r="T9" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="U9" s="12" t="s">
+      <c r="U9" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="V9" s="12" t="s">
+      <c r="V9" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="W9" s="12"/>
-      <c r="X9" s="21" t="s">
+      <c r="W9" s="10"/>
+      <c r="X9" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="Y9" s="21" t="s">
+      <c r="Y9" s="17" t="s">
         <v>97</v>
       </c>
-      <c r="Z9" s="21" t="s">
+      <c r="Z9" s="17" t="s">
         <v>98</v>
       </c>
-      <c r="AA9" s="21" t="s">
+      <c r="AA9" s="17" t="s">
         <v>99</v>
       </c>
-      <c r="AB9" s="12"/>
-      <c r="AC9" s="21" t="s">
+      <c r="AB9" s="10"/>
+      <c r="AC9" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="AD9" s="12"/>
-      <c r="AE9" s="12"/>
-      <c r="AF9" s="12"/>
-      <c r="AG9" s="12"/>
-      <c r="AH9" s="12"/>
-      <c r="AI9" s="12"/>
-      <c r="AJ9" s="12" t="s">
+      <c r="AD9" s="10"/>
+      <c r="AE9" s="10"/>
+      <c r="AF9" s="10"/>
+      <c r="AG9" s="10"/>
+      <c r="AH9" s="10"/>
+      <c r="AI9" s="10"/>
+      <c r="AJ9" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="AK9" s="21" t="s">
+      <c r="AK9" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="AL9" s="12" t="s">
+      <c r="AL9" s="10" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="10" spans="2:38">
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
     </row>
     <row r="11" spans="2:38">
-      <c r="B11" s="16" t="s">
+      <c r="B11" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
     </row>
     <row r="12" spans="2:38" ht="24.6" customHeight="1">
-      <c r="B12" s="50" t="s">
+      <c r="B12" s="32" t="s">
         <v>107</v>
       </c>
-      <c r="C12" s="50"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
+      <c r="C12" s="32"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
     </row>
     <row r="13" spans="2:38" ht="27.6" customHeight="1" thickBot="1">
-      <c r="B13" s="48" t="s">
+      <c r="B13" s="53" t="s">
         <v>108</v>
       </c>
-      <c r="C13" s="48"/>
-      <c r="D13" s="29"/>
-      <c r="E13" s="30"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="6"/>
-      <c r="K13" s="6"/>
-      <c r="L13" s="6"/>
-      <c r="M13" s="6"/>
-      <c r="N13" s="6"/>
-      <c r="O13" s="6"/>
-      <c r="P13" s="6"/>
-      <c r="Q13" s="6"/>
-      <c r="R13" s="6"/>
-      <c r="S13" s="6"/>
-      <c r="T13" s="6"/>
-      <c r="U13" s="6"/>
-      <c r="V13" s="6"/>
-      <c r="W13" s="6"/>
+      <c r="C13" s="53"/>
+      <c r="D13" s="25"/>
+      <c r="E13" s="26"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="4"/>
+      <c r="M13" s="4"/>
+      <c r="N13" s="4"/>
+      <c r="O13" s="4"/>
+      <c r="P13" s="4"/>
+      <c r="Q13" s="4"/>
+      <c r="R13" s="4"/>
+      <c r="S13" s="4"/>
+      <c r="T13" s="4"/>
+      <c r="U13" s="4"/>
+      <c r="V13" s="4"/>
+      <c r="W13" s="4"/>
     </row>
     <row r="14" spans="2:38" ht="16.8" customHeight="1" thickBot="1">
-      <c r="B14" s="45" t="s">
+      <c r="B14" s="50" t="s">
         <v>54</v>
       </c>
-      <c r="C14" s="46"/>
-      <c r="D14" s="47"/>
-      <c r="E14" s="22" t="s">
+      <c r="C14" s="51"/>
+      <c r="D14" s="52"/>
+      <c r="E14" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="6"/>
-      <c r="K14" s="6"/>
-      <c r="L14" s="6"/>
-      <c r="M14" s="6"/>
-      <c r="N14" s="6"/>
-      <c r="O14" s="6"/>
-      <c r="P14" s="6"/>
-      <c r="Q14" s="6"/>
-      <c r="R14" s="6"/>
-      <c r="S14" s="6"/>
-      <c r="T14" s="6"/>
-      <c r="U14" s="6"/>
-      <c r="V14" s="6"/>
-      <c r="W14" s="6"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
+      <c r="L14" s="4"/>
+      <c r="M14" s="4"/>
+      <c r="N14" s="4"/>
+      <c r="O14" s="4"/>
+      <c r="P14" s="4"/>
+      <c r="Q14" s="4"/>
+      <c r="R14" s="4"/>
+      <c r="S14" s="4"/>
+      <c r="T14" s="4"/>
+      <c r="U14" s="4"/>
+      <c r="V14" s="4"/>
+      <c r="W14" s="4"/>
     </row>
     <row r="15" spans="2:38" ht="15" thickBot="1">
-      <c r="B15" s="3"/>
-      <c r="C15" s="43"/>
-      <c r="D15" s="44"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="49"/>
+      <c r="D15" s="61"/>
+      <c r="E15" s="62"/>
     </row>
     <row r="16" spans="2:38" ht="29.4" thickBot="1">
-      <c r="B16" s="3"/>
-      <c r="C16" s="29"/>
-      <c r="D16" s="29"/>
-      <c r="E16" s="14" t="s">
+      <c r="B16" s="1"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="12" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="17" spans="2:15" ht="39.6" customHeight="1" thickBot="1">
-      <c r="B17" s="37" t="s">
+      <c r="B17" s="43" t="s">
         <v>58</v>
       </c>
-      <c r="C17" s="38"/>
-      <c r="D17" s="39"/>
-      <c r="E17" s="31" t="s">
+      <c r="C17" s="44"/>
+      <c r="D17" s="45"/>
+      <c r="E17" s="27" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="18" spans="2:15" ht="43.8" customHeight="1" thickBot="1">
-      <c r="B18" s="40" t="s">
+      <c r="B18" s="46" t="s">
         <v>59</v>
       </c>
-      <c r="C18" s="41"/>
-      <c r="D18" s="42"/>
-      <c r="E18" s="31" t="s">
+      <c r="C18" s="47"/>
+      <c r="D18" s="48"/>
+      <c r="E18" s="27" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="19" spans="2:15">
-      <c r="B19" s="3"/>
-      <c r="C19" s="17"/>
-      <c r="D19" s="17"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
     </row>
     <row r="20" spans="2:15">
-      <c r="B20" s="3"/>
-      <c r="C20" s="17"/>
-      <c r="D20" s="17"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
     </row>
     <row r="21" spans="2:15">
-      <c r="B21" s="16" t="s">
+      <c r="B21" s="13" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="22" spans="2:15">
-      <c r="B22" s="49" t="s">
+      <c r="B22" s="54" t="s">
         <v>60</v>
       </c>
-      <c r="C22" s="49"/>
-      <c r="D22" s="49"/>
-      <c r="E22" s="49"/>
-      <c r="F22" s="49"/>
-      <c r="G22" s="49"/>
-      <c r="H22" s="49"/>
-      <c r="I22" s="49"/>
-      <c r="J22" s="49"/>
-      <c r="K22" s="49"/>
-      <c r="L22" s="49"/>
-      <c r="M22" s="49"/>
-      <c r="N22" s="49"/>
-      <c r="O22" s="49"/>
+      <c r="C22" s="54"/>
+      <c r="D22" s="54"/>
+      <c r="E22" s="54"/>
+      <c r="F22" s="54"/>
+      <c r="G22" s="54"/>
+      <c r="H22" s="54"/>
+      <c r="I22" s="54"/>
+      <c r="J22" s="54"/>
+      <c r="K22" s="54"/>
+      <c r="L22" s="54"/>
+      <c r="M22" s="54"/>
+      <c r="N22" s="54"/>
+      <c r="O22" s="54"/>
     </row>
     <row r="23" spans="2:15">
-      <c r="B23" s="49"/>
-      <c r="C23" s="49"/>
-      <c r="D23" s="49"/>
-      <c r="E23" s="49"/>
-      <c r="F23" s="49"/>
-      <c r="G23" s="49"/>
-      <c r="H23" s="49"/>
-      <c r="I23" s="49"/>
-      <c r="J23" s="49"/>
-      <c r="K23" s="49"/>
-      <c r="L23" s="49"/>
-      <c r="M23" s="49"/>
-      <c r="N23" s="49"/>
-      <c r="O23" s="49"/>
+      <c r="B23" s="54"/>
+      <c r="C23" s="54"/>
+      <c r="D23" s="54"/>
+      <c r="E23" s="54"/>
+      <c r="F23" s="54"/>
+      <c r="G23" s="54"/>
+      <c r="H23" s="54"/>
+      <c r="I23" s="54"/>
+      <c r="J23" s="54"/>
+      <c r="K23" s="54"/>
+      <c r="L23" s="54"/>
+      <c r="M23" s="54"/>
+      <c r="N23" s="54"/>
+      <c r="O23" s="54"/>
     </row>
     <row r="24" spans="2:15">
-      <c r="B24" s="49"/>
-      <c r="C24" s="49"/>
-      <c r="D24" s="49"/>
-      <c r="E24" s="49"/>
-      <c r="F24" s="49"/>
-      <c r="G24" s="49"/>
-      <c r="H24" s="49"/>
-      <c r="I24" s="49"/>
-      <c r="J24" s="49"/>
-      <c r="K24" s="49"/>
-      <c r="L24" s="49"/>
-      <c r="M24" s="49"/>
-      <c r="N24" s="49"/>
-      <c r="O24" s="49"/>
+      <c r="B24" s="54"/>
+      <c r="C24" s="54"/>
+      <c r="D24" s="54"/>
+      <c r="E24" s="54"/>
+      <c r="F24" s="54"/>
+      <c r="G24" s="54"/>
+      <c r="H24" s="54"/>
+      <c r="I24" s="54"/>
+      <c r="J24" s="54"/>
+      <c r="K24" s="54"/>
+      <c r="L24" s="54"/>
+      <c r="M24" s="54"/>
+      <c r="N24" s="54"/>
+      <c r="O24" s="54"/>
     </row>
     <row r="25" spans="2:15">
-      <c r="B25" s="49"/>
-      <c r="C25" s="49"/>
-      <c r="D25" s="49"/>
-      <c r="E25" s="49"/>
-      <c r="F25" s="49"/>
-      <c r="G25" s="49"/>
-      <c r="H25" s="49"/>
-      <c r="I25" s="49"/>
-      <c r="J25" s="49"/>
-      <c r="K25" s="49"/>
-      <c r="L25" s="49"/>
-      <c r="M25" s="49"/>
-      <c r="N25" s="49"/>
-      <c r="O25" s="49"/>
+      <c r="B25" s="54"/>
+      <c r="C25" s="54"/>
+      <c r="D25" s="54"/>
+      <c r="E25" s="54"/>
+      <c r="F25" s="54"/>
+      <c r="G25" s="54"/>
+      <c r="H25" s="54"/>
+      <c r="I25" s="54"/>
+      <c r="J25" s="54"/>
+      <c r="K25" s="54"/>
+      <c r="L25" s="54"/>
+      <c r="M25" s="54"/>
+      <c r="N25" s="54"/>
+      <c r="O25" s="54"/>
     </row>
     <row r="26" spans="2:15">
-      <c r="B26" s="49"/>
-      <c r="C26" s="49"/>
-      <c r="D26" s="49"/>
-      <c r="E26" s="49"/>
-      <c r="F26" s="49"/>
-      <c r="G26" s="49"/>
-      <c r="H26" s="49"/>
-      <c r="I26" s="49"/>
-      <c r="J26" s="49"/>
-      <c r="K26" s="49"/>
-      <c r="L26" s="49"/>
-      <c r="M26" s="49"/>
-      <c r="N26" s="49"/>
-      <c r="O26" s="49"/>
+      <c r="B26" s="54"/>
+      <c r="C26" s="54"/>
+      <c r="D26" s="54"/>
+      <c r="E26" s="54"/>
+      <c r="F26" s="54"/>
+      <c r="G26" s="54"/>
+      <c r="H26" s="54"/>
+      <c r="I26" s="54"/>
+      <c r="J26" s="54"/>
+      <c r="K26" s="54"/>
+      <c r="L26" s="54"/>
+      <c r="M26" s="54"/>
+      <c r="N26" s="54"/>
+      <c r="O26" s="54"/>
     </row>
     <row r="27" spans="2:15">
-      <c r="B27" s="49"/>
-      <c r="C27" s="49"/>
-      <c r="D27" s="49"/>
-      <c r="E27" s="49"/>
-      <c r="F27" s="49"/>
-      <c r="G27" s="49"/>
-      <c r="H27" s="49"/>
-      <c r="I27" s="49"/>
-      <c r="J27" s="49"/>
-      <c r="K27" s="49"/>
-      <c r="L27" s="49"/>
-      <c r="M27" s="49"/>
-      <c r="N27" s="49"/>
-      <c r="O27" s="49"/>
+      <c r="B27" s="54"/>
+      <c r="C27" s="54"/>
+      <c r="D27" s="54"/>
+      <c r="E27" s="54"/>
+      <c r="F27" s="54"/>
+      <c r="G27" s="54"/>
+      <c r="H27" s="54"/>
+      <c r="I27" s="54"/>
+      <c r="J27" s="54"/>
+      <c r="K27" s="54"/>
+      <c r="L27" s="54"/>
+      <c r="M27" s="54"/>
+      <c r="N27" s="54"/>
+      <c r="O27" s="54"/>
     </row>
     <row r="28" spans="2:15">
-      <c r="B28" s="24"/>
-      <c r="C28" s="24"/>
-      <c r="D28" s="24"/>
-      <c r="E28" s="24"/>
-      <c r="F28" s="24"/>
-      <c r="G28" s="24"/>
-      <c r="H28" s="24"/>
-      <c r="I28" s="24"/>
-      <c r="J28" s="24"/>
-      <c r="K28" s="24"/>
-      <c r="L28" s="24"/>
-      <c r="M28" s="24"/>
-      <c r="N28" s="24"/>
-      <c r="O28" s="24"/>
+      <c r="B28" s="20"/>
+      <c r="C28" s="20"/>
+      <c r="D28" s="20"/>
+      <c r="E28" s="20"/>
+      <c r="F28" s="20"/>
+      <c r="G28" s="20"/>
+      <c r="H28" s="20"/>
+      <c r="I28" s="20"/>
+      <c r="J28" s="20"/>
+      <c r="K28" s="20"/>
+      <c r="L28" s="20"/>
+      <c r="M28" s="20"/>
+      <c r="N28" s="20"/>
+      <c r="O28" s="20"/>
     </row>
     <row r="29" spans="2:15">
-      <c r="B29" s="33" t="s">
+      <c r="B29" s="42" t="s">
         <v>61</v>
       </c>
-      <c r="C29" s="33"/>
-      <c r="D29" s="33"/>
-      <c r="E29" s="33"/>
-      <c r="F29" s="33"/>
-      <c r="G29" s="33"/>
-      <c r="H29" s="33"/>
-      <c r="I29" s="33"/>
-      <c r="J29" s="33"/>
-      <c r="K29" s="33"/>
-      <c r="L29" s="33"/>
-      <c r="M29" s="33"/>
-      <c r="N29" s="33"/>
-      <c r="O29" s="33"/>
+      <c r="C29" s="42"/>
+      <c r="D29" s="42"/>
+      <c r="E29" s="42"/>
+      <c r="F29" s="42"/>
+      <c r="G29" s="42"/>
+      <c r="H29" s="42"/>
+      <c r="I29" s="42"/>
+      <c r="J29" s="42"/>
+      <c r="K29" s="42"/>
+      <c r="L29" s="42"/>
+      <c r="M29" s="42"/>
+      <c r="N29" s="42"/>
+      <c r="O29" s="42"/>
     </row>
     <row r="30" spans="2:15">
-      <c r="B30" s="33" t="s">
+      <c r="B30" s="42" t="s">
         <v>62</v>
       </c>
-      <c r="C30" s="33"/>
-      <c r="D30" s="33"/>
-      <c r="E30" s="33"/>
-      <c r="F30" s="33"/>
-      <c r="G30" s="33"/>
-      <c r="H30" s="33"/>
-      <c r="I30" s="33"/>
-      <c r="J30" s="33"/>
-      <c r="K30" s="33"/>
-      <c r="L30" s="33"/>
-      <c r="M30" s="33"/>
-      <c r="N30" s="33"/>
-      <c r="O30" s="33"/>
+      <c r="C30" s="42"/>
+      <c r="D30" s="42"/>
+      <c r="E30" s="42"/>
+      <c r="F30" s="42"/>
+      <c r="G30" s="42"/>
+      <c r="H30" s="42"/>
+      <c r="I30" s="42"/>
+      <c r="J30" s="42"/>
+      <c r="K30" s="42"/>
+      <c r="L30" s="42"/>
+      <c r="M30" s="42"/>
+      <c r="N30" s="42"/>
+      <c r="O30" s="42"/>
     </row>
     <row r="31" spans="2:15">
-      <c r="B31" s="33" t="s">
+      <c r="B31" s="42" t="s">
         <v>110</v>
       </c>
-      <c r="C31" s="33"/>
-      <c r="D31" s="33"/>
-      <c r="E31" s="33"/>
-      <c r="F31" s="33"/>
-      <c r="G31" s="33"/>
-      <c r="H31" s="33"/>
-      <c r="I31" s="33"/>
-      <c r="J31" s="33"/>
-      <c r="K31" s="33"/>
-      <c r="L31" s="33"/>
-      <c r="M31" s="33"/>
-      <c r="N31" s="33"/>
-      <c r="O31" s="33"/>
+      <c r="C31" s="42"/>
+      <c r="D31" s="42"/>
+      <c r="E31" s="42"/>
+      <c r="F31" s="42"/>
+      <c r="G31" s="42"/>
+      <c r="H31" s="42"/>
+      <c r="I31" s="42"/>
+      <c r="J31" s="42"/>
+      <c r="K31" s="42"/>
+      <c r="L31" s="42"/>
+      <c r="M31" s="42"/>
+      <c r="N31" s="42"/>
+      <c r="O31" s="42"/>
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="C4:U4"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="U5:U6"/>
-    <mergeCell ref="W4:W6"/>
-    <mergeCell ref="AK1:AL1"/>
-    <mergeCell ref="AK2:AL2"/>
-    <mergeCell ref="C1:AJ2"/>
-    <mergeCell ref="X5:AC5"/>
-    <mergeCell ref="X4:AC4"/>
-    <mergeCell ref="V4:V6"/>
     <mergeCell ref="B29:O29"/>
     <mergeCell ref="B30:O30"/>
     <mergeCell ref="B31:O31"/>
@@ -2792,6 +2766,16 @@
     <mergeCell ref="B14:D14"/>
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="B22:O27"/>
+    <mergeCell ref="C4:U4"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="U5:U6"/>
+    <mergeCell ref="W4:W6"/>
+    <mergeCell ref="AK1:AL1"/>
+    <mergeCell ref="AK2:AL2"/>
+    <mergeCell ref="C1:AJ2"/>
+    <mergeCell ref="X5:AC5"/>
+    <mergeCell ref="X4:AC4"/>
+    <mergeCell ref="V4:V6"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" horizontalDpi="300" r:id="rId1"/>
@@ -2801,10 +2785,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15F5674C-6194-49DE-8C68-201941F0F769}">
-  <dimension ref="B1:U28"/>
+  <dimension ref="B1:U30"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20:O25"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
@@ -2822,505 +2806,527 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:21" ht="27" customHeight="1">
-      <c r="C1" s="58" t="s">
+      <c r="C1" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
-      <c r="F1" s="58"/>
-      <c r="G1" s="58"/>
-      <c r="H1" s="58"/>
-      <c r="I1" s="58"/>
-      <c r="J1" s="58"/>
-      <c r="K1" s="58"/>
-      <c r="L1" s="58"/>
-      <c r="M1" s="58"/>
-      <c r="N1" s="58"/>
-      <c r="O1" s="58"/>
-      <c r="P1" s="58"/>
-      <c r="Q1" s="58"/>
-      <c r="R1" s="58"/>
-      <c r="S1" s="58"/>
-      <c r="T1" s="55" t="s">
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
+      <c r="I1" s="40"/>
+      <c r="J1" s="40"/>
+      <c r="K1" s="40"/>
+      <c r="L1" s="40"/>
+      <c r="M1" s="40"/>
+      <c r="N1" s="40"/>
+      <c r="O1" s="40"/>
+      <c r="P1" s="40"/>
+      <c r="Q1" s="40"/>
+      <c r="R1" s="40"/>
+      <c r="S1" s="40"/>
+      <c r="T1" s="37" t="s">
         <v>63</v>
       </c>
-      <c r="U1" s="56"/>
+      <c r="U1" s="38"/>
     </row>
     <row r="2" spans="2:21" ht="15" thickBot="1">
-      <c r="C2" s="59"/>
-      <c r="D2" s="59"/>
-      <c r="E2" s="58"/>
-      <c r="F2" s="58"/>
-      <c r="G2" s="58"/>
-      <c r="H2" s="58"/>
-      <c r="I2" s="58"/>
-      <c r="J2" s="58"/>
-      <c r="K2" s="58"/>
-      <c r="L2" s="58"/>
-      <c r="M2" s="58"/>
-      <c r="N2" s="58"/>
-      <c r="O2" s="58"/>
-      <c r="P2" s="58"/>
-      <c r="Q2" s="58"/>
-      <c r="R2" s="58"/>
-      <c r="S2" s="58"/>
-      <c r="T2" s="57" t="s">
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="40"/>
+      <c r="K2" s="40"/>
+      <c r="L2" s="40"/>
+      <c r="M2" s="40"/>
+      <c r="N2" s="40"/>
+      <c r="O2" s="40"/>
+      <c r="P2" s="40"/>
+      <c r="Q2" s="40"/>
+      <c r="R2" s="40"/>
+      <c r="S2" s="40"/>
+      <c r="T2" s="39" t="s">
         <v>64</v>
       </c>
-      <c r="U2" s="57"/>
+      <c r="U2" s="39"/>
     </row>
     <row r="3" spans="2:21" ht="15" thickBot="1">
-      <c r="C3" s="28" t="s">
+      <c r="C3" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="28" t="s">
+      <c r="D3" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
-      <c r="K3" s="25"/>
-      <c r="L3" s="25"/>
-      <c r="M3" s="25"/>
-      <c r="N3" s="25"/>
-      <c r="O3" s="25"/>
-      <c r="P3" s="25"/>
-      <c r="Q3" s="25"/>
-      <c r="R3" s="25"/>
-      <c r="S3" s="25"/>
-      <c r="T3" s="24"/>
-      <c r="U3" s="24"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="21"/>
+      <c r="K3" s="21"/>
+      <c r="L3" s="21"/>
+      <c r="M3" s="21"/>
+      <c r="N3" s="21"/>
+      <c r="O3" s="21"/>
+      <c r="P3" s="21"/>
+      <c r="Q3" s="21"/>
+      <c r="R3" s="21"/>
+      <c r="S3" s="21"/>
+      <c r="T3" s="20"/>
+      <c r="U3" s="20"/>
     </row>
     <row r="4" spans="2:21" ht="29.4" customHeight="1" thickBot="1">
-      <c r="C4" s="34" t="s">
+      <c r="C4" s="29" t="s">
         <v>105</v>
       </c>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="35"/>
-      <c r="H4" s="36"/>
-      <c r="I4" s="51" t="s">
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="33" t="s">
         <v>68</v>
       </c>
-      <c r="J4" s="60" t="s">
+      <c r="J4" s="55" t="s">
         <v>12</v>
       </c>
-      <c r="K4" s="61"/>
-      <c r="L4" s="62"/>
+      <c r="K4" s="56"/>
+      <c r="L4" s="57"/>
     </row>
     <row r="5" spans="2:21" ht="15" thickBot="1">
-      <c r="C5" s="34" t="s">
+      <c r="C5" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="35"/>
-      <c r="G5" s="35"/>
-      <c r="H5" s="36"/>
-      <c r="I5" s="53"/>
-      <c r="J5" s="34" t="s">
+      <c r="D5" s="30"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="30"/>
+      <c r="H5" s="31"/>
+      <c r="I5" s="35"/>
+      <c r="J5" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="K5" s="35"/>
-      <c r="L5" s="36"/>
+      <c r="K5" s="30"/>
+      <c r="L5" s="31"/>
     </row>
     <row r="6" spans="2:21" ht="58.2" thickBot="1">
-      <c r="B6" s="4"/>
-      <c r="C6" s="10" t="s">
+      <c r="B6" s="2"/>
+      <c r="C6" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="D6" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="E6" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="F6" s="14" t="s">
+      <c r="F6" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="G6" s="14" t="s">
+      <c r="G6" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="H6" s="11" t="s">
+      <c r="H6" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="I6" s="54"/>
-      <c r="J6" s="14" t="s">
+      <c r="I6" s="36"/>
+      <c r="J6" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="K6" s="14" t="s">
+      <c r="K6" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="L6" s="14" t="s">
+      <c r="L6" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="M6" s="14" t="s">
+      <c r="M6" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="N6" s="14" t="s">
+      <c r="N6" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="O6" s="14" t="s">
+      <c r="O6" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="P6" s="14" t="s">
+      <c r="P6" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="Q6" s="14" t="s">
+      <c r="Q6" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="R6" s="14" t="s">
+      <c r="R6" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="S6" s="14" t="s">
+      <c r="S6" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="T6" s="14" t="s">
+      <c r="T6" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="U6" s="14" t="s">
+      <c r="U6" s="12" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="7" spans="2:21" ht="15" thickBot="1">
-      <c r="B7" s="23" t="s">
+      <c r="B7" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="20" t="s">
+      <c r="C7" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="D7" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="E7" s="20" t="s">
+      <c r="E7" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="F7" s="20" t="s">
+      <c r="F7" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="G7" s="13" t="s">
+      <c r="G7" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="H7" s="13" t="s">
+      <c r="H7" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="I7" s="13" t="s">
+      <c r="I7" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="J7" s="20" t="s">
+      <c r="J7" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="K7" s="13" t="s">
+      <c r="K7" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="L7" s="20" t="s">
+      <c r="L7" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="M7" s="20" t="s">
+      <c r="M7" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="N7" s="20" t="s">
+      <c r="N7" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="O7" s="20" t="s">
+      <c r="O7" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="P7" s="13" t="s">
+      <c r="P7" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="Q7" s="19" t="s">
+      <c r="Q7" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="R7" s="13" t="s">
+      <c r="R7" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="S7" s="13" t="s">
+      <c r="S7" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="T7" s="20" t="s">
+      <c r="T7" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="U7" s="13" t="s">
+      <c r="U7" s="11" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="8" spans="2:21" ht="15" thickBot="1">
-      <c r="B8" s="8"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
     </row>
     <row r="9" spans="2:21" ht="15" thickBot="1">
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="D9" s="12"/>
-      <c r="E9" s="21" t="s">
+      <c r="D9" s="10"/>
+      <c r="E9" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12" t="s">
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="I9" s="12" t="s">
+      <c r="I9" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="J9" s="21" t="s">
+      <c r="J9" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="K9" s="12"/>
-      <c r="L9" s="21" t="s">
+      <c r="K9" s="10"/>
+      <c r="L9" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="M9" s="12"/>
-      <c r="N9" s="12"/>
-      <c r="O9" s="12"/>
-      <c r="P9" s="12"/>
-      <c r="Q9" s="12"/>
-      <c r="R9" s="12"/>
-      <c r="S9" s="12" t="s">
+      <c r="M9" s="10"/>
+      <c r="N9" s="10"/>
+      <c r="O9" s="10"/>
+      <c r="P9" s="10"/>
+      <c r="Q9" s="10"/>
+      <c r="R9" s="10"/>
+      <c r="S9" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="T9" s="21" t="s">
+      <c r="T9" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="U9" s="12" t="s">
+      <c r="U9" s="10" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="10" spans="2:21">
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-    </row>
-    <row r="11" spans="2:21" ht="15" thickBot="1">
-      <c r="B11" s="1"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
-    </row>
-    <row r="12" spans="2:21" ht="16.8" customHeight="1" thickBot="1">
-      <c r="B12" s="45" t="s">
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+    </row>
+    <row r="11" spans="2:21">
+      <c r="B11" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+    </row>
+    <row r="12" spans="2:21" ht="22.2" customHeight="1">
+      <c r="B12" s="32" t="s">
+        <v>107</v>
+      </c>
+      <c r="C12" s="32"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+    </row>
+    <row r="13" spans="2:21" ht="32.4" customHeight="1" thickBot="1">
+      <c r="B13" s="53" t="s">
+        <v>108</v>
+      </c>
+      <c r="C13" s="53"/>
+      <c r="D13" s="59"/>
+      <c r="E13" s="60"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+    </row>
+    <row r="14" spans="2:21" ht="16.8" customHeight="1" thickBot="1">
+      <c r="B14" s="50" t="s">
         <v>54</v>
       </c>
-      <c r="C12" s="46"/>
-      <c r="D12" s="47"/>
-      <c r="E12" s="22" t="s">
+      <c r="C14" s="51"/>
+      <c r="D14" s="52"/>
+      <c r="E14" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-    </row>
-    <row r="13" spans="2:21">
-      <c r="B13" s="3"/>
-      <c r="C13" s="43"/>
-      <c r="D13" s="44"/>
-    </row>
-    <row r="14" spans="2:21" ht="15" thickBot="1">
-      <c r="B14" s="1"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="2"/>
-    </row>
-    <row r="15" spans="2:21" ht="39.6" customHeight="1" thickBot="1">
-      <c r="B15" s="37" t="s">
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+    </row>
+    <row r="15" spans="2:21" ht="15" thickBot="1">
+      <c r="B15" s="1"/>
+      <c r="C15" s="49"/>
+      <c r="D15" s="61"/>
+      <c r="E15" s="62"/>
+    </row>
+    <row r="16" spans="2:21" ht="29.4" thickBot="1">
+      <c r="B16" s="58"/>
+      <c r="C16" s="59"/>
+      <c r="D16" s="59"/>
+      <c r="E16" s="12" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="17" spans="2:15" ht="39.6" customHeight="1" thickBot="1">
+      <c r="B17" s="43" t="s">
         <v>58</v>
       </c>
-      <c r="C15" s="38"/>
-      <c r="D15" s="39"/>
-      <c r="E15" s="18" t="s">
+      <c r="C17" s="44"/>
+      <c r="D17" s="45"/>
+      <c r="E17" s="27" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="16" spans="2:21" ht="43.8" customHeight="1" thickBot="1">
-      <c r="B16" s="40" t="s">
+    <row r="18" spans="2:15" ht="43.8" customHeight="1" thickBot="1">
+      <c r="B18" s="46" t="s">
         <v>59</v>
       </c>
-      <c r="C16" s="41"/>
-      <c r="D16" s="42"/>
-      <c r="E16" s="18" t="s">
+      <c r="C18" s="47"/>
+      <c r="D18" s="48"/>
+      <c r="E18" s="27" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="17" spans="2:15">
-      <c r="B17" s="3"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
-    </row>
-    <row r="18" spans="2:15">
-      <c r="B18" s="3"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="17"/>
-    </row>
     <row r="19" spans="2:15">
-      <c r="B19" s="16" t="s">
+      <c r="B19" s="1"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+    </row>
+    <row r="20" spans="2:15">
+      <c r="B20" s="1"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
+    </row>
+    <row r="21" spans="2:15">
+      <c r="B21" s="13" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="20" spans="2:15">
-      <c r="B20" s="49" t="s">
+    <row r="22" spans="2:15">
+      <c r="B22" s="54" t="s">
         <v>60</v>
       </c>
-      <c r="C20" s="49"/>
-      <c r="D20" s="49"/>
-      <c r="E20" s="49"/>
-      <c r="F20" s="49"/>
-      <c r="G20" s="49"/>
-      <c r="H20" s="49"/>
-      <c r="I20" s="49"/>
-      <c r="J20" s="49"/>
-      <c r="K20" s="49"/>
-      <c r="L20" s="49"/>
-      <c r="M20" s="49"/>
-      <c r="N20" s="49"/>
-      <c r="O20" s="49"/>
-    </row>
-    <row r="21" spans="2:15">
-      <c r="B21" s="49"/>
-      <c r="C21" s="49"/>
-      <c r="D21" s="49"/>
-      <c r="E21" s="49"/>
-      <c r="F21" s="49"/>
-      <c r="G21" s="49"/>
-      <c r="H21" s="49"/>
-      <c r="I21" s="49"/>
-      <c r="J21" s="49"/>
-      <c r="K21" s="49"/>
-      <c r="L21" s="49"/>
-      <c r="M21" s="49"/>
-      <c r="N21" s="49"/>
-      <c r="O21" s="49"/>
-    </row>
-    <row r="22" spans="2:15">
-      <c r="B22" s="49"/>
-      <c r="C22" s="49"/>
-      <c r="D22" s="49"/>
-      <c r="E22" s="49"/>
-      <c r="F22" s="49"/>
-      <c r="G22" s="49"/>
-      <c r="H22" s="49"/>
-      <c r="I22" s="49"/>
-      <c r="J22" s="49"/>
-      <c r="K22" s="49"/>
-      <c r="L22" s="49"/>
-      <c r="M22" s="49"/>
-      <c r="N22" s="49"/>
-      <c r="O22" s="49"/>
+      <c r="C22" s="54"/>
+      <c r="D22" s="54"/>
+      <c r="E22" s="54"/>
+      <c r="F22" s="54"/>
+      <c r="G22" s="54"/>
+      <c r="H22" s="54"/>
+      <c r="I22" s="54"/>
+      <c r="J22" s="54"/>
+      <c r="K22" s="54"/>
+      <c r="L22" s="54"/>
+      <c r="M22" s="54"/>
+      <c r="N22" s="54"/>
+      <c r="O22" s="54"/>
     </row>
     <row r="23" spans="2:15">
-      <c r="B23" s="49"/>
-      <c r="C23" s="49"/>
-      <c r="D23" s="49"/>
-      <c r="E23" s="49"/>
-      <c r="F23" s="49"/>
-      <c r="G23" s="49"/>
-      <c r="H23" s="49"/>
-      <c r="I23" s="49"/>
-      <c r="J23" s="49"/>
-      <c r="K23" s="49"/>
-      <c r="L23" s="49"/>
-      <c r="M23" s="49"/>
-      <c r="N23" s="49"/>
-      <c r="O23" s="49"/>
+      <c r="B23" s="54"/>
+      <c r="C23" s="54"/>
+      <c r="D23" s="54"/>
+      <c r="E23" s="54"/>
+      <c r="F23" s="54"/>
+      <c r="G23" s="54"/>
+      <c r="H23" s="54"/>
+      <c r="I23" s="54"/>
+      <c r="J23" s="54"/>
+      <c r="K23" s="54"/>
+      <c r="L23" s="54"/>
+      <c r="M23" s="54"/>
+      <c r="N23" s="54"/>
+      <c r="O23" s="54"/>
     </row>
     <row r="24" spans="2:15">
-      <c r="B24" s="49"/>
-      <c r="C24" s="49"/>
-      <c r="D24" s="49"/>
-      <c r="E24" s="49"/>
-      <c r="F24" s="49"/>
-      <c r="G24" s="49"/>
-      <c r="H24" s="49"/>
-      <c r="I24" s="49"/>
-      <c r="J24" s="49"/>
-      <c r="K24" s="49"/>
-      <c r="L24" s="49"/>
-      <c r="M24" s="49"/>
-      <c r="N24" s="49"/>
-      <c r="O24" s="49"/>
+      <c r="B24" s="54"/>
+      <c r="C24" s="54"/>
+      <c r="D24" s="54"/>
+      <c r="E24" s="54"/>
+      <c r="F24" s="54"/>
+      <c r="G24" s="54"/>
+      <c r="H24" s="54"/>
+      <c r="I24" s="54"/>
+      <c r="J24" s="54"/>
+      <c r="K24" s="54"/>
+      <c r="L24" s="54"/>
+      <c r="M24" s="54"/>
+      <c r="N24" s="54"/>
+      <c r="O24" s="54"/>
     </row>
     <row r="25" spans="2:15">
-      <c r="B25" s="49"/>
-      <c r="C25" s="49"/>
-      <c r="D25" s="49"/>
-      <c r="E25" s="49"/>
-      <c r="F25" s="49"/>
-      <c r="G25" s="49"/>
-      <c r="H25" s="49"/>
-      <c r="I25" s="49"/>
-      <c r="J25" s="49"/>
-      <c r="K25" s="49"/>
-      <c r="L25" s="49"/>
-      <c r="M25" s="49"/>
-      <c r="N25" s="49"/>
-      <c r="O25" s="49"/>
+      <c r="B25" s="54"/>
+      <c r="C25" s="54"/>
+      <c r="D25" s="54"/>
+      <c r="E25" s="54"/>
+      <c r="F25" s="54"/>
+      <c r="G25" s="54"/>
+      <c r="H25" s="54"/>
+      <c r="I25" s="54"/>
+      <c r="J25" s="54"/>
+      <c r="K25" s="54"/>
+      <c r="L25" s="54"/>
+      <c r="M25" s="54"/>
+      <c r="N25" s="54"/>
+      <c r="O25" s="54"/>
     </row>
     <row r="26" spans="2:15">
-      <c r="B26" s="32"/>
-      <c r="C26" s="32"/>
-      <c r="D26" s="32"/>
-      <c r="E26" s="32"/>
-      <c r="F26" s="32"/>
-      <c r="G26" s="32"/>
-      <c r="H26" s="32"/>
-      <c r="I26" s="32"/>
-      <c r="J26" s="32"/>
-      <c r="K26" s="32"/>
-      <c r="L26" s="32"/>
-      <c r="M26" s="32"/>
-      <c r="N26" s="32"/>
-      <c r="O26" s="32"/>
+      <c r="B26" s="54"/>
+      <c r="C26" s="54"/>
+      <c r="D26" s="54"/>
+      <c r="E26" s="54"/>
+      <c r="F26" s="54"/>
+      <c r="G26" s="54"/>
+      <c r="H26" s="54"/>
+      <c r="I26" s="54"/>
+      <c r="J26" s="54"/>
+      <c r="K26" s="54"/>
+      <c r="L26" s="54"/>
+      <c r="M26" s="54"/>
+      <c r="N26" s="54"/>
+      <c r="O26" s="54"/>
     </row>
     <row r="27" spans="2:15">
-      <c r="B27" s="33"/>
-      <c r="C27" s="33"/>
-      <c r="D27" s="33"/>
-      <c r="E27" s="33"/>
-      <c r="F27" s="33"/>
-      <c r="G27" s="33"/>
-      <c r="H27" s="33"/>
-      <c r="I27" s="33"/>
-      <c r="J27" s="33"/>
-      <c r="K27" s="33"/>
-      <c r="L27" s="33"/>
-      <c r="M27" s="33"/>
-      <c r="N27" s="33"/>
-      <c r="O27" s="33"/>
+      <c r="B27" s="54"/>
+      <c r="C27" s="54"/>
+      <c r="D27" s="54"/>
+      <c r="E27" s="54"/>
+      <c r="F27" s="54"/>
+      <c r="G27" s="54"/>
+      <c r="H27" s="54"/>
+      <c r="I27" s="54"/>
+      <c r="J27" s="54"/>
+      <c r="K27" s="54"/>
+      <c r="L27" s="54"/>
+      <c r="M27" s="54"/>
+      <c r="N27" s="54"/>
+      <c r="O27" s="54"/>
     </row>
     <row r="28" spans="2:15">
-      <c r="B28" s="33"/>
-      <c r="C28" s="33"/>
-      <c r="D28" s="33"/>
-      <c r="E28" s="33"/>
-      <c r="F28" s="33"/>
-      <c r="G28" s="33"/>
-      <c r="H28" s="33"/>
-      <c r="I28" s="33"/>
-      <c r="J28" s="33"/>
-      <c r="K28" s="33"/>
-      <c r="L28" s="33"/>
-      <c r="M28" s="33"/>
-      <c r="N28" s="33"/>
-      <c r="O28" s="33"/>
+      <c r="B28" s="28"/>
+      <c r="C28" s="28"/>
+      <c r="D28" s="28"/>
+      <c r="E28" s="28"/>
+      <c r="F28" s="28"/>
+      <c r="G28" s="28"/>
+      <c r="H28" s="28"/>
+      <c r="I28" s="28"/>
+      <c r="J28" s="28"/>
+      <c r="K28" s="28"/>
+      <c r="L28" s="28"/>
+      <c r="M28" s="28"/>
+      <c r="N28" s="28"/>
+      <c r="O28" s="28"/>
+    </row>
+    <row r="29" spans="2:15">
+      <c r="B29" s="42"/>
+      <c r="C29" s="42"/>
+      <c r="D29" s="42"/>
+      <c r="E29" s="42"/>
+      <c r="F29" s="42"/>
+      <c r="G29" s="42"/>
+      <c r="H29" s="42"/>
+      <c r="I29" s="42"/>
+      <c r="J29" s="42"/>
+      <c r="K29" s="42"/>
+      <c r="L29" s="42"/>
+      <c r="M29" s="42"/>
+      <c r="N29" s="42"/>
+      <c r="O29" s="42"/>
+    </row>
+    <row r="30" spans="2:15">
+      <c r="B30" s="42"/>
+      <c r="C30" s="42"/>
+      <c r="D30" s="42"/>
+      <c r="E30" s="42"/>
+      <c r="F30" s="42"/>
+      <c r="G30" s="42"/>
+      <c r="H30" s="42"/>
+      <c r="I30" s="42"/>
+      <c r="J30" s="42"/>
+      <c r="K30" s="42"/>
+      <c r="L30" s="42"/>
+      <c r="M30" s="42"/>
+      <c r="N30" s="42"/>
+      <c r="O30" s="42"/>
     </row>
   </sheetData>
-  <mergeCells count="15">
-    <mergeCell ref="B20:O25"/>
-    <mergeCell ref="B27:O27"/>
-    <mergeCell ref="B28:O28"/>
+  <mergeCells count="17">
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B22:O27"/>
+    <mergeCell ref="B29:O29"/>
+    <mergeCell ref="B30:O30"/>
     <mergeCell ref="C1:S2"/>
     <mergeCell ref="T1:U1"/>
     <mergeCell ref="T2:U2"/>
@@ -3329,10 +3335,11 @@
     <mergeCell ref="C5:H5"/>
     <mergeCell ref="C4:H4"/>
     <mergeCell ref="J5:L5"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="B12:C12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -3341,10 +3348,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91203543-4EED-4AE0-859B-F0BC4BB889AE}">
-  <dimension ref="B1:U28"/>
+  <dimension ref="B1:U30"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20:O25"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11:C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
@@ -3362,502 +3369,532 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:21" ht="27" customHeight="1">
-      <c r="C1" s="58" t="s">
+      <c r="C1" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
-      <c r="F1" s="58"/>
-      <c r="G1" s="58"/>
-      <c r="H1" s="58"/>
-      <c r="I1" s="58"/>
-      <c r="J1" s="58"/>
-      <c r="K1" s="58"/>
-      <c r="L1" s="58"/>
-      <c r="M1" s="58"/>
-      <c r="N1" s="58"/>
-      <c r="O1" s="58"/>
-      <c r="P1" s="58"/>
-      <c r="Q1" s="58"/>
-      <c r="R1" s="58"/>
-      <c r="S1" s="58"/>
-      <c r="T1" s="55" t="s">
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
+      <c r="I1" s="40"/>
+      <c r="J1" s="40"/>
+      <c r="K1" s="40"/>
+      <c r="L1" s="40"/>
+      <c r="M1" s="40"/>
+      <c r="N1" s="40"/>
+      <c r="O1" s="40"/>
+      <c r="P1" s="40"/>
+      <c r="Q1" s="40"/>
+      <c r="R1" s="40"/>
+      <c r="S1" s="40"/>
+      <c r="T1" s="37" t="s">
         <v>63</v>
       </c>
-      <c r="U1" s="56"/>
+      <c r="U1" s="38"/>
     </row>
     <row r="2" spans="2:21" ht="15" thickBot="1">
-      <c r="C2" s="59"/>
-      <c r="D2" s="59"/>
-      <c r="E2" s="58"/>
-      <c r="F2" s="58"/>
-      <c r="G2" s="58"/>
-      <c r="H2" s="58"/>
-      <c r="I2" s="58"/>
-      <c r="J2" s="58"/>
-      <c r="K2" s="58"/>
-      <c r="L2" s="58"/>
-      <c r="M2" s="58"/>
-      <c r="N2" s="58"/>
-      <c r="O2" s="58"/>
-      <c r="P2" s="58"/>
-      <c r="Q2" s="58"/>
-      <c r="R2" s="58"/>
-      <c r="S2" s="58"/>
-      <c r="T2" s="57" t="s">
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="40"/>
+      <c r="K2" s="40"/>
+      <c r="L2" s="40"/>
+      <c r="M2" s="40"/>
+      <c r="N2" s="40"/>
+      <c r="O2" s="40"/>
+      <c r="P2" s="40"/>
+      <c r="Q2" s="40"/>
+      <c r="R2" s="40"/>
+      <c r="S2" s="40"/>
+      <c r="T2" s="39" t="s">
         <v>64</v>
       </c>
-      <c r="U2" s="57"/>
+      <c r="U2" s="39"/>
     </row>
     <row r="3" spans="2:21" ht="15" thickBot="1">
-      <c r="C3" s="28" t="s">
+      <c r="C3" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="28" t="s">
+      <c r="D3" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
-      <c r="K3" s="25"/>
-      <c r="L3" s="25"/>
-      <c r="M3" s="25"/>
-      <c r="N3" s="25"/>
-      <c r="O3" s="25"/>
-      <c r="P3" s="25"/>
-      <c r="Q3" s="25"/>
-      <c r="R3" s="25"/>
-      <c r="S3" s="25"/>
-      <c r="T3" s="24"/>
-      <c r="U3" s="24"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="21"/>
+      <c r="K3" s="21"/>
+      <c r="L3" s="21"/>
+      <c r="M3" s="21"/>
+      <c r="N3" s="21"/>
+      <c r="O3" s="21"/>
+      <c r="P3" s="21"/>
+      <c r="Q3" s="21"/>
+      <c r="R3" s="21"/>
+      <c r="S3" s="21"/>
+      <c r="T3" s="20"/>
+      <c r="U3" s="20"/>
     </row>
     <row r="4" spans="2:21" ht="29.4" customHeight="1" thickBot="1">
-      <c r="C4" s="34" t="s">
+      <c r="C4" s="29" t="s">
         <v>105</v>
       </c>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="35"/>
-      <c r="H4" s="36"/>
-      <c r="I4" s="51" t="s">
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="33" t="s">
         <v>68</v>
       </c>
-      <c r="J4" s="60" t="s">
+      <c r="J4" s="55" t="s">
         <v>12</v>
       </c>
-      <c r="K4" s="61"/>
-      <c r="L4" s="62"/>
+      <c r="K4" s="56"/>
+      <c r="L4" s="57"/>
     </row>
     <row r="5" spans="2:21" ht="15" thickBot="1">
-      <c r="C5" s="34" t="s">
+      <c r="C5" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="35"/>
-      <c r="G5" s="35"/>
-      <c r="H5" s="36"/>
-      <c r="I5" s="53"/>
-      <c r="J5" s="34" t="s">
+      <c r="D5" s="30"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="30"/>
+      <c r="H5" s="31"/>
+      <c r="I5" s="35"/>
+      <c r="J5" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="K5" s="35"/>
-      <c r="L5" s="36"/>
+      <c r="K5" s="30"/>
+      <c r="L5" s="31"/>
     </row>
     <row r="6" spans="2:21" ht="58.2" thickBot="1">
-      <c r="B6" s="4"/>
-      <c r="C6" s="10" t="s">
+      <c r="B6" s="2"/>
+      <c r="C6" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="D6" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="E6" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="F6" s="14" t="s">
+      <c r="F6" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="G6" s="14" t="s">
+      <c r="G6" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="H6" s="11" t="s">
+      <c r="H6" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="I6" s="54"/>
-      <c r="J6" s="14" t="s">
+      <c r="I6" s="36"/>
+      <c r="J6" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="K6" s="14" t="s">
+      <c r="K6" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="L6" s="14" t="s">
+      <c r="L6" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="M6" s="14" t="s">
+      <c r="M6" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="N6" s="14" t="s">
+      <c r="N6" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="O6" s="14" t="s">
+      <c r="O6" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="P6" s="14" t="s">
+      <c r="P6" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="Q6" s="14" t="s">
+      <c r="Q6" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="R6" s="14" t="s">
+      <c r="R6" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="S6" s="14" t="s">
+      <c r="S6" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="T6" s="14" t="s">
+      <c r="T6" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="U6" s="14" t="s">
+      <c r="U6" s="12" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="7" spans="2:21" ht="15" thickBot="1">
-      <c r="B7" s="23" t="s">
+      <c r="B7" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="20" t="s">
+      <c r="C7" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="D7" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="E7" s="20" t="s">
+      <c r="E7" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="F7" s="20" t="s">
+      <c r="F7" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="G7" s="13" t="s">
+      <c r="G7" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="H7" s="13" t="s">
+      <c r="H7" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="I7" s="13" t="s">
+      <c r="I7" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="J7" s="20" t="s">
+      <c r="J7" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="K7" s="13" t="s">
+      <c r="K7" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="L7" s="20" t="s">
+      <c r="L7" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="M7" s="20" t="s">
+      <c r="M7" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="N7" s="20" t="s">
+      <c r="N7" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="O7" s="20" t="s">
+      <c r="O7" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="P7" s="13" t="s">
+      <c r="P7" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="Q7" s="19" t="s">
+      <c r="Q7" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="R7" s="13" t="s">
+      <c r="R7" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="S7" s="13" t="s">
+      <c r="S7" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="T7" s="20" t="s">
+      <c r="T7" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="U7" s="13" t="s">
+      <c r="U7" s="11" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="8" spans="2:21" ht="15" thickBot="1">
-      <c r="B8" s="8"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
     </row>
     <row r="9" spans="2:21" ht="15" thickBot="1">
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="D9" s="12"/>
-      <c r="E9" s="21" t="s">
+      <c r="D9" s="10"/>
+      <c r="E9" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12" t="s">
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="I9" s="12" t="s">
+      <c r="I9" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="J9" s="21" t="s">
+      <c r="J9" s="17" t="s">
         <v>97</v>
       </c>
-      <c r="K9" s="12"/>
-      <c r="L9" s="21" t="s">
+      <c r="K9" s="10"/>
+      <c r="L9" s="17" t="s">
         <v>113</v>
       </c>
-      <c r="M9" s="12"/>
-      <c r="N9" s="12"/>
-      <c r="O9" s="12"/>
-      <c r="P9" s="12"/>
-      <c r="Q9" s="12"/>
-      <c r="R9" s="12"/>
-      <c r="S9" s="12" t="s">
+      <c r="M9" s="10"/>
+      <c r="N9" s="10"/>
+      <c r="O9" s="10"/>
+      <c r="P9" s="10"/>
+      <c r="Q9" s="10"/>
+      <c r="R9" s="10"/>
+      <c r="S9" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="T9" s="21" t="s">
+      <c r="T9" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="U9" s="12" t="s">
+      <c r="U9" s="10" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="10" spans="2:21">
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-    </row>
-    <row r="11" spans="2:21" ht="15" thickBot="1">
-      <c r="B11" s="1"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
-    </row>
-    <row r="12" spans="2:21" ht="16.8" customHeight="1" thickBot="1">
-      <c r="B12" s="45" t="s">
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+    </row>
+    <row r="11" spans="2:21">
+      <c r="B11" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+    </row>
+    <row r="12" spans="2:21" ht="24.6" customHeight="1">
+      <c r="B12" s="32" t="s">
+        <v>107</v>
+      </c>
+      <c r="C12" s="32"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+    </row>
+    <row r="13" spans="2:21" ht="24.6" customHeight="1" thickBot="1">
+      <c r="B13" s="53" t="s">
+        <v>108</v>
+      </c>
+      <c r="C13" s="53"/>
+      <c r="D13" s="59"/>
+      <c r="E13" s="60"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+    </row>
+    <row r="14" spans="2:21" ht="16.8" customHeight="1" thickBot="1">
+      <c r="B14" s="50" t="s">
         <v>54</v>
       </c>
-      <c r="C12" s="46"/>
-      <c r="D12" s="47"/>
-      <c r="E12" s="22" t="s">
+      <c r="C14" s="51"/>
+      <c r="D14" s="52"/>
+      <c r="E14" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-    </row>
-    <row r="13" spans="2:21">
-      <c r="B13" s="3"/>
-      <c r="C13" s="43"/>
-      <c r="D13" s="44"/>
-    </row>
-    <row r="14" spans="2:21" ht="15" thickBot="1">
-      <c r="B14" s="1"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="2"/>
-    </row>
-    <row r="15" spans="2:21" ht="39.6" customHeight="1" thickBot="1">
-      <c r="B15" s="37" t="s">
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+    </row>
+    <row r="15" spans="2:21" ht="15" thickBot="1">
+      <c r="B15" s="1"/>
+      <c r="C15" s="49"/>
+      <c r="D15" s="61"/>
+      <c r="E15" s="62"/>
+    </row>
+    <row r="16" spans="2:21" ht="29.4" thickBot="1">
+      <c r="B16" s="58"/>
+      <c r="C16" s="59"/>
+      <c r="D16" s="59"/>
+      <c r="E16" s="12" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="17" spans="2:15" ht="39.6" customHeight="1" thickBot="1">
+      <c r="B17" s="43" t="s">
         <v>58</v>
       </c>
-      <c r="C15" s="38"/>
-      <c r="D15" s="39"/>
-      <c r="E15" s="18" t="s">
+      <c r="C17" s="44"/>
+      <c r="D17" s="45"/>
+      <c r="E17" s="27" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="16" spans="2:21" ht="43.8" customHeight="1" thickBot="1">
-      <c r="B16" s="40" t="s">
+    <row r="18" spans="2:15" ht="43.8" customHeight="1" thickBot="1">
+      <c r="B18" s="46" t="s">
         <v>59</v>
       </c>
-      <c r="C16" s="41"/>
-      <c r="D16" s="42"/>
-      <c r="E16" s="18" t="s">
+      <c r="C18" s="47"/>
+      <c r="D18" s="48"/>
+      <c r="E18" s="27" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="17" spans="2:15">
-      <c r="B17" s="3"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
-    </row>
-    <row r="18" spans="2:15">
-      <c r="B18" s="3"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="17"/>
-    </row>
     <row r="19" spans="2:15">
-      <c r="B19" s="16" t="s">
+      <c r="B19" s="1"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+    </row>
+    <row r="20" spans="2:15">
+      <c r="B20" s="1"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
+    </row>
+    <row r="21" spans="2:15">
+      <c r="B21" s="13" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="20" spans="2:15">
-      <c r="B20" s="49" t="s">
+    <row r="22" spans="2:15">
+      <c r="B22" s="54" t="s">
         <v>60</v>
       </c>
-      <c r="C20" s="49"/>
-      <c r="D20" s="49"/>
-      <c r="E20" s="49"/>
-      <c r="F20" s="49"/>
-      <c r="G20" s="49"/>
-      <c r="H20" s="49"/>
-      <c r="I20" s="49"/>
-      <c r="J20" s="49"/>
-      <c r="K20" s="49"/>
-      <c r="L20" s="49"/>
-      <c r="M20" s="49"/>
-      <c r="N20" s="49"/>
-      <c r="O20" s="49"/>
-    </row>
-    <row r="21" spans="2:15">
-      <c r="B21" s="49"/>
-      <c r="C21" s="49"/>
-      <c r="D21" s="49"/>
-      <c r="E21" s="49"/>
-      <c r="F21" s="49"/>
-      <c r="G21" s="49"/>
-      <c r="H21" s="49"/>
-      <c r="I21" s="49"/>
-      <c r="J21" s="49"/>
-      <c r="K21" s="49"/>
-      <c r="L21" s="49"/>
-      <c r="M21" s="49"/>
-      <c r="N21" s="49"/>
-      <c r="O21" s="49"/>
-    </row>
-    <row r="22" spans="2:15">
-      <c r="B22" s="49"/>
-      <c r="C22" s="49"/>
-      <c r="D22" s="49"/>
-      <c r="E22" s="49"/>
-      <c r="F22" s="49"/>
-      <c r="G22" s="49"/>
-      <c r="H22" s="49"/>
-      <c r="I22" s="49"/>
-      <c r="J22" s="49"/>
-      <c r="K22" s="49"/>
-      <c r="L22" s="49"/>
-      <c r="M22" s="49"/>
-      <c r="N22" s="49"/>
-      <c r="O22" s="49"/>
+      <c r="C22" s="54"/>
+      <c r="D22" s="54"/>
+      <c r="E22" s="54"/>
+      <c r="F22" s="54"/>
+      <c r="G22" s="54"/>
+      <c r="H22" s="54"/>
+      <c r="I22" s="54"/>
+      <c r="J22" s="54"/>
+      <c r="K22" s="54"/>
+      <c r="L22" s="54"/>
+      <c r="M22" s="54"/>
+      <c r="N22" s="54"/>
+      <c r="O22" s="54"/>
     </row>
     <row r="23" spans="2:15">
-      <c r="B23" s="49"/>
-      <c r="C23" s="49"/>
-      <c r="D23" s="49"/>
-      <c r="E23" s="49"/>
-      <c r="F23" s="49"/>
-      <c r="G23" s="49"/>
-      <c r="H23" s="49"/>
-      <c r="I23" s="49"/>
-      <c r="J23" s="49"/>
-      <c r="K23" s="49"/>
-      <c r="L23" s="49"/>
-      <c r="M23" s="49"/>
-      <c r="N23" s="49"/>
-      <c r="O23" s="49"/>
+      <c r="B23" s="54"/>
+      <c r="C23" s="54"/>
+      <c r="D23" s="54"/>
+      <c r="E23" s="54"/>
+      <c r="F23" s="54"/>
+      <c r="G23" s="54"/>
+      <c r="H23" s="54"/>
+      <c r="I23" s="54"/>
+      <c r="J23" s="54"/>
+      <c r="K23" s="54"/>
+      <c r="L23" s="54"/>
+      <c r="M23" s="54"/>
+      <c r="N23" s="54"/>
+      <c r="O23" s="54"/>
     </row>
     <row r="24" spans="2:15">
-      <c r="B24" s="49"/>
-      <c r="C24" s="49"/>
-      <c r="D24" s="49"/>
-      <c r="E24" s="49"/>
-      <c r="F24" s="49"/>
-      <c r="G24" s="49"/>
-      <c r="H24" s="49"/>
-      <c r="I24" s="49"/>
-      <c r="J24" s="49"/>
-      <c r="K24" s="49"/>
-      <c r="L24" s="49"/>
-      <c r="M24" s="49"/>
-      <c r="N24" s="49"/>
-      <c r="O24" s="49"/>
+      <c r="B24" s="54"/>
+      <c r="C24" s="54"/>
+      <c r="D24" s="54"/>
+      <c r="E24" s="54"/>
+      <c r="F24" s="54"/>
+      <c r="G24" s="54"/>
+      <c r="H24" s="54"/>
+      <c r="I24" s="54"/>
+      <c r="J24" s="54"/>
+      <c r="K24" s="54"/>
+      <c r="L24" s="54"/>
+      <c r="M24" s="54"/>
+      <c r="N24" s="54"/>
+      <c r="O24" s="54"/>
     </row>
     <row r="25" spans="2:15">
-      <c r="B25" s="49"/>
-      <c r="C25" s="49"/>
-      <c r="D25" s="49"/>
-      <c r="E25" s="49"/>
-      <c r="F25" s="49"/>
-      <c r="G25" s="49"/>
-      <c r="H25" s="49"/>
-      <c r="I25" s="49"/>
-      <c r="J25" s="49"/>
-      <c r="K25" s="49"/>
-      <c r="L25" s="49"/>
-      <c r="M25" s="49"/>
-      <c r="N25" s="49"/>
-      <c r="O25" s="49"/>
+      <c r="B25" s="54"/>
+      <c r="C25" s="54"/>
+      <c r="D25" s="54"/>
+      <c r="E25" s="54"/>
+      <c r="F25" s="54"/>
+      <c r="G25" s="54"/>
+      <c r="H25" s="54"/>
+      <c r="I25" s="54"/>
+      <c r="J25" s="54"/>
+      <c r="K25" s="54"/>
+      <c r="L25" s="54"/>
+      <c r="M25" s="54"/>
+      <c r="N25" s="54"/>
+      <c r="O25" s="54"/>
     </row>
     <row r="26" spans="2:15">
-      <c r="B26" s="32"/>
-      <c r="C26" s="32"/>
-      <c r="D26" s="32"/>
-      <c r="E26" s="32"/>
-      <c r="F26" s="32"/>
-      <c r="G26" s="32"/>
-      <c r="H26" s="32"/>
-      <c r="I26" s="32"/>
-      <c r="J26" s="32"/>
-      <c r="K26" s="32"/>
-      <c r="L26" s="32"/>
-      <c r="M26" s="32"/>
-      <c r="N26" s="32"/>
-      <c r="O26" s="32"/>
+      <c r="B26" s="54"/>
+      <c r="C26" s="54"/>
+      <c r="D26" s="54"/>
+      <c r="E26" s="54"/>
+      <c r="F26" s="54"/>
+      <c r="G26" s="54"/>
+      <c r="H26" s="54"/>
+      <c r="I26" s="54"/>
+      <c r="J26" s="54"/>
+      <c r="K26" s="54"/>
+      <c r="L26" s="54"/>
+      <c r="M26" s="54"/>
+      <c r="N26" s="54"/>
+      <c r="O26" s="54"/>
     </row>
     <row r="27" spans="2:15">
-      <c r="B27" s="33"/>
-      <c r="C27" s="33"/>
-      <c r="D27" s="33"/>
-      <c r="E27" s="33"/>
-      <c r="F27" s="33"/>
-      <c r="G27" s="33"/>
-      <c r="H27" s="33"/>
-      <c r="I27" s="33"/>
-      <c r="J27" s="33"/>
-      <c r="K27" s="33"/>
-      <c r="L27" s="33"/>
-      <c r="M27" s="33"/>
-      <c r="N27" s="33"/>
-      <c r="O27" s="33"/>
+      <c r="B27" s="54"/>
+      <c r="C27" s="54"/>
+      <c r="D27" s="54"/>
+      <c r="E27" s="54"/>
+      <c r="F27" s="54"/>
+      <c r="G27" s="54"/>
+      <c r="H27" s="54"/>
+      <c r="I27" s="54"/>
+      <c r="J27" s="54"/>
+      <c r="K27" s="54"/>
+      <c r="L27" s="54"/>
+      <c r="M27" s="54"/>
+      <c r="N27" s="54"/>
+      <c r="O27" s="54"/>
     </row>
     <row r="28" spans="2:15">
-      <c r="B28" s="33"/>
-      <c r="C28" s="33"/>
-      <c r="D28" s="33"/>
-      <c r="E28" s="33"/>
-      <c r="F28" s="33"/>
-      <c r="G28" s="33"/>
-      <c r="H28" s="33"/>
-      <c r="I28" s="33"/>
-      <c r="J28" s="33"/>
-      <c r="K28" s="33"/>
-      <c r="L28" s="33"/>
-      <c r="M28" s="33"/>
-      <c r="N28" s="33"/>
-      <c r="O28" s="33"/>
+      <c r="B28" s="28"/>
+      <c r="C28" s="28"/>
+      <c r="D28" s="28"/>
+      <c r="E28" s="28"/>
+      <c r="F28" s="28"/>
+      <c r="G28" s="28"/>
+      <c r="H28" s="28"/>
+      <c r="I28" s="28"/>
+      <c r="J28" s="28"/>
+      <c r="K28" s="28"/>
+      <c r="L28" s="28"/>
+      <c r="M28" s="28"/>
+      <c r="N28" s="28"/>
+      <c r="O28" s="28"/>
+    </row>
+    <row r="29" spans="2:15">
+      <c r="B29" s="42"/>
+      <c r="C29" s="42"/>
+      <c r="D29" s="42"/>
+      <c r="E29" s="42"/>
+      <c r="F29" s="42"/>
+      <c r="G29" s="42"/>
+      <c r="H29" s="42"/>
+      <c r="I29" s="42"/>
+      <c r="J29" s="42"/>
+      <c r="K29" s="42"/>
+      <c r="L29" s="42"/>
+      <c r="M29" s="42"/>
+      <c r="N29" s="42"/>
+      <c r="O29" s="42"/>
+    </row>
+    <row r="30" spans="2:15">
+      <c r="B30" s="42"/>
+      <c r="C30" s="42"/>
+      <c r="D30" s="42"/>
+      <c r="E30" s="42"/>
+      <c r="F30" s="42"/>
+      <c r="G30" s="42"/>
+      <c r="H30" s="42"/>
+      <c r="I30" s="42"/>
+      <c r="J30" s="42"/>
+      <c r="K30" s="42"/>
+      <c r="L30" s="42"/>
+      <c r="M30" s="42"/>
+      <c r="N30" s="42"/>
+      <c r="O30" s="42"/>
     </row>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="17">
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B30:O30"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="B22:O27"/>
+    <mergeCell ref="B29:O29"/>
     <mergeCell ref="C1:S2"/>
     <mergeCell ref="T1:U1"/>
     <mergeCell ref="T2:U2"/>
@@ -3866,13 +3903,6 @@
     <mergeCell ref="J4:L4"/>
     <mergeCell ref="C5:H5"/>
     <mergeCell ref="J5:L5"/>
-    <mergeCell ref="B28:O28"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="B20:O25"/>
-    <mergeCell ref="B27:O27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -3881,10 +3911,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FBF716D-FD41-4431-A8BB-5A81BFB0390B}">
-  <dimension ref="B1:U28"/>
+  <dimension ref="B1:U30"/>
   <sheetViews>
     <sheetView topLeftCell="B7" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20:O25"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
@@ -3902,509 +3932,525 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:21" ht="27" customHeight="1">
-      <c r="C1" s="58" t="s">
+      <c r="C1" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
-      <c r="F1" s="58"/>
-      <c r="G1" s="58"/>
-      <c r="H1" s="58"/>
-      <c r="I1" s="58"/>
-      <c r="J1" s="58"/>
-      <c r="K1" s="58"/>
-      <c r="L1" s="58"/>
-      <c r="M1" s="58"/>
-      <c r="N1" s="58"/>
-      <c r="O1" s="58"/>
-      <c r="P1" s="58"/>
-      <c r="Q1" s="58"/>
-      <c r="R1" s="58"/>
-      <c r="S1" s="58"/>
-      <c r="T1" s="55" t="s">
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
+      <c r="I1" s="40"/>
+      <c r="J1" s="40"/>
+      <c r="K1" s="40"/>
+      <c r="L1" s="40"/>
+      <c r="M1" s="40"/>
+      <c r="N1" s="40"/>
+      <c r="O1" s="40"/>
+      <c r="P1" s="40"/>
+      <c r="Q1" s="40"/>
+      <c r="R1" s="40"/>
+      <c r="S1" s="40"/>
+      <c r="T1" s="37" t="s">
         <v>63</v>
       </c>
-      <c r="U1" s="56"/>
+      <c r="U1" s="38"/>
     </row>
     <row r="2" spans="2:21" ht="15" thickBot="1">
-      <c r="C2" s="59"/>
-      <c r="D2" s="59"/>
-      <c r="E2" s="58"/>
-      <c r="F2" s="58"/>
-      <c r="G2" s="58"/>
-      <c r="H2" s="58"/>
-      <c r="I2" s="58"/>
-      <c r="J2" s="58"/>
-      <c r="K2" s="58"/>
-      <c r="L2" s="58"/>
-      <c r="M2" s="58"/>
-      <c r="N2" s="58"/>
-      <c r="O2" s="58"/>
-      <c r="P2" s="58"/>
-      <c r="Q2" s="58"/>
-      <c r="R2" s="58"/>
-      <c r="S2" s="58"/>
-      <c r="T2" s="57" t="s">
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="40"/>
+      <c r="K2" s="40"/>
+      <c r="L2" s="40"/>
+      <c r="M2" s="40"/>
+      <c r="N2" s="40"/>
+      <c r="O2" s="40"/>
+      <c r="P2" s="40"/>
+      <c r="Q2" s="40"/>
+      <c r="R2" s="40"/>
+      <c r="S2" s="40"/>
+      <c r="T2" s="39" t="s">
         <v>64</v>
       </c>
-      <c r="U2" s="57"/>
+      <c r="U2" s="39"/>
     </row>
     <row r="3" spans="2:21" ht="15" thickBot="1">
-      <c r="C3" s="28" t="s">
+      <c r="C3" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="28" t="s">
+      <c r="D3" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
-      <c r="K3" s="25"/>
-      <c r="L3" s="25"/>
-      <c r="M3" s="25"/>
-      <c r="N3" s="25"/>
-      <c r="O3" s="25"/>
-      <c r="P3" s="25"/>
-      <c r="Q3" s="25"/>
-      <c r="R3" s="25"/>
-      <c r="S3" s="25"/>
-      <c r="T3" s="24"/>
-      <c r="U3" s="24"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="21"/>
+      <c r="K3" s="21"/>
+      <c r="L3" s="21"/>
+      <c r="M3" s="21"/>
+      <c r="N3" s="21"/>
+      <c r="O3" s="21"/>
+      <c r="P3" s="21"/>
+      <c r="Q3" s="21"/>
+      <c r="R3" s="21"/>
+      <c r="S3" s="21"/>
+      <c r="T3" s="20"/>
+      <c r="U3" s="20"/>
     </row>
     <row r="4" spans="2:21" ht="29.4" customHeight="1" thickBot="1">
-      <c r="C4" s="34" t="s">
+      <c r="C4" s="29" t="s">
         <v>105</v>
       </c>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="35"/>
-      <c r="H4" s="36"/>
-      <c r="I4" s="51" t="s">
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="33" t="s">
         <v>68</v>
       </c>
-      <c r="J4" s="60" t="s">
+      <c r="J4" s="55" t="s">
         <v>12</v>
       </c>
-      <c r="K4" s="61"/>
-      <c r="L4" s="62"/>
+      <c r="K4" s="56"/>
+      <c r="L4" s="57"/>
     </row>
     <row r="5" spans="2:21" ht="15" thickBot="1">
-      <c r="C5" s="34" t="s">
+      <c r="C5" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="35"/>
-      <c r="G5" s="35"/>
-      <c r="H5" s="36"/>
-      <c r="I5" s="53"/>
-      <c r="J5" s="34" t="s">
+      <c r="D5" s="30"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="30"/>
+      <c r="H5" s="31"/>
+      <c r="I5" s="35"/>
+      <c r="J5" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="K5" s="35"/>
-      <c r="L5" s="36"/>
+      <c r="K5" s="30"/>
+      <c r="L5" s="31"/>
     </row>
     <row r="6" spans="2:21" ht="58.2" thickBot="1">
-      <c r="B6" s="4"/>
-      <c r="C6" s="10" t="s">
+      <c r="B6" s="2"/>
+      <c r="C6" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="D6" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="E6" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="F6" s="14" t="s">
+      <c r="F6" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="G6" s="14" t="s">
+      <c r="G6" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="H6" s="11" t="s">
+      <c r="H6" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="I6" s="54"/>
-      <c r="J6" s="14" t="s">
+      <c r="I6" s="36"/>
+      <c r="J6" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="K6" s="14" t="s">
+      <c r="K6" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="L6" s="14" t="s">
+      <c r="L6" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="M6" s="14" t="s">
+      <c r="M6" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="N6" s="14" t="s">
+      <c r="N6" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="O6" s="14" t="s">
+      <c r="O6" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="P6" s="14" t="s">
+      <c r="P6" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="Q6" s="14" t="s">
+      <c r="Q6" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="R6" s="14" t="s">
+      <c r="R6" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="S6" s="14" t="s">
+      <c r="S6" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="T6" s="14" t="s">
+      <c r="T6" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="U6" s="14" t="s">
+      <c r="U6" s="12" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="7" spans="2:21" ht="15" thickBot="1">
-      <c r="B7" s="23" t="s">
+      <c r="B7" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="20" t="s">
+      <c r="C7" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="D7" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="E7" s="20" t="s">
+      <c r="E7" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="F7" s="20" t="s">
+      <c r="F7" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="G7" s="13" t="s">
+      <c r="G7" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="H7" s="13" t="s">
+      <c r="H7" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="I7" s="13" t="s">
+      <c r="I7" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="J7" s="20" t="s">
+      <c r="J7" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="K7" s="13" t="s">
+      <c r="K7" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="L7" s="20" t="s">
+      <c r="L7" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="M7" s="20" t="s">
+      <c r="M7" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="N7" s="20" t="s">
+      <c r="N7" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="O7" s="20" t="s">
+      <c r="O7" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="P7" s="13" t="s">
+      <c r="P7" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="Q7" s="19" t="s">
+      <c r="Q7" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="R7" s="13" t="s">
+      <c r="R7" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="S7" s="13" t="s">
+      <c r="S7" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="T7" s="20" t="s">
+      <c r="T7" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="U7" s="13" t="s">
+      <c r="U7" s="11" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="8" spans="2:21" ht="15" thickBot="1">
-      <c r="B8" s="8"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
     </row>
     <row r="9" spans="2:21" ht="15" thickBot="1">
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="D9" s="12"/>
-      <c r="E9" s="21" t="s">
+      <c r="D9" s="10"/>
+      <c r="E9" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12" t="s">
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="I9" s="12" t="s">
+      <c r="I9" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="J9" s="21" t="s">
+      <c r="J9" s="17" t="s">
         <v>98</v>
       </c>
-      <c r="K9" s="12"/>
-      <c r="L9" s="21" t="s">
+      <c r="K9" s="10"/>
+      <c r="L9" s="17" t="s">
         <v>118</v>
       </c>
-      <c r="M9" s="12"/>
-      <c r="N9" s="12"/>
-      <c r="O9" s="12"/>
-      <c r="P9" s="12"/>
-      <c r="Q9" s="12"/>
-      <c r="R9" s="12"/>
-      <c r="S9" s="12" t="s">
+      <c r="M9" s="10"/>
+      <c r="N9" s="10"/>
+      <c r="O9" s="10"/>
+      <c r="P9" s="10"/>
+      <c r="Q9" s="10"/>
+      <c r="R9" s="10"/>
+      <c r="S9" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="T9" s="21" t="s">
+      <c r="T9" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="U9" s="12" t="s">
+      <c r="U9" s="10" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="10" spans="2:21">
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-    </row>
-    <row r="11" spans="2:21" ht="15" thickBot="1">
-      <c r="B11" s="1"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
-    </row>
-    <row r="12" spans="2:21" ht="16.8" customHeight="1" thickBot="1">
-      <c r="B12" s="45" t="s">
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+    </row>
+    <row r="11" spans="2:21">
+      <c r="B11" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+    </row>
+    <row r="12" spans="2:21" ht="22.8" customHeight="1">
+      <c r="B12" s="32" t="s">
+        <v>107</v>
+      </c>
+      <c r="C12" s="32"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+    </row>
+    <row r="13" spans="2:21" ht="31.2" customHeight="1" thickBot="1">
+      <c r="B13" s="53" t="s">
+        <v>108</v>
+      </c>
+      <c r="C13" s="53"/>
+      <c r="D13" s="59"/>
+      <c r="E13" s="60"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+    </row>
+    <row r="14" spans="2:21" ht="16.8" customHeight="1" thickBot="1">
+      <c r="B14" s="50" t="s">
         <v>54</v>
       </c>
-      <c r="C12" s="46"/>
-      <c r="D12" s="47"/>
-      <c r="E12" s="22" t="s">
+      <c r="C14" s="51"/>
+      <c r="D14" s="52"/>
+      <c r="E14" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-    </row>
-    <row r="13" spans="2:21">
-      <c r="B13" s="3"/>
-      <c r="C13" s="43"/>
-      <c r="D13" s="44"/>
-    </row>
-    <row r="14" spans="2:21" ht="15" thickBot="1">
-      <c r="B14" s="1"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="2"/>
-    </row>
-    <row r="15" spans="2:21" ht="39.6" customHeight="1" thickBot="1">
-      <c r="B15" s="37" t="s">
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+    </row>
+    <row r="15" spans="2:21" ht="15" thickBot="1">
+      <c r="B15" s="1"/>
+      <c r="C15" s="49"/>
+      <c r="D15" s="61"/>
+      <c r="E15" s="62"/>
+    </row>
+    <row r="16" spans="2:21" ht="29.4" thickBot="1">
+      <c r="B16" s="58"/>
+      <c r="C16" s="59"/>
+      <c r="D16" s="59"/>
+      <c r="E16" s="12" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="17" spans="2:15" ht="39.6" customHeight="1" thickBot="1">
+      <c r="B17" s="43" t="s">
         <v>58</v>
       </c>
-      <c r="C15" s="38"/>
-      <c r="D15" s="39"/>
-      <c r="E15" s="18" t="s">
+      <c r="C17" s="44"/>
+      <c r="D17" s="45"/>
+      <c r="E17" s="27" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="16" spans="2:21" ht="43.8" customHeight="1" thickBot="1">
-      <c r="B16" s="40" t="s">
+    <row r="18" spans="2:15" ht="43.8" customHeight="1" thickBot="1">
+      <c r="B18" s="46" t="s">
         <v>59</v>
       </c>
-      <c r="C16" s="41"/>
-      <c r="D16" s="42"/>
-      <c r="E16" s="18" t="s">
+      <c r="C18" s="47"/>
+      <c r="D18" s="48"/>
+      <c r="E18" s="27" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="17" spans="2:15">
-      <c r="B17" s="3"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
-    </row>
-    <row r="18" spans="2:15">
-      <c r="B18" s="3"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="17"/>
-    </row>
     <row r="19" spans="2:15">
-      <c r="B19" s="16" t="s">
+      <c r="B19" s="1"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+    </row>
+    <row r="20" spans="2:15">
+      <c r="B20" s="1"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
+    </row>
+    <row r="21" spans="2:15">
+      <c r="B21" s="13" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="20" spans="2:15">
-      <c r="B20" s="49" t="s">
+    <row r="22" spans="2:15">
+      <c r="B22" s="54" t="s">
         <v>60</v>
       </c>
-      <c r="C20" s="49"/>
-      <c r="D20" s="49"/>
-      <c r="E20" s="49"/>
-      <c r="F20" s="49"/>
-      <c r="G20" s="49"/>
-      <c r="H20" s="49"/>
-      <c r="I20" s="49"/>
-      <c r="J20" s="49"/>
-      <c r="K20" s="49"/>
-      <c r="L20" s="49"/>
-      <c r="M20" s="49"/>
-      <c r="N20" s="49"/>
-      <c r="O20" s="49"/>
-    </row>
-    <row r="21" spans="2:15">
-      <c r="B21" s="49"/>
-      <c r="C21" s="49"/>
-      <c r="D21" s="49"/>
-      <c r="E21" s="49"/>
-      <c r="F21" s="49"/>
-      <c r="G21" s="49"/>
-      <c r="H21" s="49"/>
-      <c r="I21" s="49"/>
-      <c r="J21" s="49"/>
-      <c r="K21" s="49"/>
-      <c r="L21" s="49"/>
-      <c r="M21" s="49"/>
-      <c r="N21" s="49"/>
-      <c r="O21" s="49"/>
-    </row>
-    <row r="22" spans="2:15">
-      <c r="B22" s="49"/>
-      <c r="C22" s="49"/>
-      <c r="D22" s="49"/>
-      <c r="E22" s="49"/>
-      <c r="F22" s="49"/>
-      <c r="G22" s="49"/>
-      <c r="H22" s="49"/>
-      <c r="I22" s="49"/>
-      <c r="J22" s="49"/>
-      <c r="K22" s="49"/>
-      <c r="L22" s="49"/>
-      <c r="M22" s="49"/>
-      <c r="N22" s="49"/>
-      <c r="O22" s="49"/>
+      <c r="C22" s="54"/>
+      <c r="D22" s="54"/>
+      <c r="E22" s="54"/>
+      <c r="F22" s="54"/>
+      <c r="G22" s="54"/>
+      <c r="H22" s="54"/>
+      <c r="I22" s="54"/>
+      <c r="J22" s="54"/>
+      <c r="K22" s="54"/>
+      <c r="L22" s="54"/>
+      <c r="M22" s="54"/>
+      <c r="N22" s="54"/>
+      <c r="O22" s="54"/>
     </row>
     <row r="23" spans="2:15">
-      <c r="B23" s="49"/>
-      <c r="C23" s="49"/>
-      <c r="D23" s="49"/>
-      <c r="E23" s="49"/>
-      <c r="F23" s="49"/>
-      <c r="G23" s="49"/>
-      <c r="H23" s="49"/>
-      <c r="I23" s="49"/>
-      <c r="J23" s="49"/>
-      <c r="K23" s="49"/>
-      <c r="L23" s="49"/>
-      <c r="M23" s="49"/>
-      <c r="N23" s="49"/>
-      <c r="O23" s="49"/>
+      <c r="B23" s="54"/>
+      <c r="C23" s="54"/>
+      <c r="D23" s="54"/>
+      <c r="E23" s="54"/>
+      <c r="F23" s="54"/>
+      <c r="G23" s="54"/>
+      <c r="H23" s="54"/>
+      <c r="I23" s="54"/>
+      <c r="J23" s="54"/>
+      <c r="K23" s="54"/>
+      <c r="L23" s="54"/>
+      <c r="M23" s="54"/>
+      <c r="N23" s="54"/>
+      <c r="O23" s="54"/>
     </row>
     <row r="24" spans="2:15">
-      <c r="B24" s="49"/>
-      <c r="C24" s="49"/>
-      <c r="D24" s="49"/>
-      <c r="E24" s="49"/>
-      <c r="F24" s="49"/>
-      <c r="G24" s="49"/>
-      <c r="H24" s="49"/>
-      <c r="I24" s="49"/>
-      <c r="J24" s="49"/>
-      <c r="K24" s="49"/>
-      <c r="L24" s="49"/>
-      <c r="M24" s="49"/>
-      <c r="N24" s="49"/>
-      <c r="O24" s="49"/>
+      <c r="B24" s="54"/>
+      <c r="C24" s="54"/>
+      <c r="D24" s="54"/>
+      <c r="E24" s="54"/>
+      <c r="F24" s="54"/>
+      <c r="G24" s="54"/>
+      <c r="H24" s="54"/>
+      <c r="I24" s="54"/>
+      <c r="J24" s="54"/>
+      <c r="K24" s="54"/>
+      <c r="L24" s="54"/>
+      <c r="M24" s="54"/>
+      <c r="N24" s="54"/>
+      <c r="O24" s="54"/>
     </row>
     <row r="25" spans="2:15">
-      <c r="B25" s="49"/>
-      <c r="C25" s="49"/>
-      <c r="D25" s="49"/>
-      <c r="E25" s="49"/>
-      <c r="F25" s="49"/>
-      <c r="G25" s="49"/>
-      <c r="H25" s="49"/>
-      <c r="I25" s="49"/>
-      <c r="J25" s="49"/>
-      <c r="K25" s="49"/>
-      <c r="L25" s="49"/>
-      <c r="M25" s="49"/>
-      <c r="N25" s="49"/>
-      <c r="O25" s="49"/>
+      <c r="B25" s="54"/>
+      <c r="C25" s="54"/>
+      <c r="D25" s="54"/>
+      <c r="E25" s="54"/>
+      <c r="F25" s="54"/>
+      <c r="G25" s="54"/>
+      <c r="H25" s="54"/>
+      <c r="I25" s="54"/>
+      <c r="J25" s="54"/>
+      <c r="K25" s="54"/>
+      <c r="L25" s="54"/>
+      <c r="M25" s="54"/>
+      <c r="N25" s="54"/>
+      <c r="O25" s="54"/>
     </row>
     <row r="26" spans="2:15">
-      <c r="B26" s="32"/>
-      <c r="C26" s="32"/>
-      <c r="D26" s="32"/>
-      <c r="E26" s="32"/>
-      <c r="F26" s="32"/>
-      <c r="G26" s="32"/>
-      <c r="H26" s="32"/>
-      <c r="I26" s="32"/>
-      <c r="J26" s="32"/>
-      <c r="K26" s="32"/>
-      <c r="L26" s="32"/>
-      <c r="M26" s="32"/>
-      <c r="N26" s="32"/>
-      <c r="O26" s="32"/>
+      <c r="B26" s="54"/>
+      <c r="C26" s="54"/>
+      <c r="D26" s="54"/>
+      <c r="E26" s="54"/>
+      <c r="F26" s="54"/>
+      <c r="G26" s="54"/>
+      <c r="H26" s="54"/>
+      <c r="I26" s="54"/>
+      <c r="J26" s="54"/>
+      <c r="K26" s="54"/>
+      <c r="L26" s="54"/>
+      <c r="M26" s="54"/>
+      <c r="N26" s="54"/>
+      <c r="O26" s="54"/>
     </row>
     <row r="27" spans="2:15">
-      <c r="B27" s="33"/>
-      <c r="C27" s="33"/>
-      <c r="D27" s="33"/>
-      <c r="E27" s="33"/>
-      <c r="F27" s="33"/>
-      <c r="G27" s="33"/>
-      <c r="H27" s="33"/>
-      <c r="I27" s="33"/>
-      <c r="J27" s="33"/>
-      <c r="K27" s="33"/>
-      <c r="L27" s="33"/>
-      <c r="M27" s="33"/>
-      <c r="N27" s="33"/>
-      <c r="O27" s="33"/>
+      <c r="B27" s="54"/>
+      <c r="C27" s="54"/>
+      <c r="D27" s="54"/>
+      <c r="E27" s="54"/>
+      <c r="F27" s="54"/>
+      <c r="G27" s="54"/>
+      <c r="H27" s="54"/>
+      <c r="I27" s="54"/>
+      <c r="J27" s="54"/>
+      <c r="K27" s="54"/>
+      <c r="L27" s="54"/>
+      <c r="M27" s="54"/>
+      <c r="N27" s="54"/>
+      <c r="O27" s="54"/>
     </row>
     <row r="28" spans="2:15">
-      <c r="B28" s="33"/>
-      <c r="C28" s="33"/>
-      <c r="D28" s="33"/>
-      <c r="E28" s="33"/>
-      <c r="F28" s="33"/>
-      <c r="G28" s="33"/>
-      <c r="H28" s="33"/>
-      <c r="I28" s="33"/>
-      <c r="J28" s="33"/>
-      <c r="K28" s="33"/>
-      <c r="L28" s="33"/>
-      <c r="M28" s="33"/>
-      <c r="N28" s="33"/>
-      <c r="O28" s="33"/>
+      <c r="B28" s="28"/>
+      <c r="C28" s="28"/>
+      <c r="D28" s="28"/>
+      <c r="E28" s="28"/>
+      <c r="F28" s="28"/>
+      <c r="G28" s="28"/>
+      <c r="H28" s="28"/>
+      <c r="I28" s="28"/>
+      <c r="J28" s="28"/>
+      <c r="K28" s="28"/>
+      <c r="L28" s="28"/>
+      <c r="M28" s="28"/>
+      <c r="N28" s="28"/>
+      <c r="O28" s="28"/>
+    </row>
+    <row r="29" spans="2:15">
+      <c r="B29" s="42"/>
+      <c r="C29" s="42"/>
+      <c r="D29" s="42"/>
+      <c r="E29" s="42"/>
+      <c r="F29" s="42"/>
+      <c r="G29" s="42"/>
+      <c r="H29" s="42"/>
+      <c r="I29" s="42"/>
+      <c r="J29" s="42"/>
+      <c r="K29" s="42"/>
+      <c r="L29" s="42"/>
+      <c r="M29" s="42"/>
+      <c r="N29" s="42"/>
+      <c r="O29" s="42"/>
+    </row>
+    <row r="30" spans="2:15">
+      <c r="B30" s="42"/>
+      <c r="C30" s="42"/>
+      <c r="D30" s="42"/>
+      <c r="E30" s="42"/>
+      <c r="F30" s="42"/>
+      <c r="G30" s="42"/>
+      <c r="H30" s="42"/>
+      <c r="I30" s="42"/>
+      <c r="J30" s="42"/>
+      <c r="K30" s="42"/>
+      <c r="L30" s="42"/>
+      <c r="M30" s="42"/>
+      <c r="N30" s="42"/>
+      <c r="O30" s="42"/>
     </row>
   </sheetData>
-  <mergeCells count="15">
-    <mergeCell ref="B28:O28"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="B20:O25"/>
-    <mergeCell ref="B27:O27"/>
+  <mergeCells count="17">
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
     <mergeCell ref="C1:S2"/>
     <mergeCell ref="T1:U1"/>
     <mergeCell ref="T2:U2"/>
@@ -4413,6 +4459,13 @@
     <mergeCell ref="J4:L4"/>
     <mergeCell ref="C5:H5"/>
     <mergeCell ref="J5:L5"/>
+    <mergeCell ref="B30:O30"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="B22:O27"/>
+    <mergeCell ref="B29:O29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Cambios en observaciones Reporte Anexo 7
</commit_message>
<xml_diff>
--- a/Unna.OperationalReport.WebSite/wwwroot/plantillas/reporte/mensual/BoletadeValorizacionPetroperu.xlsx
+++ b/Unna.OperationalReport.WebSite/wwwroot/plantillas/reporte/mensual/BoletadeValorizacionPetroperu.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27809"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27816"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desarrollos\SP\APSS SP\ProyectoPrincipalAenza6\UnnaReportesOperativos\Unna.OperationalReport.WebSite\wwwroot\plantillas\reporte\mensual\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desarrollos\SP\APSS SP\ProyectoPrincipalAenza7\UnnaReportesOperativos\Unna.OperationalReport.WebSite\wwwroot\plantillas\reporte\mensual\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83D164D3-FEA4-4200-87EA-63631BC9B2F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC67E0E8-4EE3-42FD-A769-5AF86FEE98AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="759" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -912,7 +912,7 @@
     <xf numFmtId="168" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="169" fontId="7" fillId="0" borderId="0" xfId="103" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -992,6 +992,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1001,8 +1007,41 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="2" xfId="103" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="3" xfId="103" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="10" xfId="103" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="11" xfId="103" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="7" xfId="103" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="12" xfId="103" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" xfId="103" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="14" xfId="103" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="15" xfId="103" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="16" xfId="103" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1031,45 +1070,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="2" xfId="103" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="3" xfId="103" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="10" xfId="103" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="11" xfId="103" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="7" xfId="103" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="12" xfId="103" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" xfId="103" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="14" xfId="103" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="15" xfId="103" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="16" xfId="103" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1079,19 +1079,6 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" xfId="103" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="8" fillId="0" borderId="0" xfId="103" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="103" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" xfId="103" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="104">
     <cellStyle name="Euro" xfId="35" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -1228,7 +1215,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1619250</xdr:colOff>
+      <xdr:colOff>1413510</xdr:colOff>
       <xdr:row>42</xdr:row>
       <xdr:rowOff>97340</xdr:rowOff>
     </xdr:to>
@@ -1277,8 +1264,8 @@
       <xdr:rowOff>91440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>3389</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>872069</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>59055</xdr:rowOff>
     </xdr:to>
@@ -1328,6 +1315,50 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1043940</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>160020</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>245044</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>161833</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Imagen 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2DB7E5BF-AD5F-4136-307D-206AF3F1C1A7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2628900" y="8862060"/>
+          <a:ext cx="5609524" cy="733333"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1342,7 +1373,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1604010</xdr:colOff>
+      <xdr:colOff>1398270</xdr:colOff>
       <xdr:row>42</xdr:row>
       <xdr:rowOff>97340</xdr:rowOff>
     </xdr:to>
@@ -1388,13 +1419,13 @@
       <xdr:col>1</xdr:col>
       <xdr:colOff>15240</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>22860</xdr:rowOff>
+      <xdr:rowOff>83820</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>861060</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>179747</xdr:rowOff>
+      <xdr:rowOff>45720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1422,8 +1453,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="106680" y="22860"/>
-          <a:ext cx="853440" cy="499787"/>
+          <a:off x="106680" y="83820"/>
+          <a:ext cx="845820" cy="304800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1442,6 +1473,50 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>929640</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>160020</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>283125</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>83715</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Imagen 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DAA76015-66E3-AEB1-1F0D-FF121C9F8AF8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2476500" y="8862060"/>
+          <a:ext cx="5761905" cy="838095"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1456,7 +1531,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1588770</xdr:colOff>
+      <xdr:colOff>1383030</xdr:colOff>
       <xdr:row>42</xdr:row>
       <xdr:rowOff>97340</xdr:rowOff>
     </xdr:to>
@@ -1502,13 +1577,13 @@
       <xdr:col>1</xdr:col>
       <xdr:colOff>15240</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>22860</xdr:rowOff>
+      <xdr:rowOff>68581</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>861060</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>156887</xdr:rowOff>
+      <xdr:colOff>830580</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1536,8 +1611,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="106680" y="22860"/>
-          <a:ext cx="853440" cy="499787"/>
+          <a:off x="76200" y="68581"/>
+          <a:ext cx="815340" cy="411479"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1556,6 +1631,50 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>861060</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>160020</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>262164</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>26572</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{70F770CC-73BE-F908-977F-F409A301247E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2415540" y="8862060"/>
+          <a:ext cx="5809524" cy="780952"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1570,7 +1689,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1573530</xdr:colOff>
+      <xdr:colOff>1367790</xdr:colOff>
       <xdr:row>42</xdr:row>
       <xdr:rowOff>97340</xdr:rowOff>
     </xdr:to>
@@ -1614,15 +1733,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>15240</xdr:colOff>
+      <xdr:colOff>60960</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>22860</xdr:rowOff>
+      <xdr:rowOff>45721</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>853440</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>141647</xdr:rowOff>
+      <xdr:colOff>899160</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>167640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1650,8 +1769,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="106680" y="22860"/>
-          <a:ext cx="845820" cy="667427"/>
+          <a:off x="152400" y="45721"/>
+          <a:ext cx="838200" cy="464819"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1666,6 +1785,50 @@
             </a14:hiddenFill>
           </a:ext>
         </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>967740</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>167640</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>140272</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>178977</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Imagen 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B5045F6F-E112-EB98-5688-09E2EDCB422E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2552700" y="8869680"/>
+          <a:ext cx="5580952" cy="742857"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -1939,16 +2102,15 @@
   <dimension ref="B1:AL31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B12" sqref="B12:C12"/>
+      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="1.33203125" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
-    <col min="3" max="3" width="17.77734375" customWidth="1"/>
-    <col min="4" max="4" width="24.44140625" customWidth="1"/>
+    <col min="2" max="2" width="21.77734375" customWidth="1"/>
+    <col min="3" max="4" width="20.77734375" customWidth="1"/>
     <col min="5" max="5" width="29" customWidth="1"/>
     <col min="8" max="21" width="12.88671875" customWidth="1"/>
     <col min="23" max="23" width="12.44140625" customWidth="1"/>
@@ -1959,86 +2121,86 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:38" ht="27" customHeight="1">
-      <c r="C1" s="40" t="s">
+      <c r="C1" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
-      <c r="H1" s="40"/>
-      <c r="I1" s="40"/>
-      <c r="J1" s="40"/>
-      <c r="K1" s="40"/>
-      <c r="L1" s="40"/>
-      <c r="M1" s="40"/>
-      <c r="N1" s="40"/>
-      <c r="O1" s="40"/>
-      <c r="P1" s="40"/>
-      <c r="Q1" s="40"/>
-      <c r="R1" s="40"/>
-      <c r="S1" s="40"/>
-      <c r="T1" s="40"/>
-      <c r="U1" s="40"/>
-      <c r="V1" s="40"/>
-      <c r="W1" s="40"/>
-      <c r="X1" s="40"/>
-      <c r="Y1" s="40"/>
-      <c r="Z1" s="40"/>
-      <c r="AA1" s="40"/>
-      <c r="AB1" s="40"/>
-      <c r="AC1" s="40"/>
-      <c r="AD1" s="40"/>
-      <c r="AE1" s="40"/>
-      <c r="AF1" s="40"/>
-      <c r="AG1" s="40"/>
-      <c r="AH1" s="40"/>
-      <c r="AI1" s="40"/>
-      <c r="AJ1" s="40"/>
-      <c r="AK1" s="37" t="s">
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="53"/>
+      <c r="H1" s="53"/>
+      <c r="I1" s="53"/>
+      <c r="J1" s="53"/>
+      <c r="K1" s="53"/>
+      <c r="L1" s="53"/>
+      <c r="M1" s="53"/>
+      <c r="N1" s="53"/>
+      <c r="O1" s="53"/>
+      <c r="P1" s="53"/>
+      <c r="Q1" s="53"/>
+      <c r="R1" s="53"/>
+      <c r="S1" s="53"/>
+      <c r="T1" s="53"/>
+      <c r="U1" s="53"/>
+      <c r="V1" s="53"/>
+      <c r="W1" s="53"/>
+      <c r="X1" s="53"/>
+      <c r="Y1" s="53"/>
+      <c r="Z1" s="53"/>
+      <c r="AA1" s="53"/>
+      <c r="AB1" s="53"/>
+      <c r="AC1" s="53"/>
+      <c r="AD1" s="53"/>
+      <c r="AE1" s="53"/>
+      <c r="AF1" s="53"/>
+      <c r="AG1" s="53"/>
+      <c r="AH1" s="53"/>
+      <c r="AI1" s="53"/>
+      <c r="AJ1" s="53"/>
+      <c r="AK1" s="50" t="s">
         <v>63</v>
       </c>
-      <c r="AL1" s="38"/>
+      <c r="AL1" s="51"/>
     </row>
     <row r="2" spans="2:38" ht="15" thickBot="1">
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
-      <c r="J2" s="40"/>
-      <c r="K2" s="40"/>
-      <c r="L2" s="40"/>
-      <c r="M2" s="40"/>
-      <c r="N2" s="40"/>
-      <c r="O2" s="40"/>
-      <c r="P2" s="40"/>
-      <c r="Q2" s="40"/>
-      <c r="R2" s="40"/>
-      <c r="S2" s="40"/>
-      <c r="T2" s="40"/>
-      <c r="U2" s="40"/>
-      <c r="V2" s="40"/>
-      <c r="W2" s="40"/>
-      <c r="X2" s="40"/>
-      <c r="Y2" s="40"/>
-      <c r="Z2" s="40"/>
-      <c r="AA2" s="40"/>
-      <c r="AB2" s="40"/>
-      <c r="AC2" s="40"/>
-      <c r="AD2" s="40"/>
-      <c r="AE2" s="40"/>
-      <c r="AF2" s="40"/>
-      <c r="AG2" s="40"/>
-      <c r="AH2" s="40"/>
-      <c r="AI2" s="40"/>
-      <c r="AJ2" s="40"/>
-      <c r="AK2" s="39" t="s">
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="53"/>
+      <c r="I2" s="53"/>
+      <c r="J2" s="53"/>
+      <c r="K2" s="53"/>
+      <c r="L2" s="53"/>
+      <c r="M2" s="53"/>
+      <c r="N2" s="53"/>
+      <c r="O2" s="53"/>
+      <c r="P2" s="53"/>
+      <c r="Q2" s="53"/>
+      <c r="R2" s="53"/>
+      <c r="S2" s="53"/>
+      <c r="T2" s="53"/>
+      <c r="U2" s="53"/>
+      <c r="V2" s="53"/>
+      <c r="W2" s="53"/>
+      <c r="X2" s="53"/>
+      <c r="Y2" s="53"/>
+      <c r="Z2" s="53"/>
+      <c r="AA2" s="53"/>
+      <c r="AB2" s="53"/>
+      <c r="AC2" s="53"/>
+      <c r="AD2" s="53"/>
+      <c r="AE2" s="53"/>
+      <c r="AF2" s="53"/>
+      <c r="AG2" s="53"/>
+      <c r="AH2" s="53"/>
+      <c r="AI2" s="53"/>
+      <c r="AJ2" s="53"/>
+      <c r="AK2" s="52" t="s">
         <v>64</v>
       </c>
-      <c r="AL2" s="39"/>
+      <c r="AL2" s="52"/>
     </row>
     <row r="3" spans="2:38" ht="15" thickBot="1">
       <c r="C3" s="23" t="s">
@@ -2083,80 +2245,80 @@
       <c r="AL3" s="20"/>
     </row>
     <row r="4" spans="2:38" ht="29.4" customHeight="1" thickBot="1">
-      <c r="C4" s="29" t="s">
+      <c r="C4" s="31" t="s">
         <v>105</v>
       </c>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="30"/>
-      <c r="H4" s="30"/>
-      <c r="I4" s="30"/>
-      <c r="J4" s="30"/>
-      <c r="K4" s="30"/>
-      <c r="L4" s="30"/>
-      <c r="M4" s="30"/>
-      <c r="N4" s="30"/>
-      <c r="O4" s="30"/>
-      <c r="P4" s="30"/>
-      <c r="Q4" s="30"/>
-      <c r="R4" s="30"/>
-      <c r="S4" s="30"/>
-      <c r="T4" s="30"/>
-      <c r="U4" s="31"/>
-      <c r="V4" s="33" t="s">
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="32"/>
+      <c r="I4" s="32"/>
+      <c r="J4" s="32"/>
+      <c r="K4" s="32"/>
+      <c r="L4" s="32"/>
+      <c r="M4" s="32"/>
+      <c r="N4" s="32"/>
+      <c r="O4" s="32"/>
+      <c r="P4" s="32"/>
+      <c r="Q4" s="32"/>
+      <c r="R4" s="32"/>
+      <c r="S4" s="32"/>
+      <c r="T4" s="32"/>
+      <c r="U4" s="33"/>
+      <c r="V4" s="46" t="s">
         <v>68</v>
       </c>
-      <c r="W4" s="33" t="s">
+      <c r="W4" s="46" t="s">
         <v>69</v>
       </c>
-      <c r="X4" s="29" t="s">
+      <c r="X4" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="Y4" s="30"/>
-      <c r="Z4" s="30"/>
-      <c r="AA4" s="30"/>
-      <c r="AB4" s="30"/>
-      <c r="AC4" s="31"/>
+      <c r="Y4" s="32"/>
+      <c r="Z4" s="32"/>
+      <c r="AA4" s="32"/>
+      <c r="AB4" s="32"/>
+      <c r="AC4" s="33"/>
     </row>
     <row r="5" spans="2:38" ht="15" thickBot="1">
-      <c r="C5" s="29" t="s">
+      <c r="C5" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="30"/>
-      <c r="E5" s="30"/>
-      <c r="F5" s="30"/>
-      <c r="G5" s="30"/>
-      <c r="H5" s="31"/>
-      <c r="I5" s="29" t="s">
+      <c r="D5" s="32"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="32"/>
+      <c r="H5" s="33"/>
+      <c r="I5" s="31" t="s">
         <v>65</v>
       </c>
-      <c r="J5" s="30"/>
-      <c r="K5" s="30"/>
-      <c r="L5" s="30"/>
-      <c r="M5" s="30"/>
-      <c r="N5" s="31"/>
-      <c r="O5" s="29" t="s">
+      <c r="J5" s="32"/>
+      <c r="K5" s="32"/>
+      <c r="L5" s="32"/>
+      <c r="M5" s="32"/>
+      <c r="N5" s="33"/>
+      <c r="O5" s="31" t="s">
         <v>66</v>
       </c>
-      <c r="P5" s="30"/>
-      <c r="Q5" s="30"/>
-      <c r="R5" s="30"/>
-      <c r="S5" s="30"/>
-      <c r="T5" s="30"/>
-      <c r="U5" s="33" t="s">
+      <c r="P5" s="32"/>
+      <c r="Q5" s="32"/>
+      <c r="R5" s="32"/>
+      <c r="S5" s="32"/>
+      <c r="T5" s="32"/>
+      <c r="U5" s="46" t="s">
         <v>67</v>
       </c>
-      <c r="V5" s="35"/>
-      <c r="W5" s="35"/>
-      <c r="X5" s="29" t="s">
+      <c r="V5" s="48"/>
+      <c r="W5" s="48"/>
+      <c r="X5" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="Y5" s="30"/>
-      <c r="Z5" s="30"/>
-      <c r="AA5" s="30"/>
-      <c r="AB5" s="30"/>
-      <c r="AC5" s="31"/>
+      <c r="Y5" s="32"/>
+      <c r="Z5" s="32"/>
+      <c r="AA5" s="32"/>
+      <c r="AB5" s="32"/>
+      <c r="AC5" s="33"/>
     </row>
     <row r="6" spans="2:38" ht="58.2" thickBot="1">
       <c r="B6" s="2"/>
@@ -2214,9 +2376,9 @@
       <c r="T6" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="U6" s="34"/>
-      <c r="V6" s="36"/>
-      <c r="W6" s="36"/>
+      <c r="U6" s="47"/>
+      <c r="V6" s="49"/>
+      <c r="W6" s="49"/>
       <c r="X6" s="12" t="s">
         <v>8</v>
       </c>
@@ -2473,20 +2635,20 @@
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
     </row>
-    <row r="12" spans="2:38" ht="24.6" customHeight="1">
-      <c r="B12" s="32" t="s">
+    <row r="12" spans="2:38">
+      <c r="B12" s="29" t="s">
         <v>107</v>
       </c>
-      <c r="C12" s="32"/>
-      <c r="D12" s="7"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="29"/>
       <c r="E12" s="7"/>
     </row>
-    <row r="13" spans="2:38" ht="27.6" customHeight="1" thickBot="1">
-      <c r="B13" s="53" t="s">
+    <row r="13" spans="2:38" ht="15" thickBot="1">
+      <c r="B13" s="45" t="s">
         <v>108</v>
       </c>
-      <c r="C13" s="53"/>
-      <c r="D13" s="25"/>
+      <c r="C13" s="45"/>
+      <c r="D13" s="45"/>
       <c r="E13" s="26"/>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
@@ -2508,11 +2670,11 @@
       <c r="W13" s="4"/>
     </row>
     <row r="14" spans="2:38" ht="16.8" customHeight="1" thickBot="1">
-      <c r="B14" s="50" t="s">
+      <c r="B14" s="41" t="s">
         <v>54</v>
       </c>
-      <c r="C14" s="51"/>
-      <c r="D14" s="52"/>
+      <c r="C14" s="42"/>
+      <c r="D14" s="43"/>
       <c r="E14" s="18" t="s">
         <v>53</v>
       </c>
@@ -2537,9 +2699,8 @@
     </row>
     <row r="15" spans="2:38" ht="15" thickBot="1">
       <c r="B15" s="1"/>
-      <c r="C15" s="49"/>
-      <c r="D15" s="61"/>
-      <c r="E15" s="62"/>
+      <c r="C15" s="40"/>
+      <c r="D15" s="40"/>
     </row>
     <row r="16" spans="2:38" ht="29.4" thickBot="1">
       <c r="B16" s="1"/>
@@ -2549,22 +2710,22 @@
         <v>109</v>
       </c>
     </row>
-    <row r="17" spans="2:15" ht="39.6" customHeight="1" thickBot="1">
-      <c r="B17" s="43" t="s">
+    <row r="17" spans="2:15" ht="15" thickBot="1">
+      <c r="B17" s="34" t="s">
         <v>58</v>
       </c>
-      <c r="C17" s="44"/>
-      <c r="D17" s="45"/>
+      <c r="C17" s="35"/>
+      <c r="D17" s="36"/>
       <c r="E17" s="27" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="18" spans="2:15" ht="43.8" customHeight="1" thickBot="1">
-      <c r="B18" s="46" t="s">
+    <row r="18" spans="2:15" ht="15" thickBot="1">
+      <c r="B18" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="C18" s="47"/>
-      <c r="D18" s="48"/>
+      <c r="C18" s="38"/>
+      <c r="D18" s="39"/>
       <c r="E18" s="27" t="s">
         <v>57</v>
       </c>
@@ -2585,102 +2746,102 @@
       </c>
     </row>
     <row r="22" spans="2:15">
-      <c r="B22" s="54" t="s">
+      <c r="B22" s="44" t="s">
         <v>60</v>
       </c>
-      <c r="C22" s="54"/>
-      <c r="D22" s="54"/>
-      <c r="E22" s="54"/>
-      <c r="F22" s="54"/>
-      <c r="G22" s="54"/>
-      <c r="H22" s="54"/>
-      <c r="I22" s="54"/>
-      <c r="J22" s="54"/>
-      <c r="K22" s="54"/>
-      <c r="L22" s="54"/>
-      <c r="M22" s="54"/>
-      <c r="N22" s="54"/>
-      <c r="O22" s="54"/>
+      <c r="C22" s="44"/>
+      <c r="D22" s="44"/>
+      <c r="E22" s="44"/>
+      <c r="F22" s="44"/>
+      <c r="G22" s="44"/>
+      <c r="H22" s="44"/>
+      <c r="I22" s="44"/>
+      <c r="J22" s="44"/>
+      <c r="K22" s="44"/>
+      <c r="L22" s="44"/>
+      <c r="M22" s="44"/>
+      <c r="N22" s="44"/>
+      <c r="O22" s="44"/>
     </row>
     <row r="23" spans="2:15">
-      <c r="B23" s="54"/>
-      <c r="C23" s="54"/>
-      <c r="D23" s="54"/>
-      <c r="E23" s="54"/>
-      <c r="F23" s="54"/>
-      <c r="G23" s="54"/>
-      <c r="H23" s="54"/>
-      <c r="I23" s="54"/>
-      <c r="J23" s="54"/>
-      <c r="K23" s="54"/>
-      <c r="L23" s="54"/>
-      <c r="M23" s="54"/>
-      <c r="N23" s="54"/>
-      <c r="O23" s="54"/>
+      <c r="B23" s="44"/>
+      <c r="C23" s="44"/>
+      <c r="D23" s="44"/>
+      <c r="E23" s="44"/>
+      <c r="F23" s="44"/>
+      <c r="G23" s="44"/>
+      <c r="H23" s="44"/>
+      <c r="I23" s="44"/>
+      <c r="J23" s="44"/>
+      <c r="K23" s="44"/>
+      <c r="L23" s="44"/>
+      <c r="M23" s="44"/>
+      <c r="N23" s="44"/>
+      <c r="O23" s="44"/>
     </row>
     <row r="24" spans="2:15">
-      <c r="B24" s="54"/>
-      <c r="C24" s="54"/>
-      <c r="D24" s="54"/>
-      <c r="E24" s="54"/>
-      <c r="F24" s="54"/>
-      <c r="G24" s="54"/>
-      <c r="H24" s="54"/>
-      <c r="I24" s="54"/>
-      <c r="J24" s="54"/>
-      <c r="K24" s="54"/>
-      <c r="L24" s="54"/>
-      <c r="M24" s="54"/>
-      <c r="N24" s="54"/>
-      <c r="O24" s="54"/>
+      <c r="B24" s="44"/>
+      <c r="C24" s="44"/>
+      <c r="D24" s="44"/>
+      <c r="E24" s="44"/>
+      <c r="F24" s="44"/>
+      <c r="G24" s="44"/>
+      <c r="H24" s="44"/>
+      <c r="I24" s="44"/>
+      <c r="J24" s="44"/>
+      <c r="K24" s="44"/>
+      <c r="L24" s="44"/>
+      <c r="M24" s="44"/>
+      <c r="N24" s="44"/>
+      <c r="O24" s="44"/>
     </row>
     <row r="25" spans="2:15">
-      <c r="B25" s="54"/>
-      <c r="C25" s="54"/>
-      <c r="D25" s="54"/>
-      <c r="E25" s="54"/>
-      <c r="F25" s="54"/>
-      <c r="G25" s="54"/>
-      <c r="H25" s="54"/>
-      <c r="I25" s="54"/>
-      <c r="J25" s="54"/>
-      <c r="K25" s="54"/>
-      <c r="L25" s="54"/>
-      <c r="M25" s="54"/>
-      <c r="N25" s="54"/>
-      <c r="O25" s="54"/>
+      <c r="B25" s="44"/>
+      <c r="C25" s="44"/>
+      <c r="D25" s="44"/>
+      <c r="E25" s="44"/>
+      <c r="F25" s="44"/>
+      <c r="G25" s="44"/>
+      <c r="H25" s="44"/>
+      <c r="I25" s="44"/>
+      <c r="J25" s="44"/>
+      <c r="K25" s="44"/>
+      <c r="L25" s="44"/>
+      <c r="M25" s="44"/>
+      <c r="N25" s="44"/>
+      <c r="O25" s="44"/>
     </row>
     <row r="26" spans="2:15">
-      <c r="B26" s="54"/>
-      <c r="C26" s="54"/>
-      <c r="D26" s="54"/>
-      <c r="E26" s="54"/>
-      <c r="F26" s="54"/>
-      <c r="G26" s="54"/>
-      <c r="H26" s="54"/>
-      <c r="I26" s="54"/>
-      <c r="J26" s="54"/>
-      <c r="K26" s="54"/>
-      <c r="L26" s="54"/>
-      <c r="M26" s="54"/>
-      <c r="N26" s="54"/>
-      <c r="O26" s="54"/>
+      <c r="B26" s="44"/>
+      <c r="C26" s="44"/>
+      <c r="D26" s="44"/>
+      <c r="E26" s="44"/>
+      <c r="F26" s="44"/>
+      <c r="G26" s="44"/>
+      <c r="H26" s="44"/>
+      <c r="I26" s="44"/>
+      <c r="J26" s="44"/>
+      <c r="K26" s="44"/>
+      <c r="L26" s="44"/>
+      <c r="M26" s="44"/>
+      <c r="N26" s="44"/>
+      <c r="O26" s="44"/>
     </row>
     <row r="27" spans="2:15">
-      <c r="B27" s="54"/>
-      <c r="C27" s="54"/>
-      <c r="D27" s="54"/>
-      <c r="E27" s="54"/>
-      <c r="F27" s="54"/>
-      <c r="G27" s="54"/>
-      <c r="H27" s="54"/>
-      <c r="I27" s="54"/>
-      <c r="J27" s="54"/>
-      <c r="K27" s="54"/>
-      <c r="L27" s="54"/>
-      <c r="M27" s="54"/>
-      <c r="N27" s="54"/>
-      <c r="O27" s="54"/>
+      <c r="B27" s="44"/>
+      <c r="C27" s="44"/>
+      <c r="D27" s="44"/>
+      <c r="E27" s="44"/>
+      <c r="F27" s="44"/>
+      <c r="G27" s="44"/>
+      <c r="H27" s="44"/>
+      <c r="I27" s="44"/>
+      <c r="J27" s="44"/>
+      <c r="K27" s="44"/>
+      <c r="L27" s="44"/>
+      <c r="M27" s="44"/>
+      <c r="N27" s="44"/>
+      <c r="O27" s="44"/>
     </row>
     <row r="28" spans="2:15">
       <c r="B28" s="20"/>
@@ -2699,61 +2860,71 @@
       <c r="O28" s="20"/>
     </row>
     <row r="29" spans="2:15">
-      <c r="B29" s="42" t="s">
+      <c r="B29" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="C29" s="42"/>
-      <c r="D29" s="42"/>
-      <c r="E29" s="42"/>
-      <c r="F29" s="42"/>
-      <c r="G29" s="42"/>
-      <c r="H29" s="42"/>
-      <c r="I29" s="42"/>
-      <c r="J29" s="42"/>
-      <c r="K29" s="42"/>
-      <c r="L29" s="42"/>
-      <c r="M29" s="42"/>
-      <c r="N29" s="42"/>
-      <c r="O29" s="42"/>
+      <c r="C29" s="30"/>
+      <c r="D29" s="30"/>
+      <c r="E29" s="30"/>
+      <c r="F29" s="30"/>
+      <c r="G29" s="30"/>
+      <c r="H29" s="30"/>
+      <c r="I29" s="30"/>
+      <c r="J29" s="30"/>
+      <c r="K29" s="30"/>
+      <c r="L29" s="30"/>
+      <c r="M29" s="30"/>
+      <c r="N29" s="30"/>
+      <c r="O29" s="30"/>
     </row>
     <row r="30" spans="2:15">
-      <c r="B30" s="42" t="s">
+      <c r="B30" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="C30" s="42"/>
-      <c r="D30" s="42"/>
-      <c r="E30" s="42"/>
-      <c r="F30" s="42"/>
-      <c r="G30" s="42"/>
-      <c r="H30" s="42"/>
-      <c r="I30" s="42"/>
-      <c r="J30" s="42"/>
-      <c r="K30" s="42"/>
-      <c r="L30" s="42"/>
-      <c r="M30" s="42"/>
-      <c r="N30" s="42"/>
-      <c r="O30" s="42"/>
+      <c r="C30" s="30"/>
+      <c r="D30" s="30"/>
+      <c r="E30" s="30"/>
+      <c r="F30" s="30"/>
+      <c r="G30" s="30"/>
+      <c r="H30" s="30"/>
+      <c r="I30" s="30"/>
+      <c r="J30" s="30"/>
+      <c r="K30" s="30"/>
+      <c r="L30" s="30"/>
+      <c r="M30" s="30"/>
+      <c r="N30" s="30"/>
+      <c r="O30" s="30"/>
     </row>
     <row r="31" spans="2:15">
-      <c r="B31" s="42" t="s">
+      <c r="B31" s="30" t="s">
         <v>110</v>
       </c>
-      <c r="C31" s="42"/>
-      <c r="D31" s="42"/>
-      <c r="E31" s="42"/>
-      <c r="F31" s="42"/>
-      <c r="G31" s="42"/>
-      <c r="H31" s="42"/>
-      <c r="I31" s="42"/>
-      <c r="J31" s="42"/>
-      <c r="K31" s="42"/>
-      <c r="L31" s="42"/>
-      <c r="M31" s="42"/>
-      <c r="N31" s="42"/>
-      <c r="O31" s="42"/>
+      <c r="C31" s="30"/>
+      <c r="D31" s="30"/>
+      <c r="E31" s="30"/>
+      <c r="F31" s="30"/>
+      <c r="G31" s="30"/>
+      <c r="H31" s="30"/>
+      <c r="I31" s="30"/>
+      <c r="J31" s="30"/>
+      <c r="K31" s="30"/>
+      <c r="L31" s="30"/>
+      <c r="M31" s="30"/>
+      <c r="N31" s="30"/>
+      <c r="O31" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="C4:U4"/>
+    <mergeCell ref="U5:U6"/>
+    <mergeCell ref="W4:W6"/>
+    <mergeCell ref="AK1:AL1"/>
+    <mergeCell ref="AK2:AL2"/>
+    <mergeCell ref="C1:AJ2"/>
+    <mergeCell ref="X5:AC5"/>
+    <mergeCell ref="X4:AC4"/>
+    <mergeCell ref="V4:V6"/>
+    <mergeCell ref="B12:D12"/>
     <mergeCell ref="B29:O29"/>
     <mergeCell ref="B30:O30"/>
     <mergeCell ref="B31:O31"/>
@@ -2764,18 +2935,8 @@
     <mergeCell ref="B18:D18"/>
     <mergeCell ref="C15:D15"/>
     <mergeCell ref="B14:D14"/>
-    <mergeCell ref="B13:C13"/>
     <mergeCell ref="B22:O27"/>
-    <mergeCell ref="C4:U4"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="U5:U6"/>
-    <mergeCell ref="W4:W6"/>
-    <mergeCell ref="AK1:AL1"/>
-    <mergeCell ref="AK2:AL2"/>
-    <mergeCell ref="C1:AJ2"/>
-    <mergeCell ref="X5:AC5"/>
-    <mergeCell ref="X4:AC4"/>
-    <mergeCell ref="V4:V6"/>
+    <mergeCell ref="B13:D13"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" horizontalDpi="300" r:id="rId1"/>
@@ -2787,16 +2948,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15F5674C-6194-49DE-8C68-201941F0F769}">
   <dimension ref="B1:U30"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="I52" sqref="I52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="1.33203125" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
-    <col min="3" max="3" width="17.77734375" customWidth="1"/>
-    <col min="4" max="4" width="24.44140625" customWidth="1"/>
+    <col min="1" max="1" width="0.77734375" customWidth="1"/>
+    <col min="2" max="2" width="21.77734375" customWidth="1"/>
+    <col min="3" max="4" width="20.77734375" customWidth="1"/>
     <col min="5" max="5" width="29" customWidth="1"/>
     <col min="8" max="8" width="12.88671875" customWidth="1"/>
     <col min="13" max="13" width="14.109375" customWidth="1"/>
@@ -2806,52 +2966,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:21" ht="27" customHeight="1">
-      <c r="C1" s="40" t="s">
+      <c r="C1" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
-      <c r="H1" s="40"/>
-      <c r="I1" s="40"/>
-      <c r="J1" s="40"/>
-      <c r="K1" s="40"/>
-      <c r="L1" s="40"/>
-      <c r="M1" s="40"/>
-      <c r="N1" s="40"/>
-      <c r="O1" s="40"/>
-      <c r="P1" s="40"/>
-      <c r="Q1" s="40"/>
-      <c r="R1" s="40"/>
-      <c r="S1" s="40"/>
-      <c r="T1" s="37" t="s">
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="53"/>
+      <c r="H1" s="53"/>
+      <c r="I1" s="53"/>
+      <c r="J1" s="53"/>
+      <c r="K1" s="53"/>
+      <c r="L1" s="53"/>
+      <c r="M1" s="53"/>
+      <c r="N1" s="53"/>
+      <c r="O1" s="53"/>
+      <c r="P1" s="53"/>
+      <c r="Q1" s="53"/>
+      <c r="R1" s="53"/>
+      <c r="S1" s="53"/>
+      <c r="T1" s="50" t="s">
         <v>63</v>
       </c>
-      <c r="U1" s="38"/>
+      <c r="U1" s="51"/>
     </row>
     <row r="2" spans="2:21" ht="15" thickBot="1">
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
-      <c r="J2" s="40"/>
-      <c r="K2" s="40"/>
-      <c r="L2" s="40"/>
-      <c r="M2" s="40"/>
-      <c r="N2" s="40"/>
-      <c r="O2" s="40"/>
-      <c r="P2" s="40"/>
-      <c r="Q2" s="40"/>
-      <c r="R2" s="40"/>
-      <c r="S2" s="40"/>
-      <c r="T2" s="39" t="s">
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="53"/>
+      <c r="I2" s="53"/>
+      <c r="J2" s="53"/>
+      <c r="K2" s="53"/>
+      <c r="L2" s="53"/>
+      <c r="M2" s="53"/>
+      <c r="N2" s="53"/>
+      <c r="O2" s="53"/>
+      <c r="P2" s="53"/>
+      <c r="Q2" s="53"/>
+      <c r="R2" s="53"/>
+      <c r="S2" s="53"/>
+      <c r="T2" s="52" t="s">
         <v>64</v>
       </c>
-      <c r="U2" s="39"/>
+      <c r="U2" s="52"/>
     </row>
     <row r="3" spans="2:21" ht="15" thickBot="1">
       <c r="C3" s="24" t="s">
@@ -2879,15 +3039,15 @@
       <c r="U3" s="20"/>
     </row>
     <row r="4" spans="2:21" ht="29.4" customHeight="1" thickBot="1">
-      <c r="C4" s="29" t="s">
+      <c r="C4" s="31" t="s">
         <v>105</v>
       </c>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="30"/>
-      <c r="H4" s="31"/>
-      <c r="I4" s="33" t="s">
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="46" t="s">
         <v>68</v>
       </c>
       <c r="J4" s="55" t="s">
@@ -2897,20 +3057,20 @@
       <c r="L4" s="57"/>
     </row>
     <row r="5" spans="2:21" ht="15" thickBot="1">
-      <c r="C5" s="29" t="s">
+      <c r="C5" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="30"/>
-      <c r="E5" s="30"/>
-      <c r="F5" s="30"/>
-      <c r="G5" s="30"/>
-      <c r="H5" s="31"/>
-      <c r="I5" s="35"/>
-      <c r="J5" s="29" t="s">
+      <c r="D5" s="32"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="32"/>
+      <c r="H5" s="33"/>
+      <c r="I5" s="48"/>
+      <c r="J5" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="K5" s="30"/>
-      <c r="L5" s="31"/>
+      <c r="K5" s="32"/>
+      <c r="L5" s="33"/>
     </row>
     <row r="6" spans="2:21" ht="58.2" thickBot="1">
       <c r="B6" s="2"/>
@@ -2932,7 +3092,7 @@
       <c r="H6" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="I6" s="36"/>
+      <c r="I6" s="49"/>
       <c r="J6" s="12" t="s">
         <v>8</v>
       </c>
@@ -3092,32 +3252,32 @@
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
     </row>
-    <row r="12" spans="2:21" ht="22.2" customHeight="1">
-      <c r="B12" s="32" t="s">
+    <row r="12" spans="2:21">
+      <c r="B12" s="29" t="s">
         <v>107</v>
       </c>
-      <c r="C12" s="32"/>
-      <c r="D12" s="7"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="29"/>
       <c r="E12" s="7"/>
     </row>
-    <row r="13" spans="2:21" ht="32.4" customHeight="1" thickBot="1">
-      <c r="B13" s="53" t="s">
+    <row r="13" spans="2:21" ht="15" thickBot="1">
+      <c r="B13" s="45" t="s">
         <v>108</v>
       </c>
-      <c r="C13" s="53"/>
-      <c r="D13" s="59"/>
-      <c r="E13" s="60"/>
+      <c r="C13" s="45"/>
+      <c r="D13" s="45"/>
+      <c r="E13" s="26"/>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
     </row>
     <row r="14" spans="2:21" ht="16.8" customHeight="1" thickBot="1">
-      <c r="B14" s="50" t="s">
+      <c r="B14" s="41" t="s">
         <v>54</v>
       </c>
-      <c r="C14" s="51"/>
-      <c r="D14" s="52"/>
+      <c r="C14" s="42"/>
+      <c r="D14" s="43"/>
       <c r="E14" s="18" t="s">
         <v>53</v>
       </c>
@@ -3128,34 +3288,33 @@
     </row>
     <row r="15" spans="2:21" ht="15" thickBot="1">
       <c r="B15" s="1"/>
-      <c r="C15" s="49"/>
-      <c r="D15" s="61"/>
-      <c r="E15" s="62"/>
+      <c r="C15" s="40"/>
+      <c r="D15" s="40"/>
     </row>
     <row r="16" spans="2:21" ht="29.4" thickBot="1">
-      <c r="B16" s="58"/>
-      <c r="C16" s="59"/>
-      <c r="D16" s="59"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="25"/>
       <c r="E16" s="12" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="17" spans="2:15" ht="39.6" customHeight="1" thickBot="1">
-      <c r="B17" s="43" t="s">
+    <row r="17" spans="2:15" ht="15" thickBot="1">
+      <c r="B17" s="34" t="s">
         <v>58</v>
       </c>
-      <c r="C17" s="44"/>
-      <c r="D17" s="45"/>
+      <c r="C17" s="35"/>
+      <c r="D17" s="36"/>
       <c r="E17" s="27" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="18" spans="2:15" ht="43.8" customHeight="1" thickBot="1">
-      <c r="B18" s="46" t="s">
+    <row r="18" spans="2:15" ht="15" thickBot="1">
+      <c r="B18" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="C18" s="47"/>
-      <c r="D18" s="48"/>
+      <c r="C18" s="38"/>
+      <c r="D18" s="39"/>
       <c r="E18" s="27" t="s">
         <v>104</v>
       </c>
@@ -3176,102 +3335,102 @@
       </c>
     </row>
     <row r="22" spans="2:15">
-      <c r="B22" s="54" t="s">
+      <c r="B22" s="44" t="s">
         <v>60</v>
       </c>
-      <c r="C22" s="54"/>
-      <c r="D22" s="54"/>
-      <c r="E22" s="54"/>
-      <c r="F22" s="54"/>
-      <c r="G22" s="54"/>
-      <c r="H22" s="54"/>
-      <c r="I22" s="54"/>
-      <c r="J22" s="54"/>
-      <c r="K22" s="54"/>
-      <c r="L22" s="54"/>
-      <c r="M22" s="54"/>
-      <c r="N22" s="54"/>
-      <c r="O22" s="54"/>
+      <c r="C22" s="44"/>
+      <c r="D22" s="44"/>
+      <c r="E22" s="44"/>
+      <c r="F22" s="44"/>
+      <c r="G22" s="44"/>
+      <c r="H22" s="44"/>
+      <c r="I22" s="44"/>
+      <c r="J22" s="44"/>
+      <c r="K22" s="44"/>
+      <c r="L22" s="44"/>
+      <c r="M22" s="44"/>
+      <c r="N22" s="44"/>
+      <c r="O22" s="44"/>
     </row>
     <row r="23" spans="2:15">
-      <c r="B23" s="54"/>
-      <c r="C23" s="54"/>
-      <c r="D23" s="54"/>
-      <c r="E23" s="54"/>
-      <c r="F23" s="54"/>
-      <c r="G23" s="54"/>
-      <c r="H23" s="54"/>
-      <c r="I23" s="54"/>
-      <c r="J23" s="54"/>
-      <c r="K23" s="54"/>
-      <c r="L23" s="54"/>
-      <c r="M23" s="54"/>
-      <c r="N23" s="54"/>
-      <c r="O23" s="54"/>
+      <c r="B23" s="44"/>
+      <c r="C23" s="44"/>
+      <c r="D23" s="44"/>
+      <c r="E23" s="44"/>
+      <c r="F23" s="44"/>
+      <c r="G23" s="44"/>
+      <c r="H23" s="44"/>
+      <c r="I23" s="44"/>
+      <c r="J23" s="44"/>
+      <c r="K23" s="44"/>
+      <c r="L23" s="44"/>
+      <c r="M23" s="44"/>
+      <c r="N23" s="44"/>
+      <c r="O23" s="44"/>
     </row>
     <row r="24" spans="2:15">
-      <c r="B24" s="54"/>
-      <c r="C24" s="54"/>
-      <c r="D24" s="54"/>
-      <c r="E24" s="54"/>
-      <c r="F24" s="54"/>
-      <c r="G24" s="54"/>
-      <c r="H24" s="54"/>
-      <c r="I24" s="54"/>
-      <c r="J24" s="54"/>
-      <c r="K24" s="54"/>
-      <c r="L24" s="54"/>
-      <c r="M24" s="54"/>
-      <c r="N24" s="54"/>
-      <c r="O24" s="54"/>
+      <c r="B24" s="44"/>
+      <c r="C24" s="44"/>
+      <c r="D24" s="44"/>
+      <c r="E24" s="44"/>
+      <c r="F24" s="44"/>
+      <c r="G24" s="44"/>
+      <c r="H24" s="44"/>
+      <c r="I24" s="44"/>
+      <c r="J24" s="44"/>
+      <c r="K24" s="44"/>
+      <c r="L24" s="44"/>
+      <c r="M24" s="44"/>
+      <c r="N24" s="44"/>
+      <c r="O24" s="44"/>
     </row>
     <row r="25" spans="2:15">
-      <c r="B25" s="54"/>
-      <c r="C25" s="54"/>
-      <c r="D25" s="54"/>
-      <c r="E25" s="54"/>
-      <c r="F25" s="54"/>
-      <c r="G25" s="54"/>
-      <c r="H25" s="54"/>
-      <c r="I25" s="54"/>
-      <c r="J25" s="54"/>
-      <c r="K25" s="54"/>
-      <c r="L25" s="54"/>
-      <c r="M25" s="54"/>
-      <c r="N25" s="54"/>
-      <c r="O25" s="54"/>
+      <c r="B25" s="44"/>
+      <c r="C25" s="44"/>
+      <c r="D25" s="44"/>
+      <c r="E25" s="44"/>
+      <c r="F25" s="44"/>
+      <c r="G25" s="44"/>
+      <c r="H25" s="44"/>
+      <c r="I25" s="44"/>
+      <c r="J25" s="44"/>
+      <c r="K25" s="44"/>
+      <c r="L25" s="44"/>
+      <c r="M25" s="44"/>
+      <c r="N25" s="44"/>
+      <c r="O25" s="44"/>
     </row>
     <row r="26" spans="2:15">
-      <c r="B26" s="54"/>
-      <c r="C26" s="54"/>
-      <c r="D26" s="54"/>
-      <c r="E26" s="54"/>
-      <c r="F26" s="54"/>
-      <c r="G26" s="54"/>
-      <c r="H26" s="54"/>
-      <c r="I26" s="54"/>
-      <c r="J26" s="54"/>
-      <c r="K26" s="54"/>
-      <c r="L26" s="54"/>
-      <c r="M26" s="54"/>
-      <c r="N26" s="54"/>
-      <c r="O26" s="54"/>
+      <c r="B26" s="44"/>
+      <c r="C26" s="44"/>
+      <c r="D26" s="44"/>
+      <c r="E26" s="44"/>
+      <c r="F26" s="44"/>
+      <c r="G26" s="44"/>
+      <c r="H26" s="44"/>
+      <c r="I26" s="44"/>
+      <c r="J26" s="44"/>
+      <c r="K26" s="44"/>
+      <c r="L26" s="44"/>
+      <c r="M26" s="44"/>
+      <c r="N26" s="44"/>
+      <c r="O26" s="44"/>
     </row>
     <row r="27" spans="2:15">
-      <c r="B27" s="54"/>
-      <c r="C27" s="54"/>
-      <c r="D27" s="54"/>
-      <c r="E27" s="54"/>
-      <c r="F27" s="54"/>
-      <c r="G27" s="54"/>
-      <c r="H27" s="54"/>
-      <c r="I27" s="54"/>
-      <c r="J27" s="54"/>
-      <c r="K27" s="54"/>
-      <c r="L27" s="54"/>
-      <c r="M27" s="54"/>
-      <c r="N27" s="54"/>
-      <c r="O27" s="54"/>
+      <c r="B27" s="44"/>
+      <c r="C27" s="44"/>
+      <c r="D27" s="44"/>
+      <c r="E27" s="44"/>
+      <c r="F27" s="44"/>
+      <c r="G27" s="44"/>
+      <c r="H27" s="44"/>
+      <c r="I27" s="44"/>
+      <c r="J27" s="44"/>
+      <c r="K27" s="44"/>
+      <c r="L27" s="44"/>
+      <c r="M27" s="44"/>
+      <c r="N27" s="44"/>
+      <c r="O27" s="44"/>
     </row>
     <row r="28" spans="2:15">
       <c r="B28" s="28"/>
@@ -3290,44 +3449,39 @@
       <c r="O28" s="28"/>
     </row>
     <row r="29" spans="2:15">
-      <c r="B29" s="42"/>
-      <c r="C29" s="42"/>
-      <c r="D29" s="42"/>
-      <c r="E29" s="42"/>
-      <c r="F29" s="42"/>
-      <c r="G29" s="42"/>
-      <c r="H29" s="42"/>
-      <c r="I29" s="42"/>
-      <c r="J29" s="42"/>
-      <c r="K29" s="42"/>
-      <c r="L29" s="42"/>
-      <c r="M29" s="42"/>
-      <c r="N29" s="42"/>
-      <c r="O29" s="42"/>
+      <c r="B29" s="30"/>
+      <c r="C29" s="30"/>
+      <c r="D29" s="30"/>
+      <c r="E29" s="30"/>
+      <c r="F29" s="30"/>
+      <c r="G29" s="30"/>
+      <c r="H29" s="30"/>
+      <c r="I29" s="30"/>
+      <c r="J29" s="30"/>
+      <c r="K29" s="30"/>
+      <c r="L29" s="30"/>
+      <c r="M29" s="30"/>
+      <c r="N29" s="30"/>
+      <c r="O29" s="30"/>
     </row>
     <row r="30" spans="2:15">
-      <c r="B30" s="42"/>
-      <c r="C30" s="42"/>
-      <c r="D30" s="42"/>
-      <c r="E30" s="42"/>
-      <c r="F30" s="42"/>
-      <c r="G30" s="42"/>
-      <c r="H30" s="42"/>
-      <c r="I30" s="42"/>
-      <c r="J30" s="42"/>
-      <c r="K30" s="42"/>
-      <c r="L30" s="42"/>
-      <c r="M30" s="42"/>
-      <c r="N30" s="42"/>
-      <c r="O30" s="42"/>
+      <c r="B30" s="30"/>
+      <c r="C30" s="30"/>
+      <c r="D30" s="30"/>
+      <c r="E30" s="30"/>
+      <c r="F30" s="30"/>
+      <c r="G30" s="30"/>
+      <c r="H30" s="30"/>
+      <c r="I30" s="30"/>
+      <c r="J30" s="30"/>
+      <c r="K30" s="30"/>
+      <c r="L30" s="30"/>
+      <c r="M30" s="30"/>
+      <c r="N30" s="30"/>
+      <c r="O30" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B22:O27"/>
-    <mergeCell ref="B29:O29"/>
-    <mergeCell ref="B30:O30"/>
-    <mergeCell ref="C1:S2"/>
     <mergeCell ref="T1:U1"/>
     <mergeCell ref="T2:U2"/>
     <mergeCell ref="I4:I6"/>
@@ -3335,11 +3489,16 @@
     <mergeCell ref="C5:H5"/>
     <mergeCell ref="C4:H4"/>
     <mergeCell ref="J5:L5"/>
+    <mergeCell ref="B22:O27"/>
+    <mergeCell ref="B29:O29"/>
+    <mergeCell ref="B30:O30"/>
+    <mergeCell ref="C1:S2"/>
     <mergeCell ref="B14:D14"/>
     <mergeCell ref="C15:D15"/>
     <mergeCell ref="B17:D17"/>
     <mergeCell ref="B18:D18"/>
-    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B12:D12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -3350,16 +3509,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91203543-4EED-4AE0-859B-F0BC4BB889AE}">
   <dimension ref="B1:U30"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11:C13"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="J48" sqref="J48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="1.33203125" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
-    <col min="3" max="3" width="17.77734375" customWidth="1"/>
-    <col min="4" max="4" width="24.44140625" customWidth="1"/>
+    <col min="1" max="1" width="0.88671875" customWidth="1"/>
+    <col min="2" max="2" width="21.77734375" customWidth="1"/>
+    <col min="3" max="4" width="20.77734375" customWidth="1"/>
     <col min="5" max="5" width="29" customWidth="1"/>
     <col min="8" max="8" width="12.88671875" customWidth="1"/>
     <col min="13" max="13" width="14.109375" customWidth="1"/>
@@ -3369,52 +3527,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:21" ht="27" customHeight="1">
-      <c r="C1" s="40" t="s">
+      <c r="C1" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
-      <c r="H1" s="40"/>
-      <c r="I1" s="40"/>
-      <c r="J1" s="40"/>
-      <c r="K1" s="40"/>
-      <c r="L1" s="40"/>
-      <c r="M1" s="40"/>
-      <c r="N1" s="40"/>
-      <c r="O1" s="40"/>
-      <c r="P1" s="40"/>
-      <c r="Q1" s="40"/>
-      <c r="R1" s="40"/>
-      <c r="S1" s="40"/>
-      <c r="T1" s="37" t="s">
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="53"/>
+      <c r="H1" s="53"/>
+      <c r="I1" s="53"/>
+      <c r="J1" s="53"/>
+      <c r="K1" s="53"/>
+      <c r="L1" s="53"/>
+      <c r="M1" s="53"/>
+      <c r="N1" s="53"/>
+      <c r="O1" s="53"/>
+      <c r="P1" s="53"/>
+      <c r="Q1" s="53"/>
+      <c r="R1" s="53"/>
+      <c r="S1" s="53"/>
+      <c r="T1" s="50" t="s">
         <v>63</v>
       </c>
-      <c r="U1" s="38"/>
+      <c r="U1" s="51"/>
     </row>
     <row r="2" spans="2:21" ht="15" thickBot="1">
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
-      <c r="J2" s="40"/>
-      <c r="K2" s="40"/>
-      <c r="L2" s="40"/>
-      <c r="M2" s="40"/>
-      <c r="N2" s="40"/>
-      <c r="O2" s="40"/>
-      <c r="P2" s="40"/>
-      <c r="Q2" s="40"/>
-      <c r="R2" s="40"/>
-      <c r="S2" s="40"/>
-      <c r="T2" s="39" t="s">
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="53"/>
+      <c r="I2" s="53"/>
+      <c r="J2" s="53"/>
+      <c r="K2" s="53"/>
+      <c r="L2" s="53"/>
+      <c r="M2" s="53"/>
+      <c r="N2" s="53"/>
+      <c r="O2" s="53"/>
+      <c r="P2" s="53"/>
+      <c r="Q2" s="53"/>
+      <c r="R2" s="53"/>
+      <c r="S2" s="53"/>
+      <c r="T2" s="52" t="s">
         <v>64</v>
       </c>
-      <c r="U2" s="39"/>
+      <c r="U2" s="52"/>
     </row>
     <row r="3" spans="2:21" ht="15" thickBot="1">
       <c r="C3" s="24" t="s">
@@ -3442,15 +3600,15 @@
       <c r="U3" s="20"/>
     </row>
     <row r="4" spans="2:21" ht="29.4" customHeight="1" thickBot="1">
-      <c r="C4" s="29" t="s">
+      <c r="C4" s="31" t="s">
         <v>105</v>
       </c>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="30"/>
-      <c r="H4" s="31"/>
-      <c r="I4" s="33" t="s">
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="46" t="s">
         <v>68</v>
       </c>
       <c r="J4" s="55" t="s">
@@ -3460,20 +3618,20 @@
       <c r="L4" s="57"/>
     </row>
     <row r="5" spans="2:21" ht="15" thickBot="1">
-      <c r="C5" s="29" t="s">
+      <c r="C5" s="31" t="s">
         <v>65</v>
       </c>
-      <c r="D5" s="30"/>
-      <c r="E5" s="30"/>
-      <c r="F5" s="30"/>
-      <c r="G5" s="30"/>
-      <c r="H5" s="31"/>
-      <c r="I5" s="35"/>
-      <c r="J5" s="29" t="s">
+      <c r="D5" s="32"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="32"/>
+      <c r="H5" s="33"/>
+      <c r="I5" s="48"/>
+      <c r="J5" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="K5" s="30"/>
-      <c r="L5" s="31"/>
+      <c r="K5" s="32"/>
+      <c r="L5" s="33"/>
     </row>
     <row r="6" spans="2:21" ht="58.2" thickBot="1">
       <c r="B6" s="2"/>
@@ -3495,7 +3653,7 @@
       <c r="H6" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="I6" s="36"/>
+      <c r="I6" s="49"/>
       <c r="J6" s="12" t="s">
         <v>70</v>
       </c>
@@ -3655,32 +3813,32 @@
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
     </row>
-    <row r="12" spans="2:21" ht="24.6" customHeight="1">
-      <c r="B12" s="32" t="s">
+    <row r="12" spans="2:21">
+      <c r="B12" s="29" t="s">
         <v>107</v>
       </c>
-      <c r="C12" s="32"/>
-      <c r="D12" s="7"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="29"/>
       <c r="E12" s="7"/>
     </row>
-    <row r="13" spans="2:21" ht="24.6" customHeight="1" thickBot="1">
-      <c r="B13" s="53" t="s">
+    <row r="13" spans="2:21" ht="15" thickBot="1">
+      <c r="B13" s="45" t="s">
         <v>108</v>
       </c>
-      <c r="C13" s="53"/>
-      <c r="D13" s="59"/>
-      <c r="E13" s="60"/>
+      <c r="C13" s="45"/>
+      <c r="D13" s="45"/>
+      <c r="E13" s="26"/>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
     </row>
     <row r="14" spans="2:21" ht="16.8" customHeight="1" thickBot="1">
-      <c r="B14" s="50" t="s">
+      <c r="B14" s="41" t="s">
         <v>54</v>
       </c>
-      <c r="C14" s="51"/>
-      <c r="D14" s="52"/>
+      <c r="C14" s="42"/>
+      <c r="D14" s="43"/>
       <c r="E14" s="18" t="s">
         <v>53</v>
       </c>
@@ -3691,34 +3849,33 @@
     </row>
     <row r="15" spans="2:21" ht="15" thickBot="1">
       <c r="B15" s="1"/>
-      <c r="C15" s="49"/>
-      <c r="D15" s="61"/>
-      <c r="E15" s="62"/>
+      <c r="C15" s="40"/>
+      <c r="D15" s="40"/>
     </row>
     <row r="16" spans="2:21" ht="29.4" thickBot="1">
-      <c r="B16" s="58"/>
-      <c r="C16" s="59"/>
-      <c r="D16" s="59"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="25"/>
       <c r="E16" s="12" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="17" spans="2:15" ht="39.6" customHeight="1" thickBot="1">
-      <c r="B17" s="43" t="s">
+    <row r="17" spans="2:15" ht="15" thickBot="1">
+      <c r="B17" s="34" t="s">
         <v>58</v>
       </c>
-      <c r="C17" s="44"/>
-      <c r="D17" s="45"/>
+      <c r="C17" s="35"/>
+      <c r="D17" s="36"/>
       <c r="E17" s="27" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="18" spans="2:15" ht="43.8" customHeight="1" thickBot="1">
-      <c r="B18" s="46" t="s">
+    <row r="18" spans="2:15" ht="15" thickBot="1">
+      <c r="B18" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="C18" s="47"/>
-      <c r="D18" s="48"/>
+      <c r="C18" s="38"/>
+      <c r="D18" s="39"/>
       <c r="E18" s="27" t="s">
         <v>115</v>
       </c>
@@ -3739,102 +3896,102 @@
       </c>
     </row>
     <row r="22" spans="2:15">
-      <c r="B22" s="54" t="s">
+      <c r="B22" s="44" t="s">
         <v>60</v>
       </c>
-      <c r="C22" s="54"/>
-      <c r="D22" s="54"/>
-      <c r="E22" s="54"/>
-      <c r="F22" s="54"/>
-      <c r="G22" s="54"/>
-      <c r="H22" s="54"/>
-      <c r="I22" s="54"/>
-      <c r="J22" s="54"/>
-      <c r="K22" s="54"/>
-      <c r="L22" s="54"/>
-      <c r="M22" s="54"/>
-      <c r="N22" s="54"/>
-      <c r="O22" s="54"/>
+      <c r="C22" s="44"/>
+      <c r="D22" s="44"/>
+      <c r="E22" s="44"/>
+      <c r="F22" s="44"/>
+      <c r="G22" s="44"/>
+      <c r="H22" s="44"/>
+      <c r="I22" s="44"/>
+      <c r="J22" s="44"/>
+      <c r="K22" s="44"/>
+      <c r="L22" s="44"/>
+      <c r="M22" s="44"/>
+      <c r="N22" s="44"/>
+      <c r="O22" s="44"/>
     </row>
     <row r="23" spans="2:15">
-      <c r="B23" s="54"/>
-      <c r="C23" s="54"/>
-      <c r="D23" s="54"/>
-      <c r="E23" s="54"/>
-      <c r="F23" s="54"/>
-      <c r="G23" s="54"/>
-      <c r="H23" s="54"/>
-      <c r="I23" s="54"/>
-      <c r="J23" s="54"/>
-      <c r="K23" s="54"/>
-      <c r="L23" s="54"/>
-      <c r="M23" s="54"/>
-      <c r="N23" s="54"/>
-      <c r="O23" s="54"/>
+      <c r="B23" s="44"/>
+      <c r="C23" s="44"/>
+      <c r="D23" s="44"/>
+      <c r="E23" s="44"/>
+      <c r="F23" s="44"/>
+      <c r="G23" s="44"/>
+      <c r="H23" s="44"/>
+      <c r="I23" s="44"/>
+      <c r="J23" s="44"/>
+      <c r="K23" s="44"/>
+      <c r="L23" s="44"/>
+      <c r="M23" s="44"/>
+      <c r="N23" s="44"/>
+      <c r="O23" s="44"/>
     </row>
     <row r="24" spans="2:15">
-      <c r="B24" s="54"/>
-      <c r="C24" s="54"/>
-      <c r="D24" s="54"/>
-      <c r="E24" s="54"/>
-      <c r="F24" s="54"/>
-      <c r="G24" s="54"/>
-      <c r="H24" s="54"/>
-      <c r="I24" s="54"/>
-      <c r="J24" s="54"/>
-      <c r="K24" s="54"/>
-      <c r="L24" s="54"/>
-      <c r="M24" s="54"/>
-      <c r="N24" s="54"/>
-      <c r="O24" s="54"/>
+      <c r="B24" s="44"/>
+      <c r="C24" s="44"/>
+      <c r="D24" s="44"/>
+      <c r="E24" s="44"/>
+      <c r="F24" s="44"/>
+      <c r="G24" s="44"/>
+      <c r="H24" s="44"/>
+      <c r="I24" s="44"/>
+      <c r="J24" s="44"/>
+      <c r="K24" s="44"/>
+      <c r="L24" s="44"/>
+      <c r="M24" s="44"/>
+      <c r="N24" s="44"/>
+      <c r="O24" s="44"/>
     </row>
     <row r="25" spans="2:15">
-      <c r="B25" s="54"/>
-      <c r="C25" s="54"/>
-      <c r="D25" s="54"/>
-      <c r="E25" s="54"/>
-      <c r="F25" s="54"/>
-      <c r="G25" s="54"/>
-      <c r="H25" s="54"/>
-      <c r="I25" s="54"/>
-      <c r="J25" s="54"/>
-      <c r="K25" s="54"/>
-      <c r="L25" s="54"/>
-      <c r="M25" s="54"/>
-      <c r="N25" s="54"/>
-      <c r="O25" s="54"/>
+      <c r="B25" s="44"/>
+      <c r="C25" s="44"/>
+      <c r="D25" s="44"/>
+      <c r="E25" s="44"/>
+      <c r="F25" s="44"/>
+      <c r="G25" s="44"/>
+      <c r="H25" s="44"/>
+      <c r="I25" s="44"/>
+      <c r="J25" s="44"/>
+      <c r="K25" s="44"/>
+      <c r="L25" s="44"/>
+      <c r="M25" s="44"/>
+      <c r="N25" s="44"/>
+      <c r="O25" s="44"/>
     </row>
     <row r="26" spans="2:15">
-      <c r="B26" s="54"/>
-      <c r="C26" s="54"/>
-      <c r="D26" s="54"/>
-      <c r="E26" s="54"/>
-      <c r="F26" s="54"/>
-      <c r="G26" s="54"/>
-      <c r="H26" s="54"/>
-      <c r="I26" s="54"/>
-      <c r="J26" s="54"/>
-      <c r="K26" s="54"/>
-      <c r="L26" s="54"/>
-      <c r="M26" s="54"/>
-      <c r="N26" s="54"/>
-      <c r="O26" s="54"/>
+      <c r="B26" s="44"/>
+      <c r="C26" s="44"/>
+      <c r="D26" s="44"/>
+      <c r="E26" s="44"/>
+      <c r="F26" s="44"/>
+      <c r="G26" s="44"/>
+      <c r="H26" s="44"/>
+      <c r="I26" s="44"/>
+      <c r="J26" s="44"/>
+      <c r="K26" s="44"/>
+      <c r="L26" s="44"/>
+      <c r="M26" s="44"/>
+      <c r="N26" s="44"/>
+      <c r="O26" s="44"/>
     </row>
     <row r="27" spans="2:15">
-      <c r="B27" s="54"/>
-      <c r="C27" s="54"/>
-      <c r="D27" s="54"/>
-      <c r="E27" s="54"/>
-      <c r="F27" s="54"/>
-      <c r="G27" s="54"/>
-      <c r="H27" s="54"/>
-      <c r="I27" s="54"/>
-      <c r="J27" s="54"/>
-      <c r="K27" s="54"/>
-      <c r="L27" s="54"/>
-      <c r="M27" s="54"/>
-      <c r="N27" s="54"/>
-      <c r="O27" s="54"/>
+      <c r="B27" s="44"/>
+      <c r="C27" s="44"/>
+      <c r="D27" s="44"/>
+      <c r="E27" s="44"/>
+      <c r="F27" s="44"/>
+      <c r="G27" s="44"/>
+      <c r="H27" s="44"/>
+      <c r="I27" s="44"/>
+      <c r="J27" s="44"/>
+      <c r="K27" s="44"/>
+      <c r="L27" s="44"/>
+      <c r="M27" s="44"/>
+      <c r="N27" s="44"/>
+      <c r="O27" s="44"/>
     </row>
     <row r="28" spans="2:15">
       <c r="B28" s="28"/>
@@ -3853,48 +4010,39 @@
       <c r="O28" s="28"/>
     </row>
     <row r="29" spans="2:15">
-      <c r="B29" s="42"/>
-      <c r="C29" s="42"/>
-      <c r="D29" s="42"/>
-      <c r="E29" s="42"/>
-      <c r="F29" s="42"/>
-      <c r="G29" s="42"/>
-      <c r="H29" s="42"/>
-      <c r="I29" s="42"/>
-      <c r="J29" s="42"/>
-      <c r="K29" s="42"/>
-      <c r="L29" s="42"/>
-      <c r="M29" s="42"/>
-      <c r="N29" s="42"/>
-      <c r="O29" s="42"/>
+      <c r="B29" s="30"/>
+      <c r="C29" s="30"/>
+      <c r="D29" s="30"/>
+      <c r="E29" s="30"/>
+      <c r="F29" s="30"/>
+      <c r="G29" s="30"/>
+      <c r="H29" s="30"/>
+      <c r="I29" s="30"/>
+      <c r="J29" s="30"/>
+      <c r="K29" s="30"/>
+      <c r="L29" s="30"/>
+      <c r="M29" s="30"/>
+      <c r="N29" s="30"/>
+      <c r="O29" s="30"/>
     </row>
     <row r="30" spans="2:15">
-      <c r="B30" s="42"/>
-      <c r="C30" s="42"/>
-      <c r="D30" s="42"/>
-      <c r="E30" s="42"/>
-      <c r="F30" s="42"/>
-      <c r="G30" s="42"/>
-      <c r="H30" s="42"/>
-      <c r="I30" s="42"/>
-      <c r="J30" s="42"/>
-      <c r="K30" s="42"/>
-      <c r="L30" s="42"/>
-      <c r="M30" s="42"/>
-      <c r="N30" s="42"/>
-      <c r="O30" s="42"/>
+      <c r="B30" s="30"/>
+      <c r="C30" s="30"/>
+      <c r="D30" s="30"/>
+      <c r="E30" s="30"/>
+      <c r="F30" s="30"/>
+      <c r="G30" s="30"/>
+      <c r="H30" s="30"/>
+      <c r="I30" s="30"/>
+      <c r="J30" s="30"/>
+      <c r="K30" s="30"/>
+      <c r="L30" s="30"/>
+      <c r="M30" s="30"/>
+      <c r="N30" s="30"/>
+      <c r="O30" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B30:O30"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="B22:O27"/>
-    <mergeCell ref="B29:O29"/>
     <mergeCell ref="C1:S2"/>
     <mergeCell ref="T1:U1"/>
     <mergeCell ref="T2:U2"/>
@@ -3903,6 +4051,15 @@
     <mergeCell ref="J4:L4"/>
     <mergeCell ref="C5:H5"/>
     <mergeCell ref="J5:L5"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B30:O30"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="B22:O27"/>
+    <mergeCell ref="B29:O29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -3913,16 +4070,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FBF716D-FD41-4431-A8BB-5A81BFB0390B}">
   <dimension ref="B1:U30"/>
   <sheetViews>
-    <sheetView topLeftCell="B7" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView topLeftCell="B22" workbookViewId="0">
+      <selection activeCell="I46" sqref="I46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="1.33203125" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
-    <col min="3" max="3" width="17.77734375" customWidth="1"/>
-    <col min="4" max="4" width="24.44140625" customWidth="1"/>
+    <col min="2" max="2" width="21.77734375" customWidth="1"/>
+    <col min="3" max="4" width="20.77734375" customWidth="1"/>
     <col min="5" max="5" width="29" customWidth="1"/>
     <col min="8" max="8" width="12.88671875" customWidth="1"/>
     <col min="13" max="13" width="14.109375" customWidth="1"/>
@@ -3932,52 +4088,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:21" ht="27" customHeight="1">
-      <c r="C1" s="40" t="s">
+      <c r="C1" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
-      <c r="H1" s="40"/>
-      <c r="I1" s="40"/>
-      <c r="J1" s="40"/>
-      <c r="K1" s="40"/>
-      <c r="L1" s="40"/>
-      <c r="M1" s="40"/>
-      <c r="N1" s="40"/>
-      <c r="O1" s="40"/>
-      <c r="P1" s="40"/>
-      <c r="Q1" s="40"/>
-      <c r="R1" s="40"/>
-      <c r="S1" s="40"/>
-      <c r="T1" s="37" t="s">
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="53"/>
+      <c r="H1" s="53"/>
+      <c r="I1" s="53"/>
+      <c r="J1" s="53"/>
+      <c r="K1" s="53"/>
+      <c r="L1" s="53"/>
+      <c r="M1" s="53"/>
+      <c r="N1" s="53"/>
+      <c r="O1" s="53"/>
+      <c r="P1" s="53"/>
+      <c r="Q1" s="53"/>
+      <c r="R1" s="53"/>
+      <c r="S1" s="53"/>
+      <c r="T1" s="50" t="s">
         <v>63</v>
       </c>
-      <c r="U1" s="38"/>
+      <c r="U1" s="51"/>
     </row>
     <row r="2" spans="2:21" ht="15" thickBot="1">
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
-      <c r="J2" s="40"/>
-      <c r="K2" s="40"/>
-      <c r="L2" s="40"/>
-      <c r="M2" s="40"/>
-      <c r="N2" s="40"/>
-      <c r="O2" s="40"/>
-      <c r="P2" s="40"/>
-      <c r="Q2" s="40"/>
-      <c r="R2" s="40"/>
-      <c r="S2" s="40"/>
-      <c r="T2" s="39" t="s">
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="53"/>
+      <c r="I2" s="53"/>
+      <c r="J2" s="53"/>
+      <c r="K2" s="53"/>
+      <c r="L2" s="53"/>
+      <c r="M2" s="53"/>
+      <c r="N2" s="53"/>
+      <c r="O2" s="53"/>
+      <c r="P2" s="53"/>
+      <c r="Q2" s="53"/>
+      <c r="R2" s="53"/>
+      <c r="S2" s="53"/>
+      <c r="T2" s="52" t="s">
         <v>64</v>
       </c>
-      <c r="U2" s="39"/>
+      <c r="U2" s="52"/>
     </row>
     <row r="3" spans="2:21" ht="15" thickBot="1">
       <c r="C3" s="24" t="s">
@@ -4005,15 +4161,15 @@
       <c r="U3" s="20"/>
     </row>
     <row r="4" spans="2:21" ht="29.4" customHeight="1" thickBot="1">
-      <c r="C4" s="29" t="s">
+      <c r="C4" s="31" t="s">
         <v>105</v>
       </c>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="30"/>
-      <c r="H4" s="31"/>
-      <c r="I4" s="33" t="s">
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="46" t="s">
         <v>68</v>
       </c>
       <c r="J4" s="55" t="s">
@@ -4023,20 +4179,20 @@
       <c r="L4" s="57"/>
     </row>
     <row r="5" spans="2:21" ht="15" thickBot="1">
-      <c r="C5" s="29" t="s">
+      <c r="C5" s="31" t="s">
         <v>66</v>
       </c>
-      <c r="D5" s="30"/>
-      <c r="E5" s="30"/>
-      <c r="F5" s="30"/>
-      <c r="G5" s="30"/>
-      <c r="H5" s="31"/>
-      <c r="I5" s="35"/>
-      <c r="J5" s="29" t="s">
+      <c r="D5" s="32"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="32"/>
+      <c r="H5" s="33"/>
+      <c r="I5" s="48"/>
+      <c r="J5" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="K5" s="30"/>
-      <c r="L5" s="31"/>
+      <c r="K5" s="32"/>
+      <c r="L5" s="33"/>
     </row>
     <row r="6" spans="2:21" ht="58.2" thickBot="1">
       <c r="B6" s="2"/>
@@ -4058,7 +4214,7 @@
       <c r="H6" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="I6" s="36"/>
+      <c r="I6" s="49"/>
       <c r="J6" s="12" t="s">
         <v>71</v>
       </c>
@@ -4218,32 +4374,32 @@
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
     </row>
-    <row r="12" spans="2:21" ht="22.8" customHeight="1">
-      <c r="B12" s="32" t="s">
+    <row r="12" spans="2:21">
+      <c r="B12" s="29" t="s">
         <v>107</v>
       </c>
-      <c r="C12" s="32"/>
-      <c r="D12" s="7"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="29"/>
       <c r="E12" s="7"/>
     </row>
-    <row r="13" spans="2:21" ht="31.2" customHeight="1" thickBot="1">
-      <c r="B13" s="53" t="s">
+    <row r="13" spans="2:21" ht="15" thickBot="1">
+      <c r="B13" s="45" t="s">
         <v>108</v>
       </c>
-      <c r="C13" s="53"/>
-      <c r="D13" s="59"/>
-      <c r="E13" s="60"/>
+      <c r="C13" s="45"/>
+      <c r="D13" s="45"/>
+      <c r="E13" s="26"/>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
     </row>
     <row r="14" spans="2:21" ht="16.8" customHeight="1" thickBot="1">
-      <c r="B14" s="50" t="s">
+      <c r="B14" s="41" t="s">
         <v>54</v>
       </c>
-      <c r="C14" s="51"/>
-      <c r="D14" s="52"/>
+      <c r="C14" s="42"/>
+      <c r="D14" s="43"/>
       <c r="E14" s="18" t="s">
         <v>53</v>
       </c>
@@ -4254,34 +4410,33 @@
     </row>
     <row r="15" spans="2:21" ht="15" thickBot="1">
       <c r="B15" s="1"/>
-      <c r="C15" s="49"/>
-      <c r="D15" s="61"/>
-      <c r="E15" s="62"/>
+      <c r="C15" s="40"/>
+      <c r="D15" s="40"/>
     </row>
     <row r="16" spans="2:21" ht="29.4" thickBot="1">
-      <c r="B16" s="58"/>
-      <c r="C16" s="59"/>
-      <c r="D16" s="59"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="25"/>
       <c r="E16" s="12" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="17" spans="2:15" ht="39.6" customHeight="1" thickBot="1">
-      <c r="B17" s="43" t="s">
+    <row r="17" spans="2:15" ht="15" thickBot="1">
+      <c r="B17" s="34" t="s">
         <v>58</v>
       </c>
-      <c r="C17" s="44"/>
-      <c r="D17" s="45"/>
+      <c r="C17" s="35"/>
+      <c r="D17" s="36"/>
       <c r="E17" s="27" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="18" spans="2:15" ht="43.8" customHeight="1" thickBot="1">
-      <c r="B18" s="46" t="s">
+    <row r="18" spans="2:15" ht="15" thickBot="1">
+      <c r="B18" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="C18" s="47"/>
-      <c r="D18" s="48"/>
+      <c r="C18" s="38"/>
+      <c r="D18" s="39"/>
       <c r="E18" s="27" t="s">
         <v>120</v>
       </c>
@@ -4302,102 +4457,102 @@
       </c>
     </row>
     <row r="22" spans="2:15">
-      <c r="B22" s="54" t="s">
+      <c r="B22" s="44" t="s">
         <v>60</v>
       </c>
-      <c r="C22" s="54"/>
-      <c r="D22" s="54"/>
-      <c r="E22" s="54"/>
-      <c r="F22" s="54"/>
-      <c r="G22" s="54"/>
-      <c r="H22" s="54"/>
-      <c r="I22" s="54"/>
-      <c r="J22" s="54"/>
-      <c r="K22" s="54"/>
-      <c r="L22" s="54"/>
-      <c r="M22" s="54"/>
-      <c r="N22" s="54"/>
-      <c r="O22" s="54"/>
+      <c r="C22" s="44"/>
+      <c r="D22" s="44"/>
+      <c r="E22" s="44"/>
+      <c r="F22" s="44"/>
+      <c r="G22" s="44"/>
+      <c r="H22" s="44"/>
+      <c r="I22" s="44"/>
+      <c r="J22" s="44"/>
+      <c r="K22" s="44"/>
+      <c r="L22" s="44"/>
+      <c r="M22" s="44"/>
+      <c r="N22" s="44"/>
+      <c r="O22" s="44"/>
     </row>
     <row r="23" spans="2:15">
-      <c r="B23" s="54"/>
-      <c r="C23" s="54"/>
-      <c r="D23" s="54"/>
-      <c r="E23" s="54"/>
-      <c r="F23" s="54"/>
-      <c r="G23" s="54"/>
-      <c r="H23" s="54"/>
-      <c r="I23" s="54"/>
-      <c r="J23" s="54"/>
-      <c r="K23" s="54"/>
-      <c r="L23" s="54"/>
-      <c r="M23" s="54"/>
-      <c r="N23" s="54"/>
-      <c r="O23" s="54"/>
+      <c r="B23" s="44"/>
+      <c r="C23" s="44"/>
+      <c r="D23" s="44"/>
+      <c r="E23" s="44"/>
+      <c r="F23" s="44"/>
+      <c r="G23" s="44"/>
+      <c r="H23" s="44"/>
+      <c r="I23" s="44"/>
+      <c r="J23" s="44"/>
+      <c r="K23" s="44"/>
+      <c r="L23" s="44"/>
+      <c r="M23" s="44"/>
+      <c r="N23" s="44"/>
+      <c r="O23" s="44"/>
     </row>
     <row r="24" spans="2:15">
-      <c r="B24" s="54"/>
-      <c r="C24" s="54"/>
-      <c r="D24" s="54"/>
-      <c r="E24" s="54"/>
-      <c r="F24" s="54"/>
-      <c r="G24" s="54"/>
-      <c r="H24" s="54"/>
-      <c r="I24" s="54"/>
-      <c r="J24" s="54"/>
-      <c r="K24" s="54"/>
-      <c r="L24" s="54"/>
-      <c r="M24" s="54"/>
-      <c r="N24" s="54"/>
-      <c r="O24" s="54"/>
+      <c r="B24" s="44"/>
+      <c r="C24" s="44"/>
+      <c r="D24" s="44"/>
+      <c r="E24" s="44"/>
+      <c r="F24" s="44"/>
+      <c r="G24" s="44"/>
+      <c r="H24" s="44"/>
+      <c r="I24" s="44"/>
+      <c r="J24" s="44"/>
+      <c r="K24" s="44"/>
+      <c r="L24" s="44"/>
+      <c r="M24" s="44"/>
+      <c r="N24" s="44"/>
+      <c r="O24" s="44"/>
     </row>
     <row r="25" spans="2:15">
-      <c r="B25" s="54"/>
-      <c r="C25" s="54"/>
-      <c r="D25" s="54"/>
-      <c r="E25" s="54"/>
-      <c r="F25" s="54"/>
-      <c r="G25" s="54"/>
-      <c r="H25" s="54"/>
-      <c r="I25" s="54"/>
-      <c r="J25" s="54"/>
-      <c r="K25" s="54"/>
-      <c r="L25" s="54"/>
-      <c r="M25" s="54"/>
-      <c r="N25" s="54"/>
-      <c r="O25" s="54"/>
+      <c r="B25" s="44"/>
+      <c r="C25" s="44"/>
+      <c r="D25" s="44"/>
+      <c r="E25" s="44"/>
+      <c r="F25" s="44"/>
+      <c r="G25" s="44"/>
+      <c r="H25" s="44"/>
+      <c r="I25" s="44"/>
+      <c r="J25" s="44"/>
+      <c r="K25" s="44"/>
+      <c r="L25" s="44"/>
+      <c r="M25" s="44"/>
+      <c r="N25" s="44"/>
+      <c r="O25" s="44"/>
     </row>
     <row r="26" spans="2:15">
-      <c r="B26" s="54"/>
-      <c r="C26" s="54"/>
-      <c r="D26" s="54"/>
-      <c r="E26" s="54"/>
-      <c r="F26" s="54"/>
-      <c r="G26" s="54"/>
-      <c r="H26" s="54"/>
-      <c r="I26" s="54"/>
-      <c r="J26" s="54"/>
-      <c r="K26" s="54"/>
-      <c r="L26" s="54"/>
-      <c r="M26" s="54"/>
-      <c r="N26" s="54"/>
-      <c r="O26" s="54"/>
+      <c r="B26" s="44"/>
+      <c r="C26" s="44"/>
+      <c r="D26" s="44"/>
+      <c r="E26" s="44"/>
+      <c r="F26" s="44"/>
+      <c r="G26" s="44"/>
+      <c r="H26" s="44"/>
+      <c r="I26" s="44"/>
+      <c r="J26" s="44"/>
+      <c r="K26" s="44"/>
+      <c r="L26" s="44"/>
+      <c r="M26" s="44"/>
+      <c r="N26" s="44"/>
+      <c r="O26" s="44"/>
     </row>
     <row r="27" spans="2:15">
-      <c r="B27" s="54"/>
-      <c r="C27" s="54"/>
-      <c r="D27" s="54"/>
-      <c r="E27" s="54"/>
-      <c r="F27" s="54"/>
-      <c r="G27" s="54"/>
-      <c r="H27" s="54"/>
-      <c r="I27" s="54"/>
-      <c r="J27" s="54"/>
-      <c r="K27" s="54"/>
-      <c r="L27" s="54"/>
-      <c r="M27" s="54"/>
-      <c r="N27" s="54"/>
-      <c r="O27" s="54"/>
+      <c r="B27" s="44"/>
+      <c r="C27" s="44"/>
+      <c r="D27" s="44"/>
+      <c r="E27" s="44"/>
+      <c r="F27" s="44"/>
+      <c r="G27" s="44"/>
+      <c r="H27" s="44"/>
+      <c r="I27" s="44"/>
+      <c r="J27" s="44"/>
+      <c r="K27" s="44"/>
+      <c r="L27" s="44"/>
+      <c r="M27" s="44"/>
+      <c r="N27" s="44"/>
+      <c r="O27" s="44"/>
     </row>
     <row r="28" spans="2:15">
       <c r="B28" s="28"/>
@@ -4416,41 +4571,48 @@
       <c r="O28" s="28"/>
     </row>
     <row r="29" spans="2:15">
-      <c r="B29" s="42"/>
-      <c r="C29" s="42"/>
-      <c r="D29" s="42"/>
-      <c r="E29" s="42"/>
-      <c r="F29" s="42"/>
-      <c r="G29" s="42"/>
-      <c r="H29" s="42"/>
-      <c r="I29" s="42"/>
-      <c r="J29" s="42"/>
-      <c r="K29" s="42"/>
-      <c r="L29" s="42"/>
-      <c r="M29" s="42"/>
-      <c r="N29" s="42"/>
-      <c r="O29" s="42"/>
+      <c r="B29" s="30"/>
+      <c r="C29" s="30"/>
+      <c r="D29" s="30"/>
+      <c r="E29" s="30"/>
+      <c r="F29" s="30"/>
+      <c r="G29" s="30"/>
+      <c r="H29" s="30"/>
+      <c r="I29" s="30"/>
+      <c r="J29" s="30"/>
+      <c r="K29" s="30"/>
+      <c r="L29" s="30"/>
+      <c r="M29" s="30"/>
+      <c r="N29" s="30"/>
+      <c r="O29" s="30"/>
     </row>
     <row r="30" spans="2:15">
-      <c r="B30" s="42"/>
-      <c r="C30" s="42"/>
-      <c r="D30" s="42"/>
-      <c r="E30" s="42"/>
-      <c r="F30" s="42"/>
-      <c r="G30" s="42"/>
-      <c r="H30" s="42"/>
-      <c r="I30" s="42"/>
-      <c r="J30" s="42"/>
-      <c r="K30" s="42"/>
-      <c r="L30" s="42"/>
-      <c r="M30" s="42"/>
-      <c r="N30" s="42"/>
-      <c r="O30" s="42"/>
+      <c r="B30" s="30"/>
+      <c r="C30" s="30"/>
+      <c r="D30" s="30"/>
+      <c r="E30" s="30"/>
+      <c r="F30" s="30"/>
+      <c r="G30" s="30"/>
+      <c r="H30" s="30"/>
+      <c r="I30" s="30"/>
+      <c r="J30" s="30"/>
+      <c r="K30" s="30"/>
+      <c r="L30" s="30"/>
+      <c r="M30" s="30"/>
+      <c r="N30" s="30"/>
+      <c r="O30" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B30:O30"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="B22:O27"/>
+    <mergeCell ref="B29:O29"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="B13:D13"/>
     <mergeCell ref="C1:S2"/>
     <mergeCell ref="T1:U1"/>
     <mergeCell ref="T2:U2"/>
@@ -4459,13 +4621,6 @@
     <mergeCell ref="J4:L4"/>
     <mergeCell ref="C5:H5"/>
     <mergeCell ref="J5:L5"/>
-    <mergeCell ref="B30:O30"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="B22:O27"/>
-    <mergeCell ref="B29:O29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>